<commit_message>
Created animation ID in inside file To_Do_List.xlsx to check for animation ID. Created class CQuestionBrick based on CBrick class, but add animation to it, still need to do the collision stuff with this class.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940EF05F-2AE4-4D10-A887-7272B75C0626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088CFA31-DCB0-400E-98C9-4E51F704C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Pipe</t>
   </si>
   <si>
+    <t>Brick</t>
+  </si>
+  <si>
     <t>Unbreakable Brick</t>
   </si>
   <si>
@@ -55,13 +58,97 @@
   </si>
   <si>
     <t>CInvisiblePlatform</t>
+  </si>
+  <si>
+    <t>Ani_ID</t>
+  </si>
+  <si>
+    <t>Game Object</t>
+  </si>
+  <si>
+    <t>Goomba</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t>Die</t>
+  </si>
+  <si>
+    <t>Invisible Platform</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Idle Left</t>
+  </si>
+  <si>
+    <t>Idle Right</t>
+  </si>
+  <si>
+    <t>Walking Right</t>
+  </si>
+  <si>
+    <t>Walking Left</t>
+  </si>
+  <si>
+    <t>Running Right</t>
+  </si>
+  <si>
+    <t>Running Left</t>
+  </si>
+  <si>
+    <t>Jump Walk Right</t>
+  </si>
+  <si>
+    <t>Jump Walk Left</t>
+  </si>
+  <si>
+    <t>Jump Run Right</t>
+  </si>
+  <si>
+    <t>Jump Run Left</t>
+  </si>
+  <si>
+    <t>Sit Right</t>
+  </si>
+  <si>
+    <t>Sit Left</t>
+  </si>
+  <si>
+    <t>Brace Right</t>
+  </si>
+  <si>
+    <t>Brace Left</t>
+  </si>
+  <si>
+    <t>Mario Big</t>
+  </si>
+  <si>
+    <t>Mario Small</t>
+  </si>
+  <si>
+    <t>Portal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +159,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -100,15 +195,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,19 +710,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:F8"/>
+  <dimension ref="B4:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="5" max="5" width="21.109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,31 +735,364 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="L4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="12"/>
+      <c r="U4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" s="12"/>
+      <c r="W4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" s="12"/>
+    </row>
+    <row r="5" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="T6" s="15">
+        <v>10000</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="16">
+        <v>11000</v>
+      </c>
+      <c r="W6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="X6" s="18"/>
+    </row>
+    <row r="7" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="7">
+        <v>5001</v>
+      </c>
+      <c r="W7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="X7" s="20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>5</v>
+      <c r="W8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8" s="20">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="X9" s="20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="X10" s="20">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="X11" s="20">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="X12" s="20">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="X13" s="20">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="20">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="X15" s="20">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="W16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="X16" s="20">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="17" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W17" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="X17" s="20">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="18" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18" s="20">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="19" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="X19" s="20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W20" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="X20" s="20">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="21" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X21" s="20">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="22" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W22" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="X22" s="22"/>
+    </row>
+    <row r="23" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W23" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="X23" s="20">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="24" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W24" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X24" s="20">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="25" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W25" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="X25" s="20">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="26" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26" s="20">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="27" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W27" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="X27" s="20">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W28" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="X28" s="20">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="29" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W29" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="X29" s="20">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="30" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W30" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="X30" s="20">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="31" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W31" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="X31" s="20">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W32" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X32" s="20">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="33" spans="23:24" x14ac:dyDescent="0.3">
+      <c r="W33" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="X33" s="20">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="34" spans="23:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X34" s="7">
+        <v>1601</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mushroom now can be reveal when Mario hit ? Brick from bottom up, but only when Mushroom and ? brick's location are not overlap.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088CFA31-DCB0-400E-98C9-4E51F704C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922AD90C-4754-4E20-BEA8-888D2A05785C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -142,6 +142,39 @@
   </si>
   <si>
     <t>Portal</t>
+  </si>
+  <si>
+    <t>Question Brick</t>
+  </si>
+  <si>
+    <t>? mark moving</t>
+  </si>
+  <si>
+    <t>no ? ark moving</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
+    <t>Item object</t>
+  </si>
+  <si>
+    <t>Linked object</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Item id</t>
+  </si>
+  <si>
+    <t>? Brick</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -187,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -281,6 +314,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -352,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,6 +403,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,25 +422,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,23 +773,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:Z34"/>
+  <dimension ref="B4:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="6" max="8" width="16" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.77734375" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" customWidth="1"/>
+    <col min="27" max="27" width="15.88671875" customWidth="1"/>
+    <col min="31" max="31" width="15.33203125" customWidth="1"/>
+    <col min="35" max="35" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,363 +802,467 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="R4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="S4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="11" t="s">
+      <c r="T4" s="10"/>
+      <c r="U4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="11" t="s">
+      <c r="V4" s="14"/>
+      <c r="W4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="11" t="s">
+      <c r="X4" s="14"/>
+      <c r="Y4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="12"/>
-      <c r="U4" s="11" t="s">
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="12"/>
-      <c r="W4" s="11" t="s">
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="11" t="s">
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Z4" s="12"/>
-    </row>
-    <row r="5" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ4" s="14"/>
+    </row>
+    <row r="5" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="I5" s="29"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="S5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="T5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="U5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="V5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="W5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="X5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="Y5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="Z5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="AA5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="AB5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="AC5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="AD5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="AE5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="AF5" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="I6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="5">
+      <c r="T6" s="5">
         <v>5000</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="Y6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="15">
+      <c r="Z6" s="17">
         <v>10000</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="AA6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" s="18">
+        <v>10500</v>
+      </c>
+      <c r="AC6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="V6" s="16">
+      <c r="AD6" s="18">
         <v>11000</v>
       </c>
-      <c r="W6" s="17" t="s">
+      <c r="AE6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="18"/>
-    </row>
-    <row r="7" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF6" s="20"/>
+      <c r="AI6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="I7" s="27"/>
+      <c r="J7" s="31"/>
+      <c r="S7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="7">
+      <c r="T7" s="7">
         <v>5001</v>
       </c>
-      <c r="W7" s="19" t="s">
+      <c r="AA7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7">
+        <v>10600</v>
+      </c>
+      <c r="AE7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="20">
+      <c r="AF7" s="22">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="W8" s="19" t="s">
+      <c r="I8" s="27"/>
+      <c r="J8" s="31"/>
+      <c r="AE8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="20">
+      <c r="AF8" s="22">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W9" s="19" t="s">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I9" s="27"/>
+      <c r="J9" s="31"/>
+      <c r="AE9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="20">
+      <c r="AF9" s="22">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W10" s="19" t="s">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I10" s="27"/>
+      <c r="AE10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="X10" s="20">
+      <c r="AF10" s="22">
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W11" s="19" t="s">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I11" s="27"/>
+      <c r="AE11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="20">
+      <c r="AF11" s="22">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W12" s="19" t="s">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I12" s="27"/>
+      <c r="AE12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="X12" s="20">
+      <c r="AF12" s="22">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W13" s="19" t="s">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I13" s="27"/>
+      <c r="AE13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="X13" s="20">
+      <c r="AF13" s="22">
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W14" s="19" t="s">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I14" s="27"/>
+      <c r="AE14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="X14" s="20">
+      <c r="AF14" s="22">
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W15" s="19" t="s">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I15" s="27"/>
+      <c r="AE15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="X15" s="20">
+      <c r="AF15" s="22">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="W16" s="19" t="s">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="I16" s="27"/>
+      <c r="AE16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="X16" s="20">
+      <c r="AF16" s="22">
         <v>801</v>
       </c>
     </row>
-    <row r="17" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W17" s="19" t="s">
+    <row r="17" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I17" s="27"/>
+      <c r="AE17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="X17" s="20">
+      <c r="AF17" s="22">
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W18" s="19" t="s">
+    <row r="18" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I18" s="27"/>
+      <c r="AE18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="X18" s="20">
+      <c r="AF18" s="22">
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W19" s="19" t="s">
+    <row r="19" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I19" s="27"/>
+      <c r="AE19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="X19" s="20">
+      <c r="AF19" s="22">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W20" s="19" t="s">
+    <row r="20" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I20" s="27"/>
+      <c r="AE20" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="X20" s="20">
+      <c r="AF20" s="22">
         <v>1001</v>
       </c>
     </row>
-    <row r="21" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W21" s="19" t="s">
+    <row r="21" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I21" s="27"/>
+      <c r="AE21" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="X21" s="20">
+      <c r="AF21" s="22">
         <v>999</v>
       </c>
     </row>
-    <row r="22" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W22" s="21" t="s">
+    <row r="22" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE22" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="X22" s="22"/>
-    </row>
-    <row r="23" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W23" s="19" t="s">
+      <c r="AF22" s="24"/>
+    </row>
+    <row r="23" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="X23" s="20">
+      <c r="AF23" s="22">
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W24" s="19" t="s">
+    <row r="24" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE24" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="X24" s="20">
+      <c r="AF24" s="22">
         <v>1102</v>
       </c>
     </row>
-    <row r="25" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W25" s="19" t="s">
+    <row r="25" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE25" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="X25" s="20">
+      <c r="AF25" s="22">
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W26" s="19" t="s">
+    <row r="26" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE26" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="X26" s="20">
+      <c r="AF26" s="22">
         <v>1201</v>
       </c>
     </row>
-    <row r="27" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W27" s="19" t="s">
+    <row r="27" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE27" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="X27" s="20">
+      <c r="AF27" s="22">
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W28" s="19" t="s">
+    <row r="28" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE28" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="X28" s="20">
+      <c r="AF28" s="22">
         <v>1301</v>
       </c>
     </row>
-    <row r="29" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W29" s="19" t="s">
+    <row r="29" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE29" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="X29" s="20">
+      <c r="AF29" s="22">
         <v>1400</v>
       </c>
     </row>
-    <row r="30" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W30" s="19" t="s">
+    <row r="30" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE30" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="X30" s="20">
+      <c r="AF30" s="22">
         <v>1401</v>
       </c>
     </row>
-    <row r="31" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W31" s="19" t="s">
+    <row r="31" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="X31" s="20">
+      <c r="AF31" s="22">
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W32" s="19" t="s">
+    <row r="32" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="AE32" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="X32" s="20">
+      <c r="AF32" s="22">
         <v>1501</v>
       </c>
     </row>
-    <row r="33" spans="23:24" x14ac:dyDescent="0.3">
-      <c r="W33" s="19" t="s">
+    <row r="33" spans="31:32" x14ac:dyDescent="0.3">
+      <c r="AE33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="X33" s="20">
+      <c r="AF33" s="22">
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="23:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="W34" s="6" t="s">
+    <row r="34" spans="31:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE34" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="X34" s="7">
+      <c r="AF34" s="7">
         <v>1601</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="I6:I21"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE22:AF22"/>
+    <mergeCell ref="S4:T4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create class Wing Goomba with basic feature: render. And fix bug related to Mario, ? Brick and Mushroom.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922AD90C-4754-4E20-BEA8-888D2A05785C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C3AE34-E96D-4B7D-8045-8053BEE16C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Wing Goomba</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -350,19 +353,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -390,17 +380,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -427,21 +459,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,6 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AJ34"/>
+  <dimension ref="B4:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J9"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,12 +826,14 @@
     <col min="14" max="14" width="12.6640625" customWidth="1"/>
     <col min="18" max="18" width="12.77734375" customWidth="1"/>
     <col min="19" max="19" width="12.33203125" customWidth="1"/>
-    <col min="27" max="27" width="15.88671875" customWidth="1"/>
-    <col min="31" max="31" width="15.33203125" customWidth="1"/>
-    <col min="35" max="35" width="11.88671875" customWidth="1"/>
+    <col min="21" max="21" width="10.77734375" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" customWidth="1"/>
+    <col min="29" max="29" width="15.88671875" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="37" max="37" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,467 +842,486 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="9" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="R4" s="11" t="s">
+      <c r="N4" s="7"/>
+      <c r="R4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="13" t="s">
+      <c r="T4" s="8"/>
+      <c r="U4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="8"/>
+      <c r="W4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="13" t="s">
+      <c r="X4" s="12"/>
+      <c r="Y4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="13" t="s">
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="13" t="s">
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="13" t="s">
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="13" t="s">
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="13" t="s">
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="13" t="s">
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="14"/>
-    </row>
-    <row r="5" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AL4" s="12"/>
+    </row>
+    <row r="5" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="12" t="s">
+      <c r="I5" s="32"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="V5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="W5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="X5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="15" t="s">
+      <c r="Z5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="15" t="s">
+      <c r="AB5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="15" t="s">
+      <c r="AC5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="15" t="s">
+      <c r="AD5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AE5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="15" t="s">
+      <c r="AF5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="12" t="s">
+      <c r="AG5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="12" t="s">
+      <c r="AH5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="12" t="s">
+      <c r="AI5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="12" t="s">
+      <c r="AJ5" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AK5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="8">
-        <v>1</v>
-      </c>
-      <c r="L6" s="8" t="s">
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="8">
-        <v>1</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="35">
         <v>5000</v>
       </c>
-      <c r="Y6" s="16" t="s">
+      <c r="U6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" s="27">
+        <v>5500</v>
+      </c>
+      <c r="AA6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Z6" s="17">
+      <c r="AB6" s="15">
         <v>10000</v>
       </c>
-      <c r="AA6" s="18" t="s">
+      <c r="AC6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AB6" s="18">
+      <c r="AD6" s="23">
         <v>10500</v>
       </c>
-      <c r="AC6" s="16" t="s">
+      <c r="AE6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AD6" s="18">
+      <c r="AF6" s="15">
         <v>11000</v>
       </c>
-      <c r="AE6" s="19" t="s">
+      <c r="AG6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="20"/>
-      <c r="AI6" t="s">
+      <c r="AH6" s="17"/>
+      <c r="AK6" t="s">
         <v>39</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>11000</v>
       </c>
     </row>
-    <row r="7" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:38" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="31"/>
-      <c r="S7" s="6" t="s">
+      <c r="I7" s="30"/>
+      <c r="J7" s="34"/>
+      <c r="S7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="25">
         <v>5001</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="AC7" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB7">
+      <c r="AD7" s="25">
         <v>10600</v>
       </c>
-      <c r="AE7" s="21" t="s">
+      <c r="AG7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AF7" s="22">
+      <c r="AH7" s="19">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:38" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="31"/>
-      <c r="AE8" s="21" t="s">
+      <c r="I8" s="30"/>
+      <c r="J8" s="34"/>
+      <c r="AG8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AF8" s="22">
+      <c r="AH8" s="19">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I9" s="27"/>
-      <c r="J9" s="31"/>
-      <c r="AE9" s="21" t="s">
+    <row r="9" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I9" s="30"/>
+      <c r="J9" s="34"/>
+      <c r="AG9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AF9" s="22">
+      <c r="AH9" s="19">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I10" s="27"/>
-      <c r="AE10" s="21" t="s">
+    <row r="10" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I10" s="30"/>
+      <c r="AG10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="AF10" s="22">
+      <c r="AH10" s="19">
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I11" s="27"/>
-      <c r="AE11" s="21" t="s">
+    <row r="11" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I11" s="30"/>
+      <c r="AG11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AF11" s="22">
+      <c r="AH11" s="19">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I12" s="27"/>
-      <c r="AE12" s="21" t="s">
+    <row r="12" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I12" s="30"/>
+      <c r="AG12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="AF12" s="22">
+      <c r="AH12" s="19">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I13" s="27"/>
-      <c r="AE13" s="21" t="s">
+    <row r="13" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I13" s="30"/>
+      <c r="AG13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AF13" s="22">
+      <c r="AH13" s="19">
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I14" s="27"/>
-      <c r="AE14" s="21" t="s">
+    <row r="14" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I14" s="30"/>
+      <c r="AG14" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AF14" s="22">
+      <c r="AH14" s="19">
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I15" s="27"/>
-      <c r="AE15" s="21" t="s">
+    <row r="15" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I15" s="30"/>
+      <c r="AG15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="AF15" s="22">
+      <c r="AH15" s="19">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="I16" s="27"/>
-      <c r="AE16" s="21" t="s">
+    <row r="16" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="I16" s="30"/>
+      <c r="AG16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="AF16" s="22">
+      <c r="AH16" s="19">
         <v>801</v>
       </c>
     </row>
-    <row r="17" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I17" s="27"/>
-      <c r="AE17" s="21" t="s">
+    <row r="17" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="I17" s="30"/>
+      <c r="AG17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AF17" s="22">
+      <c r="AH17" s="19">
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I18" s="27"/>
-      <c r="AE18" s="21" t="s">
+    <row r="18" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="I18" s="30"/>
+      <c r="AG18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AF18" s="22">
+      <c r="AH18" s="19">
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I19" s="27"/>
-      <c r="AE19" s="21" t="s">
+    <row r="19" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="I19" s="30"/>
+      <c r="AG19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AF19" s="22">
+      <c r="AH19" s="19">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I20" s="27"/>
-      <c r="AE20" s="21" t="s">
+    <row r="20" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="I20" s="30"/>
+      <c r="AG20" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AF20" s="22">
+      <c r="AH20" s="19">
         <v>1001</v>
       </c>
     </row>
-    <row r="21" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I21" s="27"/>
-      <c r="AE21" s="21" t="s">
+    <row r="21" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="I21" s="30"/>
+      <c r="AG21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AF21" s="22">
+      <c r="AH21" s="19">
         <v>999</v>
       </c>
     </row>
-    <row r="22" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE22" s="23" t="s">
+    <row r="22" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG22" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AF22" s="24"/>
-    </row>
-    <row r="23" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE23" s="21" t="s">
+      <c r="AH22" s="21"/>
+    </row>
+    <row r="23" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AF23" s="22">
+      <c r="AH23" s="19">
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE24" s="21" t="s">
+    <row r="24" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AF24" s="22">
+      <c r="AH24" s="19">
         <v>1102</v>
       </c>
     </row>
-    <row r="25" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE25" s="21" t="s">
+    <row r="25" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG25" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AF25" s="22">
+      <c r="AH25" s="19">
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE26" s="21" t="s">
+    <row r="26" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG26" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="AF26" s="22">
+      <c r="AH26" s="19">
         <v>1201</v>
       </c>
     </row>
-    <row r="27" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE27" s="21" t="s">
+    <row r="27" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AF27" s="22">
+      <c r="AH27" s="19">
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE28" s="21" t="s">
+    <row r="28" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="AF28" s="22">
+      <c r="AH28" s="19">
         <v>1301</v>
       </c>
     </row>
-    <row r="29" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE29" s="21" t="s">
+    <row r="29" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AF29" s="22">
+      <c r="AH29" s="19">
         <v>1400</v>
       </c>
     </row>
-    <row r="30" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE30" s="21" t="s">
+    <row r="30" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG30" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AF30" s="22">
+      <c r="AH30" s="19">
         <v>1401</v>
       </c>
     </row>
-    <row r="31" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE31" s="21" t="s">
+    <row r="31" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG31" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AF31" s="22">
+      <c r="AH31" s="19">
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="AE32" s="21" t="s">
+    <row r="32" spans="9:34" x14ac:dyDescent="0.3">
+      <c r="AG32" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AF32" s="22">
+      <c r="AH32" s="19">
         <v>1501</v>
       </c>
     </row>
-    <row r="33" spans="31:32" x14ac:dyDescent="0.3">
-      <c r="AE33" s="21" t="s">
+    <row r="33" spans="33:34" x14ac:dyDescent="0.3">
+      <c r="AG33" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="AF33" s="22">
+      <c r="AH33" s="19">
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="31:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AE34" s="6" t="s">
+    <row r="34" spans="33:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF34" s="7">
+      <c r="AH34" s="5">
         <v>1601</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AI4:AJ4"/>
+  <mergeCells count="16">
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
-    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="U4:V4"/>
     <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE22:AF22"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AG22:AH22"/>
     <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Wing Goomba now have flying animation.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C3AE34-E96D-4B7D-8045-8053BEE16C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EEB6D6-4FA6-4487-B0C5-4370D6627C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Wing Goomba</t>
+  </si>
+  <si>
+    <t>Flying</t>
   </si>
 </sst>
 </file>
@@ -813,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,8 +1059,12 @@
       <c r="T7" s="25">
         <v>5001</v>
       </c>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
+      <c r="U7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="V7" s="28">
+        <v>5510</v>
+      </c>
       <c r="AC7" s="24" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Koopa now can move and collide with Blocking object.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EEB6D6-4FA6-4487-B0C5-4370D6627C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC02008-0A15-4779-8999-8CA7E9F6F0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -180,7 +180,31 @@
     <t>Wing Goomba</t>
   </si>
   <si>
-    <t>Flying</t>
+    <t>Have wing, Walking</t>
+  </si>
+  <si>
+    <t>Have wing, Flying</t>
+  </si>
+  <si>
+    <t>No wing, walking</t>
+  </si>
+  <si>
+    <t>Koopa</t>
+  </si>
+  <si>
+    <t>Các bug đã gặp trong quá trình thực hiện Project Mario</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Vector subscript out of range</t>
+  </si>
+  <si>
+    <t>Nguyên nhân</t>
+  </si>
+  <si>
+    <t>Thiếu "break" khi tạo object ở chỗ switch case trong Playscene.cpp</t>
   </si>
 </sst>
 </file>
@@ -431,8 +455,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -482,6 +509,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,6 +530,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AL34"/>
+  <dimension ref="B3:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4:AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,508 +858,567 @@
     <col min="6" max="8" width="16" customWidth="1"/>
     <col min="12" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.77734375" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" customWidth="1"/>
-    <col min="29" max="29" width="15.88671875" customWidth="1"/>
-    <col min="33" max="33" width="15.33203125" customWidth="1"/>
-    <col min="37" max="37" width="11.88671875" customWidth="1"/>
+    <col min="18" max="20" width="12.77734375" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" customWidth="1"/>
+    <col min="23" max="23" width="17.5546875" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" customWidth="1"/>
+    <col min="31" max="31" width="15.88671875" customWidth="1"/>
+    <col min="35" max="35" width="15.33203125" customWidth="1"/>
+    <col min="39" max="39" width="11.88671875" customWidth="1"/>
+    <col min="45" max="45" width="26.44140625" customWidth="1"/>
+    <col min="46" max="46" width="56.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+    <row r="3" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="AR3" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+    </row>
+    <row r="4" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="7" t="s">
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="R4" s="9" t="s">
+      <c r="N4" s="8"/>
+      <c r="R4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="9"/>
+      <c r="W4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="8"/>
-      <c r="W4" s="11" t="s">
+      <c r="X4" s="9"/>
+      <c r="Y4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="11" t="s">
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="11" t="s">
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="11" t="s">
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="11" t="s">
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="11" t="s">
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="11" t="s">
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="11" t="s">
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="12"/>
-    </row>
-    <row r="5" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AN4" s="13"/>
+      <c r="AR4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT4" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="10" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="V5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="Z5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="13" t="s">
+      <c r="AA5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AB5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="13" t="s">
+      <c r="AC5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="13" t="s">
+      <c r="AD5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AE5" s="13" t="s">
+      <c r="AE5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="13" t="s">
+      <c r="AF5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="13" t="s">
+      <c r="AG5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="13" t="s">
+      <c r="AH5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="10" t="s">
+      <c r="AI5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="10" t="s">
+      <c r="AJ5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AK5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="10" t="s">
+      <c r="AL5" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AM5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="7">
         <v>0</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>0</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="22" t="s">
+      <c r="S6" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="37">
+        <v>6000</v>
+      </c>
+      <c r="U6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="35">
+      <c r="V6" s="37">
         <v>5000</v>
       </c>
-      <c r="U6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" s="27">
+      <c r="W6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="28">
         <v>5500</v>
       </c>
-      <c r="AA6" s="14" t="s">
+      <c r="AC6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="15">
+      <c r="AD6" s="16">
         <v>10000</v>
       </c>
-      <c r="AC6" s="22" t="s">
+      <c r="AE6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AD6" s="23">
+      <c r="AF6" s="24">
         <v>10500</v>
       </c>
-      <c r="AE6" s="15" t="s">
+      <c r="AG6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="AF6" s="15">
+      <c r="AH6" s="16">
         <v>11000</v>
       </c>
-      <c r="AG6" s="16" t="s">
+      <c r="AI6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AH6" s="17"/>
-      <c r="AK6" t="s">
+      <c r="AJ6" s="18"/>
+      <c r="AM6" t="s">
         <v>39</v>
       </c>
-      <c r="AL6">
+      <c r="AN6">
         <v>11000</v>
       </c>
     </row>
-    <row r="7" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="E7" s="3" t="s">
+    <row r="7" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="34"/>
-      <c r="S7" s="24" t="s">
+      <c r="I7" s="32"/>
+      <c r="J7" s="36"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="T7" s="25">
+      <c r="V7" s="26">
         <v>5001</v>
       </c>
-      <c r="U7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="V7" s="28">
+      <c r="W7" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="30">
         <v>5510</v>
       </c>
-      <c r="AC7" s="24" t="s">
+      <c r="AE7" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="AD7" s="25">
+      <c r="AF7" s="26">
         <v>10600</v>
       </c>
-      <c r="AG7" s="18" t="s">
+      <c r="AI7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AH7" s="19">
+      <c r="AJ7" s="20">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:49" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="34"/>
-      <c r="AG8" s="18" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="36"/>
+      <c r="W8" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="X8">
+        <v>5520</v>
+      </c>
+      <c r="AI8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AH8" s="19">
+      <c r="AJ8" s="20">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I9" s="30"/>
-      <c r="J9" s="34"/>
-      <c r="AG9" s="18" t="s">
+    <row r="9" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I9" s="32"/>
+      <c r="J9" s="36"/>
+      <c r="W9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="X9">
+        <v>5530</v>
+      </c>
+      <c r="AI9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="19">
+      <c r="AJ9" s="20">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I10" s="30"/>
-      <c r="AG10" s="18" t="s">
+    <row r="10" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I10" s="32"/>
+      <c r="AI10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AH10" s="19">
+      <c r="AJ10" s="20">
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I11" s="30"/>
-      <c r="AG11" s="18" t="s">
+    <row r="11" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I11" s="32"/>
+      <c r="AI11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AH11" s="19">
+      <c r="AJ11" s="20">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I12" s="30"/>
-      <c r="AG12" s="18" t="s">
+    <row r="12" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I12" s="32"/>
+      <c r="AI12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AH12" s="19">
+      <c r="AJ12" s="20">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I13" s="30"/>
-      <c r="AG13" s="18" t="s">
+    <row r="13" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I13" s="32"/>
+      <c r="AI13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AH13" s="19">
+      <c r="AJ13" s="20">
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I14" s="30"/>
-      <c r="AG14" s="18" t="s">
+    <row r="14" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I14" s="32"/>
+      <c r="AI14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AH14" s="19">
+      <c r="AJ14" s="20">
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I15" s="30"/>
-      <c r="AG15" s="18" t="s">
+    <row r="15" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I15" s="32"/>
+      <c r="AI15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AH15" s="19">
+      <c r="AJ15" s="20">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="I16" s="30"/>
-      <c r="AG16" s="18" t="s">
+    <row r="16" spans="2:49" x14ac:dyDescent="0.3">
+      <c r="I16" s="32"/>
+      <c r="AI16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AH16" s="19">
+      <c r="AJ16" s="20">
         <v>801</v>
       </c>
     </row>
-    <row r="17" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="I17" s="30"/>
-      <c r="AG17" s="18" t="s">
+    <row r="17" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I17" s="32"/>
+      <c r="AI17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="AH17" s="19">
+      <c r="AJ17" s="20">
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="I18" s="30"/>
-      <c r="AG18" s="18" t="s">
+    <row r="18" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I18" s="32"/>
+      <c r="AI18" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AH18" s="19">
+      <c r="AJ18" s="20">
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="I19" s="30"/>
-      <c r="AG19" s="18" t="s">
+    <row r="19" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I19" s="32"/>
+      <c r="AI19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AH19" s="19">
+      <c r="AJ19" s="20">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="I20" s="30"/>
-      <c r="AG20" s="18" t="s">
+    <row r="20" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I20" s="32"/>
+      <c r="AI20" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AH20" s="19">
+      <c r="AJ20" s="20">
         <v>1001</v>
       </c>
     </row>
-    <row r="21" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="I21" s="30"/>
-      <c r="AG21" s="18" t="s">
+    <row r="21" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I21" s="32"/>
+      <c r="AI21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AH21" s="19">
+      <c r="AJ21" s="20">
         <v>999</v>
       </c>
     </row>
-    <row r="22" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG22" s="20" t="s">
+    <row r="22" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI22" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="AH22" s="21"/>
-    </row>
-    <row r="23" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG23" s="18" t="s">
+      <c r="AJ22" s="22"/>
+    </row>
+    <row r="23" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AH23" s="19">
+      <c r="AJ23" s="20">
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG24" s="18" t="s">
+    <row r="24" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI24" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AH24" s="19">
+      <c r="AJ24" s="20">
         <v>1102</v>
       </c>
     </row>
-    <row r="25" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG25" s="18" t="s">
+    <row r="25" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI25" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AH25" s="19">
+      <c r="AJ25" s="20">
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG26" s="18" t="s">
+    <row r="26" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI26" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AH26" s="19">
+      <c r="AJ26" s="20">
         <v>1201</v>
       </c>
     </row>
-    <row r="27" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG27" s="18" t="s">
+    <row r="27" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI27" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AH27" s="19">
+      <c r="AJ27" s="20">
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG28" s="18" t="s">
+    <row r="28" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI28" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AH28" s="19">
+      <c r="AJ28" s="20">
         <v>1301</v>
       </c>
     </row>
-    <row r="29" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG29" s="18" t="s">
+    <row r="29" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI29" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AH29" s="19">
+      <c r="AJ29" s="20">
         <v>1400</v>
       </c>
     </row>
-    <row r="30" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG30" s="18" t="s">
+    <row r="30" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI30" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AH30" s="19">
+      <c r="AJ30" s="20">
         <v>1401</v>
       </c>
     </row>
-    <row r="31" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG31" s="18" t="s">
+    <row r="31" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI31" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AH31" s="19">
+      <c r="AJ31" s="20">
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="9:34" x14ac:dyDescent="0.3">
-      <c r="AG32" s="18" t="s">
+    <row r="32" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI32" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AH32" s="19">
+      <c r="AJ32" s="20">
         <v>1501</v>
       </c>
     </row>
-    <row r="33" spans="33:34" x14ac:dyDescent="0.3">
-      <c r="AG33" s="18" t="s">
+    <row r="33" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI33" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AH33" s="19">
+      <c r="AJ33" s="20">
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="33:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AG34" s="4" t="s">
+    <row r="34" spans="35:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AI34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AH34" s="5">
+      <c r="AJ34" s="6">
         <v>1601</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AK4:AL4"/>
+  <mergeCells count="18">
+    <mergeCell ref="AR3:AW3"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AM4:AN4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="W4:X4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AG22:AH22"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="U4:V4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="S4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test all the ani_id of Koopa, but need to find another sprite sheet to get some animation of Koopa.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC02008-0A15-4779-8999-8CA7E9F6F0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2F720E-0D23-4FF5-89BD-CFD853DCB43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Thiếu "break" khi tạo object ở chỗ switch case trong Playscene.cpp</t>
+  </si>
+  <si>
+    <t>Shelling</t>
+  </si>
+  <si>
+    <t>Spin Shell</t>
   </si>
 </sst>
 </file>
@@ -847,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B3:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4:AT4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,8 +1133,12 @@
       </c>
       <c r="I7" s="32"/>
       <c r="J7" s="36"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="26"/>
+      <c r="S7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="26">
+        <v>6001</v>
+      </c>
       <c r="U7" s="25" t="s">
         <v>14</v>
       </c>
@@ -1160,6 +1170,12 @@
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="36"/>
+      <c r="S8" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8">
+        <v>6002</v>
+      </c>
       <c r="W8" s="38" t="s">
         <v>50</v>
       </c>
@@ -1176,6 +1192,12 @@
     <row r="9" spans="2:49" x14ac:dyDescent="0.3">
       <c r="I9" s="32"/>
       <c r="J9" s="36"/>
+      <c r="S9" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9">
+        <v>6003</v>
+      </c>
       <c r="W9" s="38" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Replace old Koopa's sprite with new sprites, now Koopa have all of its sprites.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2F720E-0D23-4FF5-89BD-CFD853DCB43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513855A7-1C7F-484D-9239-446C48930968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -210,7 +210,10 @@
     <t>Shelling</t>
   </si>
   <si>
-    <t>Spin Shell</t>
+    <t>Spin Shell Left</t>
+  </si>
+  <si>
+    <t>Spin Shell Right</t>
   </si>
 </sst>
 </file>
@@ -854,7 +857,7 @@
   <dimension ref="B3:AW34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,6 +1216,12 @@
     </row>
     <row r="10" spans="2:49" x14ac:dyDescent="0.3">
       <c r="I10" s="32"/>
+      <c r="S10" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10">
+        <v>6004</v>
+      </c>
       <c r="AI10" s="19" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Fix bug Wing Goomba can't fly after collide with blocking obejct in x-axis.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513855A7-1C7F-484D-9239-446C48930968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E981D9CB-994F-440A-8C79-C37642563EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -192,9 +194,6 @@
     <t>Koopa</t>
   </si>
   <si>
-    <t>Các bug đã gặp trong quá trình thực hiện Project Mario</t>
-  </si>
-  <si>
     <t>Tên</t>
   </si>
   <si>
@@ -214,6 +213,39 @@
   </si>
   <si>
     <t>Spin Shell Right</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Tình trạng</t>
+  </si>
+  <si>
+    <t>Giải quyết chưa?</t>
+  </si>
+  <si>
+    <t>Wing Goomba đi một khoảng  cách dài hơn quy định thì mới chịu bay</t>
+  </si>
+  <si>
+    <t>Xảy ra khi</t>
+  </si>
+  <si>
+    <t>Đi được một đoạn ngắn hơn khoảng cách để bay, đụng vào tường, đổi hướng đi, sau đó nếu đi hết một đoạn thẳng mà không đụng tường thì mới có thể bay được</t>
+  </si>
+  <si>
+    <t>Do chỉ xét vị trí cũ và mới chứ không xét quãng đường thực sự đi được nên mới gặp hiện tường này.</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Bug phát hiện trong Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quá trình làm Project nhưng không quá nghiêm trọng hoặc cần nhiều thời gian để xử lý</t>
+  </si>
+  <si>
+    <t>Các bug về mặt kĩ thuật</t>
   </si>
 </sst>
 </file>
@@ -464,11 +496,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,70 +505,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B3:AW34"/>
+  <dimension ref="B4:AN34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView topLeftCell="AS1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3:BG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,252 +919,230 @@
     <col min="31" max="31" width="15.88671875" customWidth="1"/>
     <col min="35" max="35" width="15.33203125" customWidth="1"/>
     <col min="39" max="39" width="11.88671875" customWidth="1"/>
-    <col min="45" max="45" width="26.44140625" customWidth="1"/>
-    <col min="46" max="46" width="56.44140625" customWidth="1"/>
+    <col min="44" max="44" width="63.77734375" customWidth="1"/>
+    <col min="45" max="45" width="47.33203125" customWidth="1"/>
+    <col min="46" max="46" width="26.44140625" customWidth="1"/>
+    <col min="47" max="47" width="56.44140625" customWidth="1"/>
+    <col min="48" max="48" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="AR3" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-    </row>
-    <row r="4" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="8" t="s">
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8" t="s">
+      <c r="L4" s="29"/>
+      <c r="M4" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="R4" s="10" t="s">
+      <c r="N4" s="29"/>
+      <c r="R4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9" t="s">
+      <c r="T4" s="34"/>
+      <c r="U4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9" t="s">
+      <c r="V4" s="34"/>
+      <c r="W4" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="12" t="s">
+      <c r="X4" s="34"/>
+      <c r="Y4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="12" t="s">
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="12" t="s">
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="12" t="s">
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="12" t="s">
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="12" t="s">
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="12" t="s">
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="12" t="s">
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="AN4" s="13"/>
-      <c r="AR4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AT4" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="2:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AN4" s="28"/>
+    </row>
+    <row r="5" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="S5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="V5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="W5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="14" t="s">
+      <c r="X5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Y5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="Z5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="AA5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="AB5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="14" t="s">
+      <c r="AC5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="14" t="s">
+      <c r="AD5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AE5" s="14" t="s">
+      <c r="AE5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="14" t="s">
+      <c r="AF5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="14" t="s">
+      <c r="AG5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="14" t="s">
+      <c r="AH5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="14" t="s">
+      <c r="AI5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="14" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="11" t="s">
+      <c r="AK5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AL5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="11" t="s">
+      <c r="AM5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AN5" s="11" t="s">
+      <c r="AN5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>0</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="S6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="37">
+      <c r="T6" s="23">
         <v>6000</v>
       </c>
-      <c r="U6" s="23" t="s">
+      <c r="U6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="37">
+      <c r="V6" s="23">
         <v>5000</v>
       </c>
-      <c r="W6" s="27" t="s">
+      <c r="W6" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="X6" s="28">
+      <c r="X6" s="19">
         <v>5500</v>
       </c>
-      <c r="AC6" s="15" t="s">
+      <c r="AC6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AD6" s="16">
+      <c r="AD6" s="11">
         <v>10000</v>
       </c>
-      <c r="AE6" s="23" t="s">
+      <c r="AE6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AF6" s="24">
+      <c r="AF6" s="15">
         <v>10500</v>
       </c>
-      <c r="AG6" s="16" t="s">
+      <c r="AG6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AH6" s="16">
+      <c r="AH6" s="11">
         <v>11000</v>
       </c>
-      <c r="AI6" s="17" t="s">
+      <c r="AI6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="AJ6" s="18"/>
+      <c r="AJ6" s="36"/>
       <c r="AM6" t="s">
         <v>39</v>
       </c>
@@ -1127,331 +1150,547 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="7" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="E7" s="4" t="s">
+    <row r="7" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="36"/>
-      <c r="S7" s="25" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="33"/>
+      <c r="S7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T7" s="17">
         <v>6001</v>
       </c>
-      <c r="U7" s="25" t="s">
+      <c r="U7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="26">
+      <c r="V7" s="17">
         <v>5001</v>
       </c>
-      <c r="W7" s="30" t="s">
+      <c r="W7" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="X7" s="30">
+      <c r="X7" s="20">
         <v>5510</v>
       </c>
-      <c r="AE7" s="25" t="s">
+      <c r="AE7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AF7" s="26">
+      <c r="AF7" s="17">
         <v>10600</v>
       </c>
-      <c r="AI7" s="19" t="s">
+      <c r="AI7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AJ7" s="20">
+      <c r="AJ7" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:40" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="36"/>
-      <c r="S8" s="38" t="s">
-        <v>57</v>
+      <c r="I8" s="31"/>
+      <c r="J8" s="33"/>
+      <c r="S8" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="T8">
         <v>6002</v>
       </c>
-      <c r="W8" s="38" t="s">
+      <c r="W8" s="24" t="s">
         <v>50</v>
       </c>
       <c r="X8">
         <v>5520</v>
       </c>
-      <c r="AI8" s="19" t="s">
+      <c r="AI8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AJ8" s="20">
+      <c r="AJ8" s="13">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I9" s="32"/>
-      <c r="J9" s="36"/>
-      <c r="S9" s="38" t="s">
-        <v>58</v>
+    <row r="9" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I9" s="31"/>
+      <c r="J9" s="33"/>
+      <c r="S9" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="T9">
         <v>6003</v>
       </c>
-      <c r="W9" s="38" t="s">
+      <c r="W9" s="24" t="s">
         <v>14</v>
       </c>
       <c r="X9">
         <v>5530</v>
       </c>
-      <c r="AI9" s="19" t="s">
+      <c r="AI9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AJ9" s="20">
+      <c r="AJ9" s="13">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I10" s="32"/>
-      <c r="S10" s="38" t="s">
-        <v>59</v>
+    <row r="10" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I10" s="31"/>
+      <c r="S10" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="T10">
         <v>6004</v>
       </c>
-      <c r="AI10" s="19" t="s">
+      <c r="AI10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ10" s="20">
+      <c r="AJ10" s="13">
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I11" s="32"/>
-      <c r="AI11" s="19" t="s">
+    <row r="11" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I11" s="31"/>
+      <c r="AI11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AJ11" s="20">
+      <c r="AJ11" s="13">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I12" s="32"/>
-      <c r="AI12" s="19" t="s">
+    <row r="12" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I12" s="31"/>
+      <c r="AI12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ12" s="20">
+      <c r="AJ12" s="13">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I13" s="32"/>
-      <c r="AI13" s="19" t="s">
+    <row r="13" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I13" s="31"/>
+      <c r="AI13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AJ13" s="20">
+      <c r="AJ13" s="13">
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I14" s="32"/>
-      <c r="AI14" s="19" t="s">
+    <row r="14" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I14" s="31"/>
+      <c r="AI14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AJ14" s="20">
+      <c r="AJ14" s="13">
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I15" s="32"/>
-      <c r="AI15" s="19" t="s">
+    <row r="15" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I15" s="31"/>
+      <c r="AI15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AJ15" s="20">
+      <c r="AJ15" s="13">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="I16" s="32"/>
-      <c r="AI16" s="19" t="s">
+    <row r="16" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="I16" s="31"/>
+      <c r="AI16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AJ16" s="20">
+      <c r="AJ16" s="13">
         <v>801</v>
       </c>
     </row>
     <row r="17" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I17" s="32"/>
-      <c r="AI17" s="19" t="s">
+      <c r="I17" s="31"/>
+      <c r="AI17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AJ17" s="20">
+      <c r="AJ17" s="13">
         <v>900</v>
       </c>
     </row>
     <row r="18" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I18" s="32"/>
-      <c r="AI18" s="19" t="s">
+      <c r="I18" s="31"/>
+      <c r="AI18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AJ18" s="20">
+      <c r="AJ18" s="13">
         <v>901</v>
       </c>
     </row>
     <row r="19" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I19" s="32"/>
-      <c r="AI19" s="19" t="s">
+      <c r="I19" s="31"/>
+      <c r="AI19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ19" s="20">
+      <c r="AJ19" s="13">
         <v>1000</v>
       </c>
     </row>
     <row r="20" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I20" s="32"/>
-      <c r="AI20" s="19" t="s">
+      <c r="I20" s="31"/>
+      <c r="AI20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AJ20" s="20">
+      <c r="AJ20" s="13">
         <v>1001</v>
       </c>
     </row>
     <row r="21" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I21" s="32"/>
-      <c r="AI21" s="19" t="s">
+      <c r="I21" s="31"/>
+      <c r="AI21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AJ21" s="20">
+      <c r="AJ21" s="13">
         <v>999</v>
       </c>
     </row>
     <row r="22" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI22" s="21" t="s">
+      <c r="AI22" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AJ22" s="22"/>
+      <c r="AJ22" s="38"/>
     </row>
     <row r="23" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI23" s="19" t="s">
+      <c r="AI23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AJ23" s="20">
+      <c r="AJ23" s="13">
         <v>1100</v>
       </c>
     </row>
     <row r="24" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI24" s="19" t="s">
+      <c r="AI24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AJ24" s="20">
+      <c r="AJ24" s="13">
         <v>1102</v>
       </c>
     </row>
     <row r="25" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI25" s="19" t="s">
+      <c r="AI25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AJ25" s="20">
+      <c r="AJ25" s="13">
         <v>1200</v>
       </c>
     </row>
     <row r="26" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI26" s="19" t="s">
+      <c r="AI26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ26" s="20">
+      <c r="AJ26" s="13">
         <v>1201</v>
       </c>
     </row>
     <row r="27" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI27" s="19" t="s">
+      <c r="AI27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AJ27" s="20">
+      <c r="AJ27" s="13">
         <v>1300</v>
       </c>
     </row>
     <row r="28" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI28" s="19" t="s">
+      <c r="AI28" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ28" s="20">
+      <c r="AJ28" s="13">
         <v>1301</v>
       </c>
     </row>
     <row r="29" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI29" s="19" t="s">
+      <c r="AI29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ29" s="20">
+      <c r="AJ29" s="13">
         <v>1400</v>
       </c>
     </row>
     <row r="30" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI30" s="19" t="s">
+      <c r="AI30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AJ30" s="20">
+      <c r="AJ30" s="13">
         <v>1401</v>
       </c>
     </row>
     <row r="31" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI31" s="19" t="s">
+      <c r="AI31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AJ31" s="20">
+      <c r="AJ31" s="13">
         <v>1500</v>
       </c>
     </row>
     <row r="32" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI32" s="19" t="s">
+      <c r="AI32" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AJ32" s="20">
+      <c r="AJ32" s="13">
         <v>1501</v>
       </c>
     </row>
     <row r="33" spans="35:36" x14ac:dyDescent="0.3">
-      <c r="AI33" s="19" t="s">
+      <c r="AI33" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AJ33" s="20">
+      <c r="AJ33" s="13">
         <v>1600</v>
       </c>
     </row>
     <row r="34" spans="35:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AI34" s="5" t="s">
+      <c r="AI34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ34" s="6">
+      <c r="AJ34" s="5">
         <v>1601</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AR3:AW3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
+  <mergeCells count="17">
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="S4:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42">
+        <v>1</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
+  <dimension ref="B4:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create object to help Koopa turn around when reach end of platform, currently just have basic feature like rendering.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E981D9CB-994F-440A-8C79-C37642563EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB30EF-59D4-47F4-85BA-3A62CE66A197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>Các bug về mặt kĩ thuật</t>
+  </si>
+  <si>
+    <t>ChangeDirectionOnPlatform</t>
+  </si>
+  <si>
+    <t>CDOP</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -528,49 +534,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -582,8 +548,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AN34"/>
+  <dimension ref="B4:AP34"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3:BG5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,21 +927,21 @@
     <col min="6" max="8" width="16" customWidth="1"/>
     <col min="12" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="18" max="20" width="12.77734375" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" customWidth="1"/>
-    <col min="23" max="23" width="17.5546875" customWidth="1"/>
-    <col min="24" max="24" width="8.88671875" customWidth="1"/>
-    <col min="31" max="31" width="15.88671875" customWidth="1"/>
-    <col min="35" max="35" width="15.33203125" customWidth="1"/>
-    <col min="39" max="39" width="11.88671875" customWidth="1"/>
-    <col min="44" max="44" width="63.77734375" customWidth="1"/>
-    <col min="45" max="45" width="47.33203125" customWidth="1"/>
-    <col min="46" max="46" width="26.44140625" customWidth="1"/>
-    <col min="47" max="47" width="56.44140625" customWidth="1"/>
-    <col min="48" max="48" width="14.44140625" customWidth="1"/>
+    <col min="18" max="22" width="12.77734375" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" customWidth="1"/>
+    <col min="41" max="41" width="11.88671875" customWidth="1"/>
+    <col min="46" max="46" width="63.77734375" customWidth="1"/>
+    <col min="47" max="47" width="47.33203125" customWidth="1"/>
+    <col min="48" max="48" width="26.44140625" customWidth="1"/>
+    <col min="49" max="49" width="56.44140625" customWidth="1"/>
+    <col min="50" max="50" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,63 +952,67 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29" t="s">
+      <c r="L4" s="40"/>
+      <c r="M4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="29"/>
+      <c r="N4" s="40"/>
       <c r="R4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="34" t="s">
+      <c r="S4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34" t="s">
+      <c r="T4" s="31"/>
+      <c r="U4" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34" t="s">
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="27" t="s">
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="27" t="s">
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="27" t="s">
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="27" t="s">
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="27" t="s">
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="27" t="s">
+      <c r="AJ4" s="33"/>
+      <c r="AK4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="27" t="s">
+      <c r="AL4" s="33"/>
+      <c r="AM4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="27" t="s">
+      <c r="AN4" s="33"/>
+      <c r="AO4" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="AN4" s="28"/>
-    </row>
-    <row r="5" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AP4" s="33"/>
+    </row>
+    <row r="5" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1011,31 +1030,31 @@
       <c r="N5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="T5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="U5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="9" t="s">
+      <c r="V5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="X5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Y5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="Z5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AA5" s="8" t="s">
@@ -1044,10 +1063,10 @@
       <c r="AB5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AC5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AD5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AE5" s="9" t="s">
@@ -1068,10 +1087,10 @@
       <c r="AJ5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="8" t="s">
+      <c r="AL5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AM5" s="8" t="s">
@@ -1080,15 +1099,21 @@
       <c r="AN5" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AO5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="36" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="6">
@@ -1103,375 +1128,384 @@
       <c r="N6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="23">
+      <c r="T6" s="6">
         <v>6000</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" s="20">
+        <v>7000</v>
+      </c>
+      <c r="W6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="23">
+      <c r="X6" s="6">
         <v>5000</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="Y6" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="X6" s="19">
+      <c r="Z6" s="19">
         <v>5500</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="AE6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AF6" s="11">
         <v>10000</v>
       </c>
-      <c r="AE6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AF6" s="15">
+      <c r="AH6" s="15">
         <v>10500</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AI6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AJ6" s="11">
         <v>11000</v>
       </c>
-      <c r="AI6" s="35" t="s">
+      <c r="AK6" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AJ6" s="36"/>
-      <c r="AM6" t="s">
+      <c r="AL6" s="39"/>
+      <c r="AO6" t="s">
         <v>39</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>11000</v>
       </c>
     </row>
-    <row r="7" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="33"/>
-      <c r="S7" s="16" t="s">
+      <c r="I7" s="35"/>
+      <c r="J7" s="37"/>
+      <c r="S7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="6">
         <v>6001</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="17">
+      <c r="X7" s="6">
         <v>5001</v>
       </c>
-      <c r="W7" s="20" t="s">
+      <c r="Y7" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="X7" s="20">
+      <c r="Z7" s="20">
         <v>5510</v>
       </c>
-      <c r="AE7" s="16" t="s">
+      <c r="AG7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AF7" s="17">
+      <c r="AH7" s="17">
         <v>10600</v>
       </c>
-      <c r="AI7" s="12" t="s">
+      <c r="AK7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AJ7" s="13">
+      <c r="AL7" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="33"/>
-      <c r="S8" s="24" t="s">
+      <c r="I8" s="35"/>
+      <c r="J8" s="37"/>
+      <c r="S8" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="6">
         <v>6002</v>
       </c>
-      <c r="W8" s="24" t="s">
+      <c r="Y8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AI8" s="12" t="s">
+      <c r="AK8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AJ8" s="13">
+      <c r="AL8" s="13">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I9" s="31"/>
-      <c r="J9" s="33"/>
-      <c r="S9" s="24" t="s">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I9" s="35"/>
+      <c r="J9" s="37"/>
+      <c r="S9" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="6">
         <v>6003</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="Y9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AI9" s="12" t="s">
+      <c r="AK9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AJ9" s="13">
+      <c r="AL9" s="13">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I10" s="31"/>
-      <c r="S10" s="24" t="s">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I10" s="35"/>
+      <c r="S10" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="6">
         <v>6004</v>
       </c>
-      <c r="AI10" s="12" t="s">
+      <c r="AK10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ10" s="13">
+      <c r="AL10" s="13">
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I11" s="31"/>
-      <c r="AI11" s="12" t="s">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I11" s="35"/>
+      <c r="AK11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AJ11" s="13">
+      <c r="AL11" s="13">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I12" s="31"/>
-      <c r="AI12" s="12" t="s">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I12" s="35"/>
+      <c r="AK12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ12" s="13">
+      <c r="AL12" s="13">
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I13" s="31"/>
-      <c r="AI13" s="12" t="s">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I13" s="35"/>
+      <c r="AK13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AJ13" s="13">
+      <c r="AL13" s="13">
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I14" s="31"/>
-      <c r="AI14" s="12" t="s">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I14" s="35"/>
+      <c r="AK14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AJ14" s="13">
+      <c r="AL14" s="13">
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I15" s="31"/>
-      <c r="AI15" s="12" t="s">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I15" s="35"/>
+      <c r="AK15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AJ15" s="13">
+      <c r="AL15" s="13">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.3">
-      <c r="I16" s="31"/>
-      <c r="AI16" s="12" t="s">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="I16" s="35"/>
+      <c r="AK16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AJ16" s="13">
+      <c r="AL16" s="13">
         <v>801</v>
       </c>
     </row>
-    <row r="17" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I17" s="31"/>
-      <c r="AI17" s="12" t="s">
+    <row r="17" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="I17" s="35"/>
+      <c r="AK17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AJ17" s="13">
+      <c r="AL17" s="13">
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I18" s="31"/>
-      <c r="AI18" s="12" t="s">
+    <row r="18" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="I18" s="35"/>
+      <c r="AK18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AJ18" s="13">
+      <c r="AL18" s="13">
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I19" s="31"/>
-      <c r="AI19" s="12" t="s">
+    <row r="19" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="I19" s="35"/>
+      <c r="AK19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ19" s="13">
+      <c r="AL19" s="13">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I20" s="31"/>
-      <c r="AI20" s="12" t="s">
+    <row r="20" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="I20" s="35"/>
+      <c r="AK20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AJ20" s="13">
+      <c r="AL20" s="13">
         <v>1001</v>
       </c>
     </row>
-    <row r="21" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I21" s="31"/>
-      <c r="AI21" s="12" t="s">
+    <row r="21" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="I21" s="35"/>
+      <c r="AK21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AJ21" s="13">
+      <c r="AL21" s="13">
         <v>999</v>
       </c>
     </row>
-    <row r="22" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI22" s="37" t="s">
+    <row r="22" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK22" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="AJ22" s="38"/>
-    </row>
-    <row r="23" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI23" s="12" t="s">
+      <c r="AL22" s="30"/>
+    </row>
+    <row r="23" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AJ23" s="13">
+      <c r="AL23" s="13">
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI24" s="12" t="s">
+    <row r="24" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AJ24" s="13">
+      <c r="AL24" s="13">
         <v>1102</v>
       </c>
     </row>
-    <row r="25" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI25" s="12" t="s">
+    <row r="25" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AJ25" s="13">
+      <c r="AL25" s="13">
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI26" s="12" t="s">
+    <row r="26" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ26" s="13">
+      <c r="AL26" s="13">
         <v>1201</v>
       </c>
     </row>
-    <row r="27" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI27" s="12" t="s">
+    <row r="27" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AJ27" s="13">
+      <c r="AL27" s="13">
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI28" s="12" t="s">
+    <row r="28" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK28" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ28" s="13">
+      <c r="AL28" s="13">
         <v>1301</v>
       </c>
     </row>
-    <row r="29" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI29" s="12" t="s">
+    <row r="29" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ29" s="13">
+      <c r="AL29" s="13">
         <v>1400</v>
       </c>
     </row>
-    <row r="30" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI30" s="12" t="s">
+    <row r="30" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AJ30" s="13">
+      <c r="AL30" s="13">
         <v>1401</v>
       </c>
     </row>
-    <row r="31" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI31" s="12" t="s">
+    <row r="31" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AJ31" s="13">
+      <c r="AL31" s="13">
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI32" s="12" t="s">
+    <row r="32" spans="9:38" x14ac:dyDescent="0.3">
+      <c r="AK32" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AJ32" s="13">
+      <c r="AL32" s="13">
         <v>1501</v>
       </c>
     </row>
-    <row r="33" spans="35:36" x14ac:dyDescent="0.3">
-      <c r="AI33" s="12" t="s">
+    <row r="33" spans="37:38" x14ac:dyDescent="0.3">
+      <c r="AK33" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AJ33" s="13">
+      <c r="AL33" s="13">
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="35:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AI34" s="4" t="s">
+    <row r="34" spans="37:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AK34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ34" s="5">
+      <c r="AL34" s="5">
         <v>1601</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="AI22:AJ22"/>
+  <mergeCells count="18">
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="AM4:AN4"/>
     <mergeCell ref="U4:V4"/>
+    <mergeCell ref="I6:I21"/>
+    <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK22:AL22"/>
+    <mergeCell ref="W4:X4"/>
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="I6:I21"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="S4:T4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="AK4:AL4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1496,21 +1530,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E3" s="40"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -1533,103 +1567,103 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1645,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
   <dimension ref="B4:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,14 +1693,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">

</xml_diff>

<commit_message>
Add some game object to make report Milestone-01 faster.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB30EF-59D4-47F4-85BA-3A62CE66A197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CE1711-79B6-4555-95EA-F2F2BC95F12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -536,6 +536,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -916,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,6 +935,7 @@
     <col min="25" max="25" width="17.5546875" customWidth="1"/>
     <col min="26" max="26" width="8.88671875" customWidth="1"/>
     <col min="33" max="33" width="15.88671875" customWidth="1"/>
+    <col min="35" max="35" width="10.44140625" customWidth="1"/>
     <col min="37" max="37" width="15.33203125" customWidth="1"/>
     <col min="41" max="41" width="11.88671875" customWidth="1"/>
     <col min="46" max="46" width="63.77734375" customWidth="1"/>
@@ -952,65 +956,65 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40" t="s">
+      <c r="L4" s="41"/>
+      <c r="M4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="40"/>
+      <c r="N4" s="41"/>
       <c r="R4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="31" t="s">
+      <c r="S4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31" t="s">
+      <c r="T4" s="32"/>
+      <c r="U4" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31" t="s">
+      <c r="V4" s="32"/>
+      <c r="W4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31" t="s">
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="32" t="s">
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="32" t="s">
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="32" t="s">
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="32" t="s">
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="32" t="s">
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="AJ4" s="33"/>
-      <c r="AK4" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN4" s="33"/>
-      <c r="AO4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP4" s="33"/>
+      <c r="AP4" s="34"/>
     </row>
     <row r="5" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
@@ -1039,10 +1043,10 @@
       <c r="T5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="46" t="s">
+      <c r="V5" s="47" t="s">
         <v>12</v>
       </c>
       <c r="W5" s="8" t="s">
@@ -1081,10 +1085,10 @@
       <c r="AH5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AI5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AK5" s="9" t="s">
@@ -1099,10 +1103,10 @@
       <c r="AN5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AO5" s="8" t="s">
+      <c r="AO5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AP5" s="8" t="s">
+      <c r="AP5" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1110,10 +1114,10 @@
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="37" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="6">
@@ -1164,20 +1168,20 @@
       <c r="AH6" s="15">
         <v>10500</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AI6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6">
+        <v>12000</v>
+      </c>
+      <c r="AK6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL6" s="40"/>
+      <c r="AO6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AJ6" s="11">
-        <v>11000</v>
-      </c>
-      <c r="AK6" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL6" s="39"/>
-      <c r="AO6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP6">
+      <c r="AP6" s="11">
         <v>11000</v>
       </c>
     </row>
@@ -1188,8 +1192,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="37"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="38"/>
       <c r="S7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1227,9 +1231,9 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="37"/>
-      <c r="S8" s="45" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="38"/>
+      <c r="S8" s="46" t="s">
         <v>56</v>
       </c>
       <c r="T8" s="6">
@@ -1249,9 +1253,9 @@
       </c>
     </row>
     <row r="9" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I9" s="35"/>
-      <c r="J9" s="37"/>
-      <c r="S9" s="45" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="38"/>
+      <c r="S9" s="46" t="s">
         <v>57</v>
       </c>
       <c r="T9" s="6">
@@ -1271,8 +1275,8 @@
       </c>
     </row>
     <row r="10" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I10" s="35"/>
-      <c r="S10" s="45" t="s">
+      <c r="I10" s="36"/>
+      <c r="S10" s="46" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="6">
@@ -1286,34 +1290,40 @@
       </c>
     </row>
     <row r="11" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I11" s="35"/>
+      <c r="I11" s="36"/>
       <c r="AK11" s="12" t="s">
         <v>23</v>
       </c>
       <c r="AL11" s="13">
         <v>600</v>
       </c>
+      <c r="AN11" s="22"/>
+      <c r="AO11" s="22"/>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I12" s="35"/>
+      <c r="I12" s="36"/>
       <c r="AK12" s="12" t="s">
         <v>24</v>
       </c>
       <c r="AL12" s="13">
         <v>601</v>
       </c>
+      <c r="AN12" s="25"/>
+      <c r="AO12" s="25"/>
     </row>
     <row r="13" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I13" s="35"/>
+      <c r="I13" s="36"/>
       <c r="AK13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="AL13" s="13">
         <v>700</v>
       </c>
+      <c r="AN13" s="20"/>
+      <c r="AO13" s="20"/>
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I14" s="35"/>
+      <c r="I14" s="36"/>
       <c r="AK14" s="12" t="s">
         <v>26</v>
       </c>
@@ -1322,7 +1332,7 @@
       </c>
     </row>
     <row r="15" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I15" s="35"/>
+      <c r="I15" s="36"/>
       <c r="AK15" s="12" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1341,7 @@
       </c>
     </row>
     <row r="16" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="I16" s="35"/>
+      <c r="I16" s="36"/>
       <c r="AK16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1340,7 +1350,7 @@
       </c>
     </row>
     <row r="17" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I17" s="35"/>
+      <c r="I17" s="36"/>
       <c r="AK17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1349,7 +1359,7 @@
       </c>
     </row>
     <row r="18" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I18" s="35"/>
+      <c r="I18" s="36"/>
       <c r="AK18" s="12" t="s">
         <v>30</v>
       </c>
@@ -1358,7 +1368,7 @@
       </c>
     </row>
     <row r="19" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I19" s="35"/>
+      <c r="I19" s="36"/>
       <c r="AK19" s="12" t="s">
         <v>31</v>
       </c>
@@ -1367,7 +1377,7 @@
       </c>
     </row>
     <row r="20" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I20" s="35"/>
+      <c r="I20" s="36"/>
       <c r="AK20" s="12" t="s">
         <v>32</v>
       </c>
@@ -1376,7 +1386,7 @@
       </c>
     </row>
     <row r="21" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I21" s="35"/>
+      <c r="I21" s="36"/>
       <c r="AK21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1385,10 +1395,10 @@
       </c>
     </row>
     <row r="22" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK22" s="29" t="s">
+      <c r="AK22" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AL22" s="30"/>
+      <c r="AL22" s="31"/>
     </row>
     <row r="23" spans="9:38" x14ac:dyDescent="0.3">
       <c r="AK23" s="12" t="s">
@@ -1530,21 +1540,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -1567,103 +1577,103 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+      <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1693,14 +1703,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">

</xml_diff>

<commit_message>
Mario now can jump through Invisible Platform (or One-Way Platform).
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CE1711-79B6-4555-95EA-F2F2BC95F12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F86C9B4-0D70-44CD-9023-DEA1A4F00E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>CDOP</t>
+  </si>
+  <si>
+    <t>Image Map</t>
   </si>
 </sst>
 </file>
@@ -917,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AP34"/>
+  <dimension ref="B4:AR34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,15 +940,15 @@
     <col min="33" max="33" width="15.88671875" customWidth="1"/>
     <col min="35" max="35" width="10.44140625" customWidth="1"/>
     <col min="37" max="37" width="15.33203125" customWidth="1"/>
-    <col min="41" max="41" width="11.88671875" customWidth="1"/>
-    <col min="46" max="46" width="63.77734375" customWidth="1"/>
-    <col min="47" max="47" width="47.33203125" customWidth="1"/>
-    <col min="48" max="48" width="26.44140625" customWidth="1"/>
-    <col min="49" max="49" width="56.44140625" customWidth="1"/>
-    <col min="50" max="50" width="14.44140625" customWidth="1"/>
+    <col min="41" max="41" width="9.33203125" customWidth="1"/>
+    <col min="43" max="43" width="10.88671875" customWidth="1"/>
+    <col min="46" max="46" width="8" customWidth="1"/>
+    <col min="47" max="47" width="5.6640625" customWidth="1"/>
+    <col min="48" max="49" width="7.77734375" customWidth="1"/>
+    <col min="50" max="50" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:44" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,8 +1018,12 @@
         <v>17</v>
       </c>
       <c r="AP4" s="34"/>
-    </row>
-    <row r="5" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AQ4" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR4" s="34"/>
+    </row>
+    <row r="5" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1109,8 +1116,14 @@
       <c r="AP5" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AQ5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -1184,8 +1197,14 @@
       <c r="AP6" s="11">
         <v>11000</v>
       </c>
-    </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="AQ6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR6" s="11">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1227,7 +1246,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:44" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I9" s="36"/>
       <c r="J9" s="38"/>
       <c r="S9" s="46" t="s">
@@ -1274,7 +1293,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I10" s="36"/>
       <c r="S10" s="46" t="s">
         <v>58</v>
@@ -1289,7 +1308,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I11" s="36"/>
       <c r="AK11" s="12" t="s">
         <v>23</v>
@@ -1300,7 +1319,7 @@
       <c r="AN11" s="22"/>
       <c r="AO11" s="22"/>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I12" s="36"/>
       <c r="AK12" s="12" t="s">
         <v>24</v>
@@ -1311,7 +1330,7 @@
       <c r="AN12" s="25"/>
       <c r="AO12" s="25"/>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I13" s="36"/>
       <c r="AK13" s="12" t="s">
         <v>25</v>
@@ -1322,7 +1341,7 @@
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I14" s="36"/>
       <c r="AK14" s="12" t="s">
         <v>26</v>
@@ -1331,7 +1350,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I15" s="36"/>
       <c r="AK15" s="12" t="s">
         <v>27</v>
@@ -1340,7 +1359,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:44" x14ac:dyDescent="0.3">
       <c r="I16" s="36"/>
       <c r="AK16" s="12" t="s">
         <v>28</v>
@@ -1497,7 +1516,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>

</xml_diff>

<commit_message>
Create class Pipe with basic feature like render, but this feature is enough for Milestone-01's requirements.
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F86C9B4-0D70-44CD-9023-DEA1A4F00E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3263FB6F-30B8-4A61-87E3-54F07CE87C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>Image Map</t>
+  </si>
+  <si>
+    <t>current_frame == -1</t>
+  </si>
+  <si>
+    <t>Tên file asset của object không có trong file scene, hoặc tên file asset bị viết sai chính tả</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -544,6 +550,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -605,6 +614,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AR34"/>
+  <dimension ref="B4:AT34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV13" sqref="AV13"/>
+    <sheetView topLeftCell="AG1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,13 +954,14 @@
     <col min="37" max="37" width="15.33203125" customWidth="1"/>
     <col min="41" max="41" width="9.33203125" customWidth="1"/>
     <col min="43" max="43" width="10.88671875" customWidth="1"/>
-    <col min="46" max="46" width="8" customWidth="1"/>
+    <col min="45" max="45" width="9.77734375" customWidth="1"/>
+    <col min="46" max="46" width="8.44140625" customWidth="1"/>
     <col min="47" max="47" width="5.6640625" customWidth="1"/>
     <col min="48" max="49" width="7.77734375" customWidth="1"/>
     <col min="50" max="50" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:46" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,71 +972,75 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41" t="s">
+      <c r="L4" s="42"/>
+      <c r="M4" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="41"/>
+      <c r="N4" s="42"/>
       <c r="R4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="32" t="s">
+      <c r="S4" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32" t="s">
+      <c r="T4" s="33"/>
+      <c r="U4" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32" t="s">
+      <c r="V4" s="33"/>
+      <c r="W4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32" t="s">
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="33" t="s">
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="33" t="s">
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="33" t="s">
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="33" t="s">
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="33" t="s">
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="33" t="s">
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="33" t="s">
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="33" t="s">
+      <c r="AP4" s="35"/>
+      <c r="AQ4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="34"/>
-    </row>
-    <row r="5" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AR4" s="35"/>
+      <c r="AS4" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT4" s="35"/>
+    </row>
+    <row r="5" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1050,10 +1067,10 @@
       <c r="T5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="45" t="s">
+      <c r="U5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="47" t="s">
+      <c r="V5" s="48" t="s">
         <v>12</v>
       </c>
       <c r="W5" s="8" t="s">
@@ -1122,15 +1139,21 @@
       <c r="AR5" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AS5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="38" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="6">
@@ -1187,10 +1210,10 @@
       <c r="AJ6">
         <v>12000</v>
       </c>
-      <c r="AK6" s="39" t="s">
+      <c r="AK6" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="AL6" s="40"/>
+      <c r="AL6" s="41"/>
       <c r="AO6" s="11" t="s">
         <v>17</v>
       </c>
@@ -1203,16 +1226,22 @@
       <c r="AR6" s="11">
         <v>13000</v>
       </c>
-    </row>
-    <row r="7" spans="2:44" x14ac:dyDescent="0.3">
+      <c r="AS6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="11">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:46" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="39"/>
       <c r="S7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1246,13 +1275,13 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:46" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="38"/>
-      <c r="S8" s="46" t="s">
+      <c r="I8" s="37"/>
+      <c r="J8" s="39"/>
+      <c r="S8" s="47" t="s">
         <v>56</v>
       </c>
       <c r="T8" s="6">
@@ -1271,10 +1300,10 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I9" s="36"/>
-      <c r="J9" s="38"/>
-      <c r="S9" s="46" t="s">
+    <row r="9" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I9" s="37"/>
+      <c r="J9" s="39"/>
+      <c r="S9" s="47" t="s">
         <v>57</v>
       </c>
       <c r="T9" s="6">
@@ -1293,9 +1322,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I10" s="36"/>
-      <c r="S10" s="46" t="s">
+    <row r="10" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I10" s="37"/>
+      <c r="S10" s="47" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="6">
@@ -1308,8 +1337,8 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I11" s="36"/>
+    <row r="11" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I11" s="37"/>
       <c r="AK11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1319,8 +1348,8 @@
       <c r="AN11" s="22"/>
       <c r="AO11" s="22"/>
     </row>
-    <row r="12" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I12" s="36"/>
+    <row r="12" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I12" s="37"/>
       <c r="AK12" s="12" t="s">
         <v>24</v>
       </c>
@@ -1330,8 +1359,8 @@
       <c r="AN12" s="25"/>
       <c r="AO12" s="25"/>
     </row>
-    <row r="13" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I13" s="36"/>
+    <row r="13" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I13" s="37"/>
       <c r="AK13" s="12" t="s">
         <v>25</v>
       </c>
@@ -1341,8 +1370,8 @@
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
     </row>
-    <row r="14" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I14" s="36"/>
+    <row r="14" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I14" s="37"/>
       <c r="AK14" s="12" t="s">
         <v>26</v>
       </c>
@@ -1350,8 +1379,8 @@
         <v>701</v>
       </c>
     </row>
-    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I15" s="36"/>
+    <row r="15" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I15" s="37"/>
       <c r="AK15" s="12" t="s">
         <v>27</v>
       </c>
@@ -1359,8 +1388,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="I16" s="36"/>
+    <row r="16" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="I16" s="37"/>
       <c r="AK16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1369,7 +1398,7 @@
       </c>
     </row>
     <row r="17" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I17" s="36"/>
+      <c r="I17" s="37"/>
       <c r="AK17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1378,7 +1407,7 @@
       </c>
     </row>
     <row r="18" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I18" s="36"/>
+      <c r="I18" s="37"/>
       <c r="AK18" s="12" t="s">
         <v>30</v>
       </c>
@@ -1387,7 +1416,7 @@
       </c>
     </row>
     <row r="19" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I19" s="36"/>
+      <c r="I19" s="37"/>
       <c r="AK19" s="12" t="s">
         <v>31</v>
       </c>
@@ -1396,7 +1425,7 @@
       </c>
     </row>
     <row r="20" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I20" s="36"/>
+      <c r="I20" s="37"/>
       <c r="AK20" s="12" t="s">
         <v>32</v>
       </c>
@@ -1405,7 +1434,7 @@
       </c>
     </row>
     <row r="21" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="AK21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1414,10 +1443,10 @@
       </c>
     </row>
     <row r="22" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK22" s="30" t="s">
+      <c r="AK22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AL22" s="31"/>
+      <c r="AL22" s="32"/>
     </row>
     <row r="23" spans="9:38" x14ac:dyDescent="0.3">
       <c r="AK23" s="12" t="s">
@@ -1516,8 +1545,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:AT4"/>
     <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
@@ -1547,7 +1577,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1560,21 +1590,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E3" s="27"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -1597,103 +1627,103 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
+      <c r="A5" s="30">
         <v>1</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1707,48 +1737,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
-  <dimension ref="B4:G6"/>
+  <dimension ref="A4:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="44" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="49" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove sample codes and other codes
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3263FB6F-30B8-4A61-87E3-54F07CE87C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7167DD3-9C9F-44DA-AD30-CD3F35E8A629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -261,6 +261,33 @@
   </si>
   <si>
     <t>Tên file asset của object không có trong file scene, hoặc tên file asset bị viết sai chính tả</t>
+  </si>
+  <si>
+    <t>Mario nhỏ không consume được Mushroom</t>
+  </si>
+  <si>
+    <t>Khi Mushroom rớt xuống đầu Mario nhỏ</t>
+  </si>
+  <si>
+    <t>Mario lớn bị rớt khỏi platform khi consume Mushroom</t>
+  </si>
+  <si>
+    <t>Khi Mushroom rớt xuống đầu Mario lớn</t>
+  </si>
+  <si>
+    <t>Còn bug</t>
+  </si>
+  <si>
+    <t>Tần suất xảy ra</t>
+  </si>
+  <si>
+    <t>Rất ít xảy ra, chỉ mới ghi nhận lần đầu tiên khi Demo cho mấy đứa bạn</t>
+  </si>
+  <si>
+    <t>Khá thường xuyên xảy ra</t>
+  </si>
+  <si>
+    <t>Luôn luôn xảy ra khi có va chạm với blocking object và chưa bay</t>
   </si>
 </sst>
 </file>
@@ -511,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -559,9 +586,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,73 +996,73 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42" t="s">
+      <c r="L4" s="41"/>
+      <c r="M4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="41"/>
       <c r="R4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="33" t="s">
+      <c r="S4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33" t="s">
+      <c r="T4" s="32"/>
+      <c r="U4" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33" t="s">
+      <c r="V4" s="32"/>
+      <c r="W4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33" t="s">
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="34" t="s">
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="34" t="s">
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="34" t="s">
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="34" t="s">
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="34" t="s">
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="35"/>
-      <c r="AM4" s="34" t="s">
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="AN4" s="35"/>
-      <c r="AO4" s="34" t="s">
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="AP4" s="35"/>
-      <c r="AQ4" s="34" t="s">
+      <c r="AP4" s="34"/>
+      <c r="AQ4" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="35"/>
-      <c r="AS4" s="34" t="s">
+      <c r="AR4" s="34"/>
+      <c r="AS4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="AT4" s="35"/>
+      <c r="AT4" s="34"/>
     </row>
     <row r="5" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
@@ -1067,10 +1091,10 @@
       <c r="T5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="48" t="s">
+      <c r="V5" s="47" t="s">
         <v>12</v>
       </c>
       <c r="W5" s="8" t="s">
@@ -1150,10 +1174,10 @@
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="6">
@@ -1210,10 +1234,10 @@
       <c r="AJ6">
         <v>12000</v>
       </c>
-      <c r="AK6" s="40" t="s">
+      <c r="AK6" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AL6" s="41"/>
+      <c r="AL6" s="40"/>
       <c r="AO6" s="11" t="s">
         <v>17</v>
       </c>
@@ -1240,8 +1264,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="39"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="38"/>
       <c r="S7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1279,9 +1303,9 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="39"/>
-      <c r="S8" s="47" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="38"/>
+      <c r="S8" s="46" t="s">
         <v>56</v>
       </c>
       <c r="T8" s="6">
@@ -1301,9 +1325,9 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I9" s="37"/>
-      <c r="J9" s="39"/>
-      <c r="S9" s="47" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="38"/>
+      <c r="S9" s="46" t="s">
         <v>57</v>
       </c>
       <c r="T9" s="6">
@@ -1323,8 +1347,8 @@
       </c>
     </row>
     <row r="10" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I10" s="37"/>
-      <c r="S10" s="47" t="s">
+      <c r="I10" s="36"/>
+      <c r="S10" s="46" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="6">
@@ -1338,7 +1362,7 @@
       </c>
     </row>
     <row r="11" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I11" s="37"/>
+      <c r="I11" s="36"/>
       <c r="AK11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1349,7 +1373,7 @@
       <c r="AO11" s="22"/>
     </row>
     <row r="12" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I12" s="37"/>
+      <c r="I12" s="36"/>
       <c r="AK12" s="12" t="s">
         <v>24</v>
       </c>
@@ -1360,7 +1384,7 @@
       <c r="AO12" s="25"/>
     </row>
     <row r="13" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I13" s="37"/>
+      <c r="I13" s="36"/>
       <c r="AK13" s="12" t="s">
         <v>25</v>
       </c>
@@ -1371,7 +1395,7 @@
       <c r="AO13" s="20"/>
     </row>
     <row r="14" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I14" s="37"/>
+      <c r="I14" s="36"/>
       <c r="AK14" s="12" t="s">
         <v>26</v>
       </c>
@@ -1380,7 +1404,7 @@
       </c>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I15" s="37"/>
+      <c r="I15" s="36"/>
       <c r="AK15" s="12" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1413,7 @@
       </c>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I16" s="37"/>
+      <c r="I16" s="36"/>
       <c r="AK16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1398,7 +1422,7 @@
       </c>
     </row>
     <row r="17" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I17" s="37"/>
+      <c r="I17" s="36"/>
       <c r="AK17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1407,7 +1431,7 @@
       </c>
     </row>
     <row r="18" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I18" s="37"/>
+      <c r="I18" s="36"/>
       <c r="AK18" s="12" t="s">
         <v>30</v>
       </c>
@@ -1416,7 +1440,7 @@
       </c>
     </row>
     <row r="19" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I19" s="37"/>
+      <c r="I19" s="36"/>
       <c r="AK19" s="12" t="s">
         <v>31</v>
       </c>
@@ -1425,7 +1449,7 @@
       </c>
     </row>
     <row r="20" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I20" s="37"/>
+      <c r="I20" s="36"/>
       <c r="AK20" s="12" t="s">
         <v>32</v>
       </c>
@@ -1434,7 +1458,7 @@
       </c>
     </row>
     <row r="21" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I21" s="37"/>
+      <c r="I21" s="36"/>
       <c r="AK21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1443,10 +1467,10 @@
       </c>
     </row>
     <row r="22" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK22" s="31" t="s">
+      <c r="AK22" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AL22" s="32"/>
+      <c r="AL22" s="31"/>
     </row>
     <row r="23" spans="9:38" x14ac:dyDescent="0.3">
       <c r="AK23" s="12" t="s">
@@ -1574,39 +1598,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="3" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>66</v>
       </c>
@@ -1616,119 +1642,172 @@
       <c r="C4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+    <row r="5" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="48" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1739,7 +1818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
   <dimension ref="A4:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1753,14 +1832,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -1781,10 +1860,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1793,10 +1872,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="48" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Mario Raccom with basic feature: draw idle sprites
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7167DD3-9C9F-44DA-AD30-CD3F35E8A629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F0ED75-76FA-4343-AC1F-949512C8C65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -288,6 +288,27 @@
   </si>
   <si>
     <t>Luôn luôn xảy ra khi có va chạm với blocking object và chưa bay</t>
+  </si>
+  <si>
+    <t>Mario Raccon</t>
+  </si>
+  <si>
+    <t>Sprite ID</t>
+  </si>
+  <si>
+    <t>Game object</t>
+  </si>
+  <si>
+    <t>Số lượng sprite</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Ani ID</t>
+  </si>
+  <si>
+    <t>Hoặc return nhầm ani_id (xem mục Debug Out để biết được ani_id return nhầm là gì</t>
   </si>
 </sst>
 </file>
@@ -333,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -342,50 +363,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -474,6 +451,70 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -483,101 +524,54 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -587,40 +581,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -632,16 +633,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,36 +972,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:AT34"/>
+  <dimension ref="B4:BF37"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView topLeftCell="AG1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AU12" sqref="AU12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.07421875" customWidth="1"/>
     <col min="6" max="8" width="16" customWidth="1"/>
-    <col min="12" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="18" max="22" width="12.77734375" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" customWidth="1"/>
-    <col min="25" max="25" width="17.5546875" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="33" max="33" width="15.88671875" customWidth="1"/>
-    <col min="35" max="35" width="10.44140625" customWidth="1"/>
-    <col min="37" max="37" width="15.33203125" customWidth="1"/>
-    <col min="41" max="41" width="9.33203125" customWidth="1"/>
-    <col min="43" max="43" width="10.88671875" customWidth="1"/>
-    <col min="45" max="45" width="9.77734375" customWidth="1"/>
-    <col min="46" max="46" width="8.44140625" customWidth="1"/>
-    <col min="47" max="47" width="5.6640625" customWidth="1"/>
-    <col min="48" max="49" width="7.77734375" customWidth="1"/>
-    <col min="50" max="50" width="7.33203125" customWidth="1"/>
+    <col min="12" max="13" width="11.69140625" customWidth="1"/>
+    <col min="14" max="14" width="12.69140625" customWidth="1"/>
+    <col min="18" max="22" width="12.765625" customWidth="1"/>
+    <col min="23" max="23" width="12.3046875" customWidth="1"/>
+    <col min="25" max="25" width="17.53515625" customWidth="1"/>
+    <col min="26" max="26" width="8.84375" customWidth="1"/>
+    <col min="33" max="33" width="15.84375" customWidth="1"/>
+    <col min="35" max="35" width="10.4609375" customWidth="1"/>
+    <col min="37" max="37" width="15.3046875" customWidth="1"/>
+    <col min="38" max="38" width="9.23046875" customWidth="1"/>
+    <col min="39" max="39" width="14.15234375" customWidth="1"/>
+    <col min="41" max="41" width="14.84375" customWidth="1"/>
+    <col min="45" max="45" width="9.3046875" customWidth="1"/>
+    <col min="47" max="47" width="10.84375" customWidth="1"/>
+    <col min="49" max="49" width="9.765625" customWidth="1"/>
+    <col min="50" max="50" width="8.4609375" customWidth="1"/>
+    <col min="51" max="51" width="5.69140625" customWidth="1"/>
+    <col min="52" max="53" width="7.765625" customWidth="1"/>
+    <col min="54" max="54" width="11.61328125" customWidth="1"/>
+    <col min="55" max="56" width="13.4609375" customWidth="1"/>
+    <col min="57" max="57" width="13.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:58" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,8 +1015,8 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="41" t="s">
         <v>40</v>
       </c>
@@ -1004,228 +1025,256 @@
         <v>41</v>
       </c>
       <c r="N4" s="41"/>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="32" t="s">
+      <c r="S4" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32" t="s">
+      <c r="T4" s="34"/>
+      <c r="U4" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32" t="s">
+      <c r="V4" s="34"/>
+      <c r="W4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32" t="s">
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="33" t="s">
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="33" t="s">
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="33" t="s">
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="33" t="s">
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="33" t="s">
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="33" t="s">
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="45"/>
+      <c r="AN4" s="45"/>
+      <c r="AO4" s="45"/>
+      <c r="AP4" s="36"/>
+      <c r="AQ4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="33" t="s">
+      <c r="AR4" s="36"/>
+      <c r="AS4" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="33" t="s">
+      <c r="AT4" s="36"/>
+      <c r="AU4" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="34"/>
-      <c r="AS4" s="33" t="s">
+      <c r="AV4" s="36"/>
+      <c r="AW4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="AT4" s="34"/>
-    </row>
-    <row r="5" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX4" s="36"/>
+      <c r="BB4" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC4" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="BD4" s="43"/>
+      <c r="BE4" s="43"/>
+      <c r="BF4" s="43"/>
+    </row>
+    <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="8" t="s">
+      <c r="I5" s="19"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="R5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="45" t="s">
+      <c r="U5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="47" t="s">
+      <c r="V5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Y5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Z5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AA5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="8" t="s">
+      <c r="AB5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AC5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AD5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AE5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AF5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AG5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AH5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="8" t="s">
+      <c r="AI5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AJ5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AK5" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN5" s="53"/>
+      <c r="AO5" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP5" s="33"/>
+      <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AR5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="8" t="s">
+      <c r="AS5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AN5" s="8" t="s">
+      <c r="AT5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AO5" s="9" t="s">
+      <c r="AU5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AP5" s="9" t="s">
+      <c r="AV5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AQ5" s="9" t="s">
+      <c r="AW5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AR5" s="9" t="s">
+      <c r="AX5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AT5" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB5" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC5" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD5" s="43"/>
+      <c r="BE5" s="43"/>
+      <c r="BF5" s="43"/>
+    </row>
+    <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="4">
         <v>6000</v>
       </c>
-      <c r="U6" s="20" t="s">
+      <c r="U6" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="V6" s="20">
+      <c r="V6" s="17">
         <v>7000</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="4">
         <v>5000</v>
       </c>
-      <c r="Y6" s="18" t="s">
+      <c r="Y6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="19">
+      <c r="Z6" s="16">
         <v>5500</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AE6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6" s="9">
         <v>10000</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AG6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AH6" s="15">
+      <c r="AH6" s="12">
         <v>10500</v>
       </c>
       <c r="AI6" t="s">
@@ -1234,358 +1283,581 @@
       <c r="AJ6">
         <v>12000</v>
       </c>
-      <c r="AK6" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL6" s="40"/>
-      <c r="AO6" s="11" t="s">
+      <c r="AK6" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL6" s="51">
+        <v>400</v>
+      </c>
+      <c r="AM6" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN6" s="51">
+        <v>1100</v>
+      </c>
+      <c r="AO6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP6" s="20">
+        <v>1700</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AP6" s="11">
+      <c r="AT6" s="9">
         <v>11000</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="AU6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AR6" s="11">
+      <c r="AV6" s="9">
         <v>13000</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="AW6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AT6" s="11">
+      <c r="AX6" s="9">
         <v>14000</v>
       </c>
-    </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="BC6" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD6" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="BE6" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="BF6" s="31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:58" x14ac:dyDescent="0.4">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="38"/>
-      <c r="S7" s="6" t="s">
+      <c r="I7" s="38"/>
+      <c r="J7" s="40"/>
+      <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="4">
         <v>6001</v>
       </c>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="6" t="s">
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7" s="4">
         <v>5001</v>
       </c>
-      <c r="Y7" s="20" t="s">
+      <c r="Y7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="20">
+      <c r="Z7" s="17">
         <v>5510</v>
       </c>
-      <c r="AG7" s="16" t="s">
+      <c r="AG7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AH7" s="17">
+      <c r="AH7" s="14">
         <v>10600</v>
       </c>
-      <c r="AK7" s="12" t="s">
+      <c r="AK7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL7" s="51">
+        <v>401</v>
+      </c>
+      <c r="AM7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN7" s="51">
+        <v>1102</v>
+      </c>
+      <c r="AO7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP7" s="20">
+        <v>1701</v>
+      </c>
+      <c r="BC7" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="AL7" s="13">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="BD7" s="51">
+        <v>1100</v>
+      </c>
+      <c r="BE7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:58" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="38"/>
-      <c r="S8" s="46" t="s">
+      <c r="I8" s="38"/>
+      <c r="J8" s="40"/>
+      <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="4">
         <v>6002</v>
       </c>
-      <c r="Y8" s="23" t="s">
+      <c r="Y8" s="20" t="s">
         <v>50</v>
       </c>
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AK8" s="12" t="s">
+      <c r="AK8" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL8" s="51">
+        <v>500</v>
+      </c>
+      <c r="AM8" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN8" s="51">
+        <v>1200</v>
+      </c>
+      <c r="AO8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP8">
+        <v>1800</v>
+      </c>
+      <c r="BC8" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="AL8" s="13">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I9" s="36"/>
-      <c r="J9" s="38"/>
-      <c r="S9" s="46" t="s">
+      <c r="BD8" s="51">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I9" s="38"/>
+      <c r="J9" s="40"/>
+      <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="4">
         <v>6003</v>
       </c>
-      <c r="Y9" s="23" t="s">
+      <c r="Y9" s="20" t="s">
         <v>14</v>
       </c>
       <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AK9" s="12" t="s">
+      <c r="AK9" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL9" s="51">
+        <v>501</v>
+      </c>
+      <c r="AM9" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN9" s="51">
+        <v>1201</v>
+      </c>
+      <c r="AO9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP9">
+        <v>1801</v>
+      </c>
+      <c r="BC9" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AL9" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I10" s="36"/>
-      <c r="S10" s="46" t="s">
+      <c r="BD9" s="51">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I10" s="38"/>
+      <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="4">
         <v>6004</v>
       </c>
-      <c r="AK10" s="12" t="s">
+      <c r="AK10" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL10" s="51">
+        <v>600</v>
+      </c>
+      <c r="AM10" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN10" s="51">
+        <v>1300</v>
+      </c>
+      <c r="AO10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC10" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="AL10" s="13">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="11" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I11" s="36"/>
-      <c r="AK11" s="12" t="s">
+      <c r="BD10" s="51">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="11" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I11" s="38"/>
+      <c r="AK11" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL11" s="51">
+        <v>601</v>
+      </c>
+      <c r="AM11" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN11" s="51">
+        <v>1301</v>
+      </c>
+      <c r="AO11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR11" s="19"/>
+      <c r="AS11" s="19"/>
+      <c r="BC11" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AL11" s="13">
-        <v>600</v>
-      </c>
-      <c r="AN11" s="22"/>
-      <c r="AO11" s="22"/>
-    </row>
-    <row r="12" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I12" s="36"/>
-      <c r="AK12" s="12" t="s">
+      <c r="BD11" s="51">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="12" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I12" s="38"/>
+      <c r="AK12" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL12" s="51">
+        <v>700</v>
+      </c>
+      <c r="AM12" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN12" s="51">
+        <v>1400</v>
+      </c>
+      <c r="AO12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR12" s="22"/>
+      <c r="AS12" s="22"/>
+      <c r="BC12" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="AL12" s="13">
-        <v>601</v>
-      </c>
-      <c r="AN12" s="25"/>
-      <c r="AO12" s="25"/>
-    </row>
-    <row r="13" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I13" s="36"/>
-      <c r="AK13" s="12" t="s">
+      <c r="BD12" s="51">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="13" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I13" s="38"/>
+      <c r="AK13" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL13" s="51">
+        <v>701</v>
+      </c>
+      <c r="AM13" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN13" s="51">
+        <v>1401</v>
+      </c>
+      <c r="AO13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR13" s="17"/>
+      <c r="AS13" s="17"/>
+      <c r="BC13" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD13" s="51">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I14" s="38"/>
+      <c r="AK14" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL14" s="51">
+        <v>800</v>
+      </c>
+      <c r="AM14" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="AL13" s="13">
-        <v>700</v>
-      </c>
-      <c r="AN13" s="20"/>
-      <c r="AO13" s="20"/>
-    </row>
-    <row r="14" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I14" s="36"/>
-      <c r="AK14" s="12" t="s">
+      <c r="AN14" s="51">
+        <v>1500</v>
+      </c>
+      <c r="AO14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="BC14" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD14" s="51">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="15" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I15" s="38"/>
+      <c r="AK15" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL15" s="51">
+        <v>801</v>
+      </c>
+      <c r="AM15" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AL14" s="13">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="15" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I15" s="36"/>
-      <c r="AK15" s="12" t="s">
+      <c r="AN15" s="51">
+        <v>1501</v>
+      </c>
+      <c r="AO15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC15" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD15" s="51">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="2:58" x14ac:dyDescent="0.4">
+      <c r="I16" s="38"/>
+      <c r="AK16" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL16" s="51">
+        <v>900</v>
+      </c>
+      <c r="AM16" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AL15" s="13">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="16" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="I16" s="36"/>
-      <c r="AK16" s="12" t="s">
+      <c r="AN16" s="51">
+        <v>1600</v>
+      </c>
+      <c r="AO16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC16" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD16" s="51">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="17" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="I17" s="38"/>
+      <c r="AG17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK17" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL17" s="51">
+        <v>901</v>
+      </c>
+      <c r="AM17" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AL16" s="13">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="17" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I17" s="36"/>
-      <c r="AK17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL17" s="13">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="18" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I18" s="36"/>
-      <c r="AK18" s="12" t="s">
+      <c r="AN17" s="51">
+        <v>1601</v>
+      </c>
+      <c r="AO17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AL18" s="13">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="19" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I19" s="36"/>
-      <c r="AK19" s="12" t="s">
+      <c r="BC17" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="BD17" s="51">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="18" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="I18" s="38"/>
+      <c r="AK18" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="AL19" s="13">
+      <c r="AL18" s="51">
         <v>1000</v>
       </c>
-    </row>
-    <row r="20" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I20" s="36"/>
-      <c r="AK20" s="12" t="s">
+      <c r="AM18" s="13"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="BC18" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="BD18" s="51">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="19" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="I19" s="38"/>
+      <c r="AK19" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="AL20" s="13">
+      <c r="AL19" s="51">
         <v>1001</v>
       </c>
-    </row>
-    <row r="21" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="I21" s="36"/>
-      <c r="AK21" s="12" t="s">
+      <c r="AM19" s="17"/>
+      <c r="AN19" s="17"/>
+      <c r="AO19" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="I20" s="38"/>
+      <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AL21" s="13">
+      <c r="AL20" s="14">
         <v>999</v>
       </c>
-    </row>
-    <row r="22" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL22" s="31"/>
-    </row>
-    <row r="23" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL23" s="13">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="24" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL24" s="13">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="25" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL25" s="13">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="26" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK26" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL26" s="13">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="27" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL27" s="13">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="28" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL28" s="13">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="29" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL29" s="13">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="30" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK30" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL30" s="13">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="31" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL31" s="13">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="32" spans="9:38" x14ac:dyDescent="0.3">
-      <c r="AK32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL32" s="13">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="33" spans="37:38" x14ac:dyDescent="0.3">
-      <c r="AK33" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL33" s="13">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="34" spans="37:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AK34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL34" s="5">
-        <v>1601</v>
-      </c>
+      <c r="AM20" s="17"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+    </row>
+    <row r="21" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="I21" s="38"/>
+      <c r="AM21" s="17"/>
+      <c r="AN21" s="17"/>
+      <c r="AO21" s="17"/>
+      <c r="AP21" s="17"/>
+    </row>
+    <row r="22" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM22" s="46"/>
+      <c r="AN22" s="46"/>
+      <c r="AO22" s="46"/>
+      <c r="AP22" s="46"/>
+    </row>
+    <row r="23" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM23" s="17"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="17"/>
+      <c r="AP23" s="17"/>
+    </row>
+    <row r="24" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM24" s="17"/>
+      <c r="AN24" s="17"/>
+      <c r="AO24" s="17"/>
+      <c r="AP24" s="17"/>
+    </row>
+    <row r="25" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM25" s="17"/>
+      <c r="AN25" s="17"/>
+      <c r="AO25" s="17"/>
+      <c r="AP25" s="17"/>
+    </row>
+    <row r="26" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM26" s="17"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="17"/>
+      <c r="AP26" s="17"/>
+    </row>
+    <row r="27" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM27" s="17"/>
+      <c r="AN27" s="17"/>
+      <c r="AO27" s="17"/>
+      <c r="AP27" s="17"/>
+    </row>
+    <row r="28" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+    </row>
+    <row r="29" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM29" s="17"/>
+      <c r="AN29" s="17"/>
+      <c r="AO29" s="17"/>
+      <c r="AP29" s="17"/>
+    </row>
+    <row r="30" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM30" s="17"/>
+      <c r="AN30" s="17"/>
+      <c r="AO30" s="17"/>
+      <c r="AP30" s="17"/>
+    </row>
+    <row r="31" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM31" s="17"/>
+      <c r="AN31" s="17"/>
+      <c r="AO31" s="17"/>
+      <c r="AP31" s="17"/>
+    </row>
+    <row r="32" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AM32" s="17"/>
+      <c r="AN32" s="17"/>
+      <c r="AO32" s="17"/>
+      <c r="AP32" s="17"/>
+    </row>
+    <row r="33" spans="39:42" x14ac:dyDescent="0.4">
+      <c r="AM33" s="17"/>
+      <c r="AN33" s="17"/>
+      <c r="AO33" s="17"/>
+      <c r="AP33" s="17"/>
+    </row>
+    <row r="34" spans="39:42" x14ac:dyDescent="0.4">
+      <c r="AM34" s="17"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="17"/>
+      <c r="AP34" s="17"/>
+    </row>
+    <row r="35" spans="39:42" x14ac:dyDescent="0.4">
+      <c r="AM35" s="32"/>
+      <c r="AN35" s="32"/>
+      <c r="AO35" s="32"/>
+      <c r="AP35" s="32"/>
+    </row>
+    <row r="36" spans="39:42" x14ac:dyDescent="0.4">
+      <c r="AM36" s="20"/>
+      <c r="AN36" s="20"/>
+      <c r="AO36" s="20"/>
+      <c r="AP36" s="20"/>
+    </row>
+    <row r="37" spans="39:42" x14ac:dyDescent="0.4">
+      <c r="AM37" s="20"/>
+      <c r="AN37" s="20"/>
+      <c r="AO37" s="20"/>
+      <c r="AP37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="AQ4:AR4"/>
+  <mergeCells count="22">
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AK4:AP4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK6:AL6"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK22:AL22"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
@@ -1600,20 +1872,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.23046875" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
+    <col min="7" max="7" width="16.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B1" s="43" t="s">
         <v>68</v>
       </c>
@@ -1621,7 +1893,7 @@
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" s="42" t="s">
         <v>67</v>
       </c>
@@ -1629,180 +1901,180 @@
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+    <row r="5" spans="1:7" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1816,22 +2088,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
-  <dimension ref="A4:G7"/>
+  <dimension ref="A4:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="23.69140625" customWidth="1"/>
+    <col min="4" max="4" width="56.23046875" customWidth="1"/>
+    <col min="5" max="5" width="12.23046875" customWidth="1"/>
+    <col min="6" max="6" width="15.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B4" s="44" t="s">
         <v>69</v>
       </c>
@@ -1841,42 +2113,47 @@
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="48" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="30" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="D8" s="24" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix blurry sprites of Raccon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F0ED75-76FA-4343-AC1F-949512C8C65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6C9192-D462-4EF3-8135-32F25F92E74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2091,7 +2091,7 @@
   <dimension ref="A4:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add Brace animations for Raccon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6C9192-D462-4EF3-8135-32F25F92E74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC2FD9-B50F-4A7B-B05C-12BAA7ECB980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="754" yWindow="754" windowWidth="24686" windowHeight="13337" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,67 +597,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BF37"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AU12" sqref="AU12"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1017,86 +1017,86 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41" t="s">
+      <c r="L4" s="43"/>
+      <c r="M4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="41"/>
+      <c r="N4" s="43"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="34" t="s">
+      <c r="S4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34" t="s">
+      <c r="T4" s="44"/>
+      <c r="U4" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34" t="s">
+      <c r="V4" s="44"/>
+      <c r="W4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34" t="s">
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="35" t="s">
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="35" t="s">
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="35" t="s">
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="35" t="s">
+      <c r="AF4" s="42"/>
+      <c r="AG4" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="35" t="s">
+      <c r="AH4" s="42"/>
+      <c r="AI4" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="37"/>
-      <c r="AM4" s="45"/>
-      <c r="AN4" s="45"/>
-      <c r="AO4" s="45"/>
-      <c r="AP4" s="36"/>
-      <c r="AQ4" s="35" t="s">
+      <c r="AL4" s="46"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="36"/>
-      <c r="AS4" s="35" t="s">
+      <c r="AR4" s="42"/>
+      <c r="AS4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="AT4" s="36"/>
-      <c r="AU4" s="35" t="s">
+      <c r="AT4" s="42"/>
+      <c r="AU4" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="AV4" s="36"/>
-      <c r="AW4" s="35" t="s">
+      <c r="AV4" s="42"/>
+      <c r="AW4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="36"/>
-      <c r="BB4" s="54" t="s">
+      <c r="AX4" s="42"/>
+      <c r="BB4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="43" t="s">
+      <c r="BC4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="43"/>
-      <c r="BE4" s="43"/>
-      <c r="BF4" s="43"/>
+      <c r="BD4" s="40"/>
+      <c r="BE4" s="40"/>
+      <c r="BF4" s="40"/>
     </row>
     <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1173,18 +1173,18 @@
       <c r="AJ5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="48" t="s">
+      <c r="AK5" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="AL5" s="49"/>
+      <c r="AL5" s="35"/>
       <c r="AM5" s="52" t="s">
         <v>34</v>
       </c>
       <c r="AN5" s="53"/>
-      <c r="AO5" s="33" t="s">
+      <c r="AO5" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="33"/>
+      <c r="AP5" s="51"/>
       <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1209,24 +1209,24 @@
       <c r="AX5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BB5" s="54" t="s">
+      <c r="BB5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="43" t="s">
+      <c r="BC5" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="43"/>
-      <c r="BE5" s="43"/>
-      <c r="BF5" s="43"/>
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="40"/>
+      <c r="BF5" s="40"/>
     </row>
     <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="49" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1283,16 +1283,16 @@
       <c r="AJ6">
         <v>12000</v>
       </c>
-      <c r="AK6" s="50" t="s">
+      <c r="AK6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AL6" s="51">
+      <c r="AL6" s="37">
         <v>400</v>
       </c>
-      <c r="AM6" s="50" t="s">
+      <c r="AM6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="51">
+      <c r="AN6" s="37">
         <v>1100</v>
       </c>
       <c r="AO6" s="17" t="s">
@@ -1319,10 +1319,10 @@
       <c r="AX6" s="9">
         <v>14000</v>
       </c>
-      <c r="BC6" s="55" t="s">
+      <c r="BC6" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="BD6" s="55" t="s">
+      <c r="BD6" s="39" t="s">
         <v>89</v>
       </c>
       <c r="BE6" s="31" t="s">
@@ -1339,8 +1339,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="40"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="50"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1367,16 +1367,16 @@
       <c r="AH7" s="14">
         <v>10600</v>
       </c>
-      <c r="AK7" s="50" t="s">
+      <c r="AK7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="AL7" s="51">
+      <c r="AL7" s="37">
         <v>401</v>
       </c>
-      <c r="AM7" s="50" t="s">
+      <c r="AM7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="AN7" s="51">
+      <c r="AN7" s="37">
         <v>1102</v>
       </c>
       <c r="AO7" s="17" t="s">
@@ -1385,10 +1385,10 @@
       <c r="AP7" s="20">
         <v>1701</v>
       </c>
-      <c r="BC7" s="50" t="s">
+      <c r="BC7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="BD7" s="51">
+      <c r="BD7" s="37">
         <v>1100</v>
       </c>
       <c r="BE7">
@@ -1399,8 +1399,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="40"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="50"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1413,16 +1413,16 @@
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AK8" s="50" t="s">
+      <c r="AK8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AL8" s="51">
+      <c r="AL8" s="37">
         <v>500</v>
       </c>
-      <c r="AM8" s="50" t="s">
+      <c r="AM8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AN8" s="51">
+      <c r="AN8" s="37">
         <v>1200</v>
       </c>
       <c r="AO8" s="17" t="s">
@@ -1431,16 +1431,16 @@
       <c r="AP8">
         <v>1800</v>
       </c>
-      <c r="BC8" s="50" t="s">
+      <c r="BC8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="BD8" s="51">
+      <c r="BD8" s="37">
         <v>1102</v>
       </c>
     </row>
     <row r="9" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I9" s="38"/>
-      <c r="J9" s="40"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="50"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1453,16 +1453,16 @@
       <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AK9" s="50" t="s">
+      <c r="AK9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AL9" s="51">
+      <c r="AL9" s="37">
         <v>501</v>
       </c>
-      <c r="AM9" s="50" t="s">
+      <c r="AM9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AN9" s="51">
+      <c r="AN9" s="37">
         <v>1201</v>
       </c>
       <c r="AO9" s="17" t="s">
@@ -1471,229 +1471,253 @@
       <c r="AP9">
         <v>1801</v>
       </c>
-      <c r="BC9" s="50" t="s">
+      <c r="BC9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="BD9" s="51">
+      <c r="BD9" s="37">
         <v>1200</v>
       </c>
     </row>
     <row r="10" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I10" s="38"/>
+      <c r="I10" s="48"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="4">
         <v>6004</v>
       </c>
-      <c r="AK10" s="50" t="s">
+      <c r="AK10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AL10" s="51">
+      <c r="AL10" s="37">
         <v>600</v>
       </c>
-      <c r="AM10" s="50" t="s">
+      <c r="AM10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AN10" s="51">
+      <c r="AN10" s="37">
         <v>1300</v>
       </c>
       <c r="AO10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="BC10" s="50" t="s">
+      <c r="AP10">
+        <v>1900</v>
+      </c>
+      <c r="BC10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="BD10" s="51">
+      <c r="BD10" s="37">
         <v>1201</v>
       </c>
     </row>
     <row r="11" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I11" s="38"/>
-      <c r="AK11" s="50" t="s">
+      <c r="I11" s="48"/>
+      <c r="AK11" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AL11" s="51">
+      <c r="AL11" s="37">
         <v>601</v>
       </c>
-      <c r="AM11" s="50" t="s">
+      <c r="AM11" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AN11" s="51">
+      <c r="AN11" s="37">
         <v>1301</v>
       </c>
       <c r="AO11" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="AP11">
+        <v>1901</v>
+      </c>
       <c r="AR11" s="19"/>
       <c r="AS11" s="19"/>
-      <c r="BC11" s="50" t="s">
+      <c r="BC11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="BD11" s="51">
+      <c r="BD11" s="37">
         <v>1300</v>
       </c>
     </row>
     <row r="12" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I12" s="38"/>
-      <c r="AK12" s="50" t="s">
+      <c r="I12" s="48"/>
+      <c r="AK12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AL12" s="51">
+      <c r="AL12" s="37">
         <v>700</v>
       </c>
-      <c r="AM12" s="50" t="s">
+      <c r="AM12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AN12" s="51">
+      <c r="AN12" s="37">
         <v>1400</v>
       </c>
       <c r="AO12" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="AP12">
+        <v>2000</v>
+      </c>
       <c r="AR12" s="22"/>
       <c r="AS12" s="22"/>
-      <c r="BC12" s="50" t="s">
+      <c r="BC12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="BD12" s="51">
+      <c r="BD12" s="37">
         <v>1301</v>
       </c>
     </row>
     <row r="13" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I13" s="38"/>
-      <c r="AK13" s="50" t="s">
+      <c r="I13" s="48"/>
+      <c r="AK13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AL13" s="51">
+      <c r="AL13" s="37">
         <v>701</v>
       </c>
-      <c r="AM13" s="50" t="s">
+      <c r="AM13" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AN13" s="51">
+      <c r="AN13" s="37">
         <v>1401</v>
       </c>
       <c r="AO13" s="17" t="s">
         <v>26</v>
       </c>
+      <c r="AP13">
+        <v>2001</v>
+      </c>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
-      <c r="BC13" s="50" t="s">
+      <c r="BC13" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="BD13" s="51">
+      <c r="BD13" s="37">
         <v>1400</v>
       </c>
     </row>
     <row r="14" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I14" s="38"/>
-      <c r="AK14" s="50" t="s">
+      <c r="I14" s="48"/>
+      <c r="AK14" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AL14" s="51">
+      <c r="AL14" s="37">
         <v>800</v>
       </c>
-      <c r="AM14" s="50" t="s">
+      <c r="AM14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AN14" s="51">
+      <c r="AN14" s="37">
         <v>1500</v>
       </c>
       <c r="AO14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="BC14" s="50" t="s">
+      <c r="AP14">
+        <v>2100</v>
+      </c>
+      <c r="BC14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BD14" s="51">
+      <c r="BD14" s="37">
         <v>1401</v>
       </c>
     </row>
     <row r="15" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I15" s="38"/>
-      <c r="AK15" s="50" t="s">
+      <c r="I15" s="48"/>
+      <c r="AK15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AL15" s="51">
+      <c r="AL15" s="37">
         <v>801</v>
       </c>
-      <c r="AM15" s="50" t="s">
+      <c r="AM15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AN15" s="51">
+      <c r="AN15" s="37">
         <v>1501</v>
       </c>
       <c r="AO15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="BC15" s="50" t="s">
+      <c r="AP15">
+        <v>2101</v>
+      </c>
+      <c r="BC15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="BD15" s="51">
+      <c r="BD15" s="37">
         <v>1500</v>
       </c>
     </row>
     <row r="16" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I16" s="38"/>
-      <c r="AK16" s="50" t="s">
+      <c r="I16" s="48"/>
+      <c r="AK16" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="AL16" s="51">
+      <c r="AL16" s="37">
         <v>900</v>
       </c>
-      <c r="AM16" s="50" t="s">
+      <c r="AM16" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AN16" s="51">
+      <c r="AN16" s="37">
         <v>1600</v>
       </c>
       <c r="AO16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="BC16" s="50" t="s">
+      <c r="AP16">
+        <v>2200</v>
+      </c>
+      <c r="BC16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="BD16" s="51">
+      <c r="BD16" s="37">
         <v>1501</v>
       </c>
     </row>
     <row r="17" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I17" s="38"/>
+      <c r="I17" s="48"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="AH17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AK17" s="50" t="s">
+      <c r="AK17" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AL17" s="51">
+      <c r="AL17" s="37">
         <v>901</v>
       </c>
-      <c r="AM17" s="50" t="s">
+      <c r="AM17" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AN17" s="51">
+      <c r="AN17" s="37">
         <v>1601</v>
       </c>
       <c r="AO17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="BC17" s="50" t="s">
+      <c r="AP17">
+        <v>2201</v>
+      </c>
+      <c r="BC17" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="BD17" s="51">
+      <c r="BD17" s="37">
         <v>1600</v>
       </c>
     </row>
     <row r="18" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I18" s="38"/>
-      <c r="AK18" s="50" t="s">
+      <c r="I18" s="48"/>
+      <c r="AK18" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AL18" s="51">
+      <c r="AL18" s="37">
         <v>1000</v>
       </c>
       <c r="AM18" s="13"/>
@@ -1701,19 +1725,22 @@
       <c r="AO18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="BC18" s="50" t="s">
+      <c r="AP18">
+        <v>2300</v>
+      </c>
+      <c r="BC18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="BD18" s="51">
+      <c r="BD18" s="37">
         <v>1601</v>
       </c>
     </row>
     <row r="19" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I19" s="38"/>
-      <c r="AK19" s="50" t="s">
+      <c r="I19" s="48"/>
+      <c r="AK19" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AL19" s="51">
+      <c r="AL19" s="37">
         <v>1001</v>
       </c>
       <c r="AM19" s="17"/>
@@ -1721,9 +1748,12 @@
       <c r="AO19" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="AP19">
+        <v>2301</v>
+      </c>
     </row>
     <row r="20" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I20" s="38"/>
+      <c r="I20" s="48"/>
       <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1736,17 +1766,17 @@
       <c r="AP20" s="17"/>
     </row>
     <row r="21" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I21" s="38"/>
+      <c r="I21" s="48"/>
       <c r="AM21" s="17"/>
       <c r="AN21" s="17"/>
       <c r="AO21" s="17"/>
       <c r="AP21" s="17"/>
     </row>
     <row r="22" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="AM22" s="46"/>
-      <c r="AN22" s="46"/>
-      <c r="AO22" s="46"/>
-      <c r="AP22" s="46"/>
+      <c r="AM22" s="33"/>
+      <c r="AN22" s="33"/>
+      <c r="AO22" s="33"/>
+      <c r="AP22" s="33"/>
     </row>
     <row r="23" spans="9:56" x14ac:dyDescent="0.4">
       <c r="AM23" s="17"/>
@@ -1840,28 +1870,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BF5"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AK4:AP4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AK4:AP4"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AS4:AT4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1886,20 +1916,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="25"/>
@@ -2090,7 +2120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
   <dimension ref="A4:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2104,14 +2134,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add Jump Walk animations for Raccon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC2FD9-B50F-4A7B-B05C-12BAA7ECB980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394FA867-0B14-4EEE-99D9-81497626008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="754" yWindow="754" windowWidth="24686" windowHeight="13337" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="1097" yWindow="1097" windowWidth="24686" windowHeight="13337" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,8 +610,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,37 +628,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1017,86 +1017,86 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43" t="s">
+      <c r="L4" s="50"/>
+      <c r="M4" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="43"/>
+      <c r="N4" s="50"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="44" t="s">
+      <c r="S4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44" t="s">
+      <c r="T4" s="43"/>
+      <c r="U4" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44" t="s">
+      <c r="V4" s="43"/>
+      <c r="W4" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="44" t="s">
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="44"/>
-      <c r="AA4" s="41" t="s">
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="41" t="s">
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="41" t="s">
+      <c r="AD4" s="45"/>
+      <c r="AE4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="41" t="s">
+      <c r="AF4" s="45"/>
+      <c r="AG4" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="41" t="s">
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="42"/>
-      <c r="AK4" s="45" t="s">
+      <c r="AJ4" s="45"/>
+      <c r="AK4" s="51" t="s">
         <v>18</v>
       </c>
       <c r="AL4" s="46"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="42"/>
-      <c r="AQ4" s="41" t="s">
+      <c r="AM4" s="52"/>
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="52"/>
+      <c r="AP4" s="45"/>
+      <c r="AQ4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="41" t="s">
+      <c r="AR4" s="45"/>
+      <c r="AS4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="AT4" s="42"/>
-      <c r="AU4" s="41" t="s">
+      <c r="AT4" s="45"/>
+      <c r="AU4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AV4" s="42"/>
-      <c r="AW4" s="41" t="s">
+      <c r="AV4" s="45"/>
+      <c r="AW4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="42"/>
+      <c r="AX4" s="45"/>
       <c r="BB4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="40" t="s">
+      <c r="BC4" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="40"/>
-      <c r="BE4" s="40"/>
-      <c r="BF4" s="40"/>
+      <c r="BD4" s="53"/>
+      <c r="BE4" s="53"/>
+      <c r="BF4" s="53"/>
     </row>
     <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1177,14 +1177,14 @@
         <v>33</v>
       </c>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="52" t="s">
+      <c r="AM5" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" s="53"/>
-      <c r="AO5" s="51" t="s">
+      <c r="AN5" s="42"/>
+      <c r="AO5" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="51"/>
+      <c r="AP5" s="40"/>
       <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1212,12 +1212,12 @@
       <c r="BB5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="40" t="s">
+      <c r="BC5" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="40"/>
-      <c r="BF5" s="40"/>
+      <c r="BD5" s="53"/>
+      <c r="BE5" s="53"/>
+      <c r="BF5" s="53"/>
     </row>
     <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
@@ -1226,7 +1226,7 @@
       <c r="I6" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="48" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1339,8 +1339,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="50"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1399,8 +1399,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="50"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="49"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1439,8 +1439,8 @@
       </c>
     </row>
     <row r="9" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I9" s="48"/>
-      <c r="J9" s="50"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="49"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1479,7 +1479,7 @@
       </c>
     </row>
     <row r="10" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I10" s="48"/>
+      <c r="I10" s="47"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="11" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I11" s="48"/>
+      <c r="I11" s="47"/>
       <c r="AK11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1541,7 +1541,7 @@
       </c>
     </row>
     <row r="12" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I12" s="48"/>
+      <c r="I12" s="47"/>
       <c r="AK12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1570,7 @@
       </c>
     </row>
     <row r="13" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I13" s="48"/>
+      <c r="I13" s="47"/>
       <c r="AK13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="14" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I14" s="48"/>
+      <c r="I14" s="47"/>
       <c r="AK14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1626,7 +1626,7 @@
       </c>
     </row>
     <row r="15" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I15" s="48"/>
+      <c r="I15" s="47"/>
       <c r="AK15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="16" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I16" s="48"/>
+      <c r="I16" s="47"/>
       <c r="AK16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
     </row>
     <row r="17" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I17" s="48"/>
+      <c r="I17" s="47"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="18" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I18" s="48"/>
+      <c r="I18" s="47"/>
       <c r="AK18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="19" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I19" s="48"/>
+      <c r="I19" s="47"/>
       <c r="AK19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="20" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I20" s="48"/>
+      <c r="I20" s="47"/>
       <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1766,7 +1766,7 @@
       <c r="AP20" s="17"/>
     </row>
     <row r="21" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I21" s="48"/>
+      <c r="I21" s="47"/>
       <c r="AM21" s="17"/>
       <c r="AN21" s="17"/>
       <c r="AO21" s="17"/>
@@ -1870,12 +1870,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AK4:AP4"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AS4:AT4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -1884,14 +1886,12 @@
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AK4:AP4"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BF5"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1916,12 +1916,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" s="54" t="s">
@@ -2137,11 +2137,11 @@
       <c r="B4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add Jump Run animations for Raccon Mario. Fix bug: Jump Run animation always display when pressed Run button
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394FA867-0B14-4EEE-99D9-81497626008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5843BF8-4F97-47C7-A4D5-3B2BEBD615DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1097" yWindow="1097" windowWidth="24686" windowHeight="13337" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="1097" yWindow="1097" windowWidth="24686" windowHeight="13337" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -309,6 +309,30 @@
   </si>
   <si>
     <t>Hoặc return nhầm ani_id (xem mục Debug Out để biết được ani_id return nhầm là gì</t>
+  </si>
+  <si>
+    <t>Mario luôn tăng được speed ngay cả khi đang bay</t>
+  </si>
+  <si>
+    <t>Nhấm phím chạy</t>
+  </si>
+  <si>
+    <t>Do chưa xét Mario có đứng trên platform hoặc blocking obejct. Mario phải đứng trên một bề mặt cứng nào đó thì mới có thể tăng tốc được (vật lý)</t>
+  </si>
+  <si>
+    <t>Mario luôn có animation JUMP RUNNING ngay cả khi chưa đạt được tốc độ tối đa</t>
+  </si>
+  <si>
+    <t>Luôn luôn</t>
+  </si>
+  <si>
+    <t>Do sample code chỉ xét giá trị tuyệt đối của gia tốc, chứ không có xét tốc độ nên luôn có animation đó nếu nhấm phím chạy</t>
+  </si>
+  <si>
+    <t>Đã fix</t>
+  </si>
+  <si>
+    <t>Oke rồi</t>
   </si>
 </sst>
 </file>
@@ -535,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -657,6 +681,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="AJ1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
@@ -1902,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2016,17 +2046,49 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+    <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A8" s="56">
+        <v>4</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B10" s="26"/>

</xml_diff>

<commit_message>
Implement basic camera: Camere now won't flow Mario in y-axis
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5843BF8-4F97-47C7-A4D5-3B2BEBD615DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FA69E-ED1E-4541-907B-DE78865309C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1097" yWindow="1097" windowWidth="24686" windowHeight="13337" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="4680" yWindow="2366" windowWidth="24686" windowHeight="13337" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -333,6 +334,21 @@
   </si>
   <si>
     <t>Oke rồi</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Đặt giới hạn cho tốc độ rơi của mọi game object</t>
+  </si>
+  <si>
+    <t>Lý do</t>
+  </si>
+  <si>
+    <t>Việc cần làm</t>
+  </si>
+  <si>
+    <t>Nếu mỗi frame mà cứ tăng vận tốc cho đến khi gặp platform thì đặt lại bằng 0 thì object sẽ rơi rất nhanh xuống mặt đất, tuy là đúng với vật lý nhưng player sẽ rất khó theo kịp tốc độ rơi như vậy, vì game obejct rơi quá nhanh</t>
   </si>
 </sst>
 </file>
@@ -559,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -634,6 +650,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,50 +704,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1047,33 +1075,33 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="50" t="s">
+      <c r="K4" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50" t="s">
+      <c r="L4" s="54"/>
+      <c r="M4" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="50"/>
+      <c r="N4" s="54"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="S4" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43" t="s">
+      <c r="T4" s="46"/>
+      <c r="U4" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43" t="s">
+      <c r="V4" s="46"/>
+      <c r="W4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43" t="s">
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="43"/>
+      <c r="Z4" s="46"/>
       <c r="AA4" s="44" t="s">
         <v>15</v>
       </c>
@@ -1094,13 +1122,13 @@
         <v>39</v>
       </c>
       <c r="AJ4" s="45"/>
-      <c r="AK4" s="51" t="s">
+      <c r="AK4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="46"/>
-      <c r="AM4" s="52"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="52"/>
+      <c r="AL4" s="48"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
       <c r="AP4" s="45"/>
       <c r="AQ4" s="44" t="s">
         <v>35</v>
@@ -1121,12 +1149,12 @@
       <c r="BB4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="53" t="s">
+      <c r="BC4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="53"/>
-      <c r="BE4" s="53"/>
-      <c r="BF4" s="53"/>
+      <c r="BD4" s="50"/>
+      <c r="BE4" s="50"/>
+      <c r="BF4" s="50"/>
     </row>
     <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1207,14 +1235,14 @@
         <v>33</v>
       </c>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="41" t="s">
+      <c r="AM5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" s="42"/>
-      <c r="AO5" s="40" t="s">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="40"/>
+      <c r="AP5" s="55"/>
       <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1242,21 +1270,21 @@
       <c r="BB5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="53" t="s">
+      <c r="BC5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="53"/>
-      <c r="BE5" s="53"/>
-      <c r="BF5" s="53"/>
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
     </row>
     <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="48" t="s">
+      <c r="J6" s="52" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1369,8 +1397,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="49"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="53"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1429,8 +1457,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="49"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="53"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1469,8 +1497,8 @@
       </c>
     </row>
     <row r="9" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I9" s="47"/>
-      <c r="J9" s="49"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="53"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1509,7 +1537,7 @@
       </c>
     </row>
     <row r="10" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I10" s="47"/>
+      <c r="I10" s="51"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1542,7 +1570,7 @@
       </c>
     </row>
     <row r="11" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I11" s="47"/>
+      <c r="I11" s="51"/>
       <c r="AK11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1571,7 +1599,7 @@
       </c>
     </row>
     <row r="12" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I12" s="47"/>
+      <c r="I12" s="51"/>
       <c r="AK12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1628,7 @@
       </c>
     </row>
     <row r="13" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I13" s="47"/>
+      <c r="I13" s="51"/>
       <c r="AK13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1629,7 +1657,7 @@
       </c>
     </row>
     <row r="14" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I14" s="47"/>
+      <c r="I14" s="51"/>
       <c r="AK14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1656,7 +1684,7 @@
       </c>
     </row>
     <row r="15" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I15" s="47"/>
+      <c r="I15" s="51"/>
       <c r="AK15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1683,7 +1711,7 @@
       </c>
     </row>
     <row r="16" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I16" s="47"/>
+      <c r="I16" s="51"/>
       <c r="AK16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1710,7 +1738,7 @@
       </c>
     </row>
     <row r="17" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I17" s="47"/>
+      <c r="I17" s="51"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
@@ -1743,7 +1771,7 @@
       </c>
     </row>
     <row r="18" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I18" s="47"/>
+      <c r="I18" s="51"/>
       <c r="AK18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1766,7 +1794,7 @@
       </c>
     </row>
     <row r="19" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I19" s="47"/>
+      <c r="I19" s="51"/>
       <c r="AK19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1783,7 +1811,7 @@
       </c>
     </row>
     <row r="20" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I20" s="47"/>
+      <c r="I20" s="51"/>
       <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1796,7 +1824,7 @@
       <c r="AP20" s="17"/>
     </row>
     <row r="21" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I21" s="47"/>
+      <c r="I21" s="51"/>
       <c r="AM21" s="17"/>
       <c r="AN21" s="17"/>
       <c r="AO21" s="17"/>
@@ -1900,6 +1928,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I6:I21"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="AK4:AP4"/>
@@ -1908,20 +1948,8 @@
     <mergeCell ref="AU4:AV4"/>
     <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="I6:I21"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
     <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1932,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:G9"/>
     </sheetView>
   </sheetViews>
@@ -1946,20 +1974,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="25"/>
@@ -2047,25 +2075,25 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A8" s="56">
+      <c r="A8" s="42">
         <v>4</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="43" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2085,7 +2113,7 @@
       <c r="E9" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="43" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="4"/>
@@ -2179,6 +2207,104 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069F29C-963D-4DAE-A0BD-503262FD907C}">
+  <dimension ref="B3:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="9.23046875" style="40"/>
+    <col min="3" max="3" width="40.84375" customWidth="1"/>
+    <col min="4" max="4" width="55.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B3" s="40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B4" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="B5" s="61">
+        <v>1</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="61"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B7" s="61"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B8" s="61"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B9" s="61"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B10" s="61"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B11" s="61"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B12" s="61"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B13" s="61"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B14" s="61"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B15" s="61"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
   <dimension ref="A4:G8"/>
   <sheetViews>
@@ -2196,14 +2322,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Adjust Mario's y when changing level. Add button to switch to Mario Raccon
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FA69E-ED1E-4541-907B-DE78865309C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C12C41C-DFD8-45EB-87D4-6211B7E90AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2366" windowWidth="24686" windowHeight="13337" activeTab="2" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="4680" yWindow="2366" windowWidth="24686" windowHeight="13337" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="107">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -349,6 +349,15 @@
   </si>
   <si>
     <t>Nếu mỗi frame mà cứ tăng vận tốc cho đến khi gặp platform thì đặt lại bằng 0 thì object sẽ rơi rất nhanh xuống mặt đất, tuy là đúng với vật lý nhưng player sẽ rất khó theo kịp tốc độ rơi như vậy, vì game obejct rơi quá nhanh</t>
+  </si>
+  <si>
+    <t>Thỉnh thoảng, Mario không ăn được Mushroom</t>
+  </si>
+  <si>
+    <t>Mario ở trên platform + gravity</t>
+  </si>
+  <si>
+    <t>thỉnh thoảng</t>
   </si>
 </sst>
 </file>
@@ -394,7 +403,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -571,11 +580,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,6 +735,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1960,13 +1986,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="26.23046875" customWidth="1"/>
+    <col min="2" max="2" width="28.61328125" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="11.69140625" customWidth="1"/>
@@ -2118,11 +2144,23 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A10" s="62">
+        <v>6</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="E10" s="26"/>
+      <c r="F10" s="63" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B11" s="26"/>
@@ -2210,8 +2248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069F29C-963D-4DAE-A0BD-503262FD907C}">
   <dimension ref="B3:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Raccon Mario now can fall slow using his tail, currently no tail animation
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C12C41C-DFD8-45EB-87D4-6211B7E90AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FED9F5C-B410-4807-8D5D-5FEBE2F082CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2366" windowWidth="24686" windowHeight="13337" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="4843" yWindow="3891" windowWidth="24686" windowHeight="13338" activeTab="3" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>thỉnh thoảng</t>
+  </si>
+  <si>
+    <t>Giải quyết các Warnings</t>
+  </si>
+  <si>
+    <t>Không làm thì bị trừ điểm, ngoài ra còn giúp code chạy đúng hơn</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2245,109 +2251,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069F29C-963D-4DAE-A0BD-503262FD907C}">
-  <dimension ref="B3:D15"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="9.23046875" style="40"/>
-    <col min="3" max="3" width="40.84375" customWidth="1"/>
-    <col min="4" max="4" width="55.23046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B3" s="40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="B5" s="61">
-        <v>1</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B6" s="61"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B7" s="61"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="61"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B9" s="61"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B10" s="61"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B11" s="61"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B12" s="61"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B13" s="61"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B14" s="61"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B15" s="61"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1680CB-5C54-4A77-B843-20CCD9A61EA0}">
   <dimension ref="A4:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2418,4 +2326,108 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069F29C-963D-4DAE-A0BD-503262FD907C}">
+  <dimension ref="B3:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="9.23046875" style="40"/>
+    <col min="3" max="3" width="40.84375" customWidth="1"/>
+    <col min="4" max="4" width="55.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B3" s="40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B4" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="B5" s="61">
+        <v>1</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="61">
+        <v>2</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B7" s="61"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B8" s="61"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B9" s="61"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B10" s="61"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B11" s="61"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B12" s="61"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B13" s="61"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B14" s="61"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B15" s="61"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Fall Slow (wagging tail) for Raccoon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FED9F5C-B410-4807-8D5D-5FEBE2F082CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C90B96E-6640-4879-81EA-ADD0AD38AC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4843" yWindow="3891" windowWidth="24686" windowHeight="13338" activeTab="3" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="4757" yWindow="2563" windowWidth="23014" windowHeight="12308" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>Không làm thì bị trừ điểm, ngoài ra còn giúp code chạy đúng hơn</t>
+  </si>
+  <si>
+    <t>Fall Slow Right</t>
+  </si>
+  <si>
+    <t>Fall Slow Left</t>
   </si>
 </sst>
 </file>
@@ -688,6 +694,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -695,32 +728,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -735,18 +753,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,39 +1070,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BF37"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AP20" sqref="AP20"/>
+    <sheetView tabSelected="1" topLeftCell="AJ7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AS17" sqref="AS17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.07421875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
     <col min="6" max="8" width="16" customWidth="1"/>
-    <col min="12" max="13" width="11.69140625" customWidth="1"/>
-    <col min="14" max="14" width="12.69140625" customWidth="1"/>
-    <col min="18" max="22" width="12.765625" customWidth="1"/>
-    <col min="23" max="23" width="12.3046875" customWidth="1"/>
-    <col min="25" max="25" width="17.53515625" customWidth="1"/>
-    <col min="26" max="26" width="8.84375" customWidth="1"/>
-    <col min="33" max="33" width="15.84375" customWidth="1"/>
-    <col min="35" max="35" width="10.4609375" customWidth="1"/>
-    <col min="37" max="37" width="15.3046875" customWidth="1"/>
-    <col min="38" max="38" width="9.23046875" customWidth="1"/>
-    <col min="39" max="39" width="14.15234375" customWidth="1"/>
-    <col min="41" max="41" width="14.84375" customWidth="1"/>
-    <col min="45" max="45" width="9.3046875" customWidth="1"/>
-    <col min="47" max="47" width="10.84375" customWidth="1"/>
-    <col min="49" max="49" width="9.765625" customWidth="1"/>
-    <col min="50" max="50" width="8.4609375" customWidth="1"/>
-    <col min="51" max="51" width="5.69140625" customWidth="1"/>
-    <col min="52" max="53" width="7.765625" customWidth="1"/>
-    <col min="54" max="54" width="11.61328125" customWidth="1"/>
-    <col min="55" max="56" width="13.4609375" customWidth="1"/>
-    <col min="57" max="57" width="13.15234375" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="18" max="22" width="12.77734375" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" customWidth="1"/>
+    <col min="35" max="35" width="10.44140625" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" customWidth="1"/>
+    <col min="38" max="38" width="9.21875" customWidth="1"/>
+    <col min="39" max="39" width="14.109375" customWidth="1"/>
+    <col min="41" max="41" width="14.88671875" customWidth="1"/>
+    <col min="45" max="45" width="9.33203125" customWidth="1"/>
+    <col min="47" max="47" width="10.88671875" customWidth="1"/>
+    <col min="49" max="49" width="9.77734375" customWidth="1"/>
+    <col min="50" max="50" width="8.44140625" customWidth="1"/>
+    <col min="51" max="51" width="5.6640625" customWidth="1"/>
+    <col min="52" max="53" width="7.77734375" customWidth="1"/>
+    <col min="54" max="54" width="11.6640625" customWidth="1"/>
+    <col min="55" max="56" width="13.44140625" customWidth="1"/>
+    <col min="57" max="57" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:58" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:58" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1107,88 +1113,88 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54" t="s">
+      <c r="L4" s="55"/>
+      <c r="M4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="54"/>
+      <c r="N4" s="55"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="46" t="s">
+      <c r="S4" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46" t="s">
+      <c r="T4" s="52"/>
+      <c r="U4" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46" t="s">
+      <c r="V4" s="52"/>
+      <c r="W4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46" t="s">
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="44" t="s">
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="44" t="s">
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="44" t="s">
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="44" t="s">
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="44" t="s">
+      <c r="AH4" s="54"/>
+      <c r="AI4" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="45"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AJ4" s="54"/>
+      <c r="AK4" s="56" t="s">
         <v>18</v>
       </c>
       <c r="AL4" s="48"/>
-      <c r="AM4" s="49"/>
-      <c r="AN4" s="49"/>
-      <c r="AO4" s="49"/>
-      <c r="AP4" s="45"/>
-      <c r="AQ4" s="44" t="s">
+      <c r="AM4" s="57"/>
+      <c r="AN4" s="57"/>
+      <c r="AO4" s="57"/>
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="45"/>
-      <c r="AS4" s="44" t="s">
+      <c r="AR4" s="54"/>
+      <c r="AS4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="AT4" s="45"/>
-      <c r="AU4" s="44" t="s">
+      <c r="AT4" s="54"/>
+      <c r="AU4" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="AV4" s="45"/>
-      <c r="AW4" s="44" t="s">
+      <c r="AV4" s="54"/>
+      <c r="AW4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="45"/>
+      <c r="AX4" s="54"/>
       <c r="BB4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="50" t="s">
+      <c r="BC4" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="50"/>
-      <c r="BE4" s="50"/>
-      <c r="BF4" s="50"/>
-    </row>
-    <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="58"/>
+      <c r="BF4" s="58"/>
+    </row>
+    <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1267,14 +1273,14 @@
         <v>33</v>
       </c>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="56" t="s">
+      <c r="AM5" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="55" t="s">
+      <c r="AN5" s="61"/>
+      <c r="AO5" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="55"/>
+      <c r="AP5" s="59"/>
       <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1302,21 +1308,21 @@
       <c r="BB5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="50" t="s">
+      <c r="BC5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="50"/>
-      <c r="BE5" s="50"/>
-      <c r="BF5" s="50"/>
-    </row>
-    <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BD5" s="58"/>
+      <c r="BE5" s="58"/>
+      <c r="BF5" s="58"/>
+    </row>
+    <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="50" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1422,15 +1428,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="2:58" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:58" x14ac:dyDescent="0.3">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="51"/>
-      <c r="J7" s="53"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="51"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1485,12 +1491,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:58" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:58" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="53"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="51"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1528,9 +1534,9 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I9" s="51"/>
-      <c r="J9" s="53"/>
+    <row r="9" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I9" s="49"/>
+      <c r="J9" s="51"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1568,8 +1574,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I10" s="51"/>
+    <row r="10" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I10" s="49"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1601,8 +1607,8 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I11" s="51"/>
+    <row r="11" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I11" s="49"/>
       <c r="AK11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1630,8 +1636,8 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I12" s="51"/>
+    <row r="12" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I12" s="49"/>
       <c r="AK12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1659,8 +1665,8 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I13" s="51"/>
+    <row r="13" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I13" s="49"/>
       <c r="AK13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1688,8 +1694,8 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I14" s="51"/>
+    <row r="14" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I14" s="49"/>
       <c r="AK14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1715,8 +1721,8 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I15" s="51"/>
+    <row r="15" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I15" s="49"/>
       <c r="AK15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1742,8 +1748,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:58" x14ac:dyDescent="0.4">
-      <c r="I16" s="51"/>
+    <row r="16" spans="2:58" x14ac:dyDescent="0.3">
+      <c r="I16" s="49"/>
       <c r="AK16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1769,8 +1775,8 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I17" s="51"/>
+    <row r="17" spans="9:56" x14ac:dyDescent="0.3">
+      <c r="I17" s="49"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
@@ -1802,8 +1808,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I18" s="51"/>
+    <row r="18" spans="9:56" x14ac:dyDescent="0.3">
+      <c r="I18" s="49"/>
       <c r="AK18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1825,8 +1831,8 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I19" s="51"/>
+    <row r="19" spans="9:56" x14ac:dyDescent="0.3">
+      <c r="I19" s="49"/>
       <c r="AK19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1842,8 +1848,8 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="20" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I20" s="51"/>
+    <row r="20" spans="9:56" x14ac:dyDescent="0.3">
+      <c r="I20" s="49"/>
       <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1852,107 +1858,115 @@
       </c>
       <c r="AM20" s="17"/>
       <c r="AN20" s="17"/>
-      <c r="AO20" s="17"/>
-      <c r="AP20" s="17"/>
-    </row>
-    <row r="21" spans="9:56" x14ac:dyDescent="0.4">
-      <c r="I21" s="51"/>
+      <c r="AO20" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP20" s="17">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="21" spans="9:56" x14ac:dyDescent="0.3">
+      <c r="I21" s="49"/>
       <c r="AM21" s="17"/>
       <c r="AN21" s="17"/>
-      <c r="AO21" s="17"/>
-      <c r="AP21" s="17"/>
-    </row>
-    <row r="22" spans="9:56" x14ac:dyDescent="0.4">
+      <c r="AO21" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP21" s="20">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="22" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM22" s="33"/>
       <c r="AN22" s="33"/>
       <c r="AO22" s="33"/>
       <c r="AP22" s="33"/>
     </row>
-    <row r="23" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="23" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM23" s="17"/>
       <c r="AN23" s="17"/>
       <c r="AO23" s="17"/>
       <c r="AP23" s="17"/>
     </row>
-    <row r="24" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="24" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM24" s="17"/>
       <c r="AN24" s="17"/>
       <c r="AO24" s="17"/>
       <c r="AP24" s="17"/>
     </row>
-    <row r="25" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="25" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM25" s="17"/>
       <c r="AN25" s="17"/>
       <c r="AO25" s="17"/>
       <c r="AP25" s="17"/>
     </row>
-    <row r="26" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="26" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM26" s="17"/>
       <c r="AN26" s="17"/>
       <c r="AO26" s="17"/>
       <c r="AP26" s="17"/>
     </row>
-    <row r="27" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="27" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM27" s="17"/>
       <c r="AN27" s="17"/>
       <c r="AO27" s="17"/>
       <c r="AP27" s="17"/>
     </row>
-    <row r="28" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="28" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM28" s="17"/>
       <c r="AN28" s="17"/>
       <c r="AO28" s="17"/>
       <c r="AP28" s="17"/>
     </row>
-    <row r="29" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="29" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM29" s="17"/>
       <c r="AN29" s="17"/>
       <c r="AO29" s="17"/>
       <c r="AP29" s="17"/>
     </row>
-    <row r="30" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="30" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM30" s="17"/>
       <c r="AN30" s="17"/>
       <c r="AO30" s="17"/>
       <c r="AP30" s="17"/>
     </row>
-    <row r="31" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="31" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM31" s="17"/>
       <c r="AN31" s="17"/>
       <c r="AO31" s="17"/>
       <c r="AP31" s="17"/>
     </row>
-    <row r="32" spans="9:56" x14ac:dyDescent="0.4">
+    <row r="32" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM32" s="17"/>
       <c r="AN32" s="17"/>
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
     </row>
-    <row r="33" spans="39:42" x14ac:dyDescent="0.4">
+    <row r="33" spans="39:42" x14ac:dyDescent="0.3">
       <c r="AM33" s="17"/>
       <c r="AN33" s="17"/>
       <c r="AO33" s="17"/>
       <c r="AP33" s="17"/>
     </row>
-    <row r="34" spans="39:42" x14ac:dyDescent="0.4">
+    <row r="34" spans="39:42" x14ac:dyDescent="0.3">
       <c r="AM34" s="17"/>
       <c r="AN34" s="17"/>
       <c r="AO34" s="17"/>
       <c r="AP34" s="17"/>
     </row>
-    <row r="35" spans="39:42" x14ac:dyDescent="0.4">
+    <row r="35" spans="39:42" x14ac:dyDescent="0.3">
       <c r="AM35" s="32"/>
       <c r="AN35" s="32"/>
       <c r="AO35" s="32"/>
       <c r="AP35" s="32"/>
     </row>
-    <row r="36" spans="39:42" x14ac:dyDescent="0.4">
+    <row r="36" spans="39:42" x14ac:dyDescent="0.3">
       <c r="AM36" s="20"/>
       <c r="AN36" s="20"/>
       <c r="AO36" s="20"/>
       <c r="AP36" s="20"/>
     </row>
-    <row r="37" spans="39:42" x14ac:dyDescent="0.4">
+    <row r="37" spans="39:42" x14ac:dyDescent="0.3">
       <c r="AM37" s="20"/>
       <c r="AN37" s="20"/>
       <c r="AO37" s="20"/>
@@ -1960,6 +1974,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AK4:AP4"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -1972,16 +1996,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AK4:AP4"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BF5"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1996,35 +2010,35 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.61328125" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="11.69140625" customWidth="1"/>
-    <col min="7" max="7" width="16.3046875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="50" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="58" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2047,7 +2061,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -2068,7 +2082,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -2087,7 +2101,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -2106,7 +2120,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="42">
         <v>4</v>
       </c>
@@ -2129,7 +2143,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -2150,8 +2164,8 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="62">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="46">
         <v>6</v>
       </c>
       <c r="B10" s="26" t="s">
@@ -2164,77 +2178,77 @@
         <v>106</v>
       </c>
       <c r="E10" s="26"/>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="47" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -2258,26 +2272,26 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.84375" customWidth="1"/>
-    <col min="3" max="3" width="23.69140625" customWidth="1"/>
-    <col min="4" max="4" width="56.23046875" customWidth="1"/>
-    <col min="5" max="5" width="12.23046875" customWidth="1"/>
-    <col min="6" max="6" width="15.07421875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="59" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
@@ -2291,7 +2305,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -2303,7 +2317,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -2315,7 +2329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="24" t="s">
         <v>90</v>
       </c>
@@ -2332,23 +2346,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069F29C-963D-4DAE-A0BD-503262FD907C}">
   <dimension ref="B3:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.23046875" style="40"/>
-    <col min="3" max="3" width="40.84375" customWidth="1"/>
-    <col min="4" max="4" width="55.23046875" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="40"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="55.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -2359,72 +2373,72 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="B5" s="61">
+    <row r="5" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="45">
         <v>1</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="44" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B6" s="61">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="45">
         <v>2</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="44" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B7" s="61"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="61"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B9" s="61"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B10" s="61"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B11" s="61"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B12" s="61"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B13" s="61"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B14" s="61"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B15" s="61"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="45"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="45"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="45"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="45"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="45"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="45"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="45"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="45"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="45"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Raccoon Mario now can fly, but not smooth
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C90B96E-6640-4879-81EA-ADD0AD38AC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774BAA6-5DC6-4558-A290-B797C70317FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4757" yWindow="2563" windowWidth="23014" windowHeight="12308" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="2289" yWindow="3711" windowWidth="20871" windowHeight="10895" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Fall Slow Left</t>
+  </si>
+  <si>
+    <t>Flying Right</t>
+  </si>
+  <si>
+    <t>Flying Left</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -706,9 +712,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -719,33 +752,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,6 +759,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AS17" sqref="AS17"/>
+    <sheetView tabSelected="1" topLeftCell="AJ13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AT23" sqref="AT23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,86 +1125,86 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55" t="s">
+      <c r="L4" s="61"/>
+      <c r="M4" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="55"/>
+      <c r="N4" s="61"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="52" t="s">
+      <c r="S4" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52" t="s">
+      <c r="T4" s="50"/>
+      <c r="U4" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52" t="s">
+      <c r="V4" s="50"/>
+      <c r="W4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52" t="s">
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="53" t="s">
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="53" t="s">
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="54"/>
-      <c r="AE4" s="53" t="s">
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="53" t="s">
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="54"/>
-      <c r="AI4" s="53" t="s">
+      <c r="AH4" s="49"/>
+      <c r="AI4" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="54"/>
-      <c r="AK4" s="56" t="s">
+      <c r="AJ4" s="49"/>
+      <c r="AK4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="48"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="57"/>
-      <c r="AO4" s="57"/>
-      <c r="AP4" s="54"/>
-      <c r="AQ4" s="53" t="s">
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="53"/>
+      <c r="AN4" s="53"/>
+      <c r="AO4" s="53"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="54"/>
-      <c r="AS4" s="53" t="s">
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="AT4" s="54"/>
-      <c r="AU4" s="53" t="s">
+      <c r="AT4" s="49"/>
+      <c r="AU4" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AV4" s="54"/>
-      <c r="AW4" s="53" t="s">
+      <c r="AV4" s="49"/>
+      <c r="AW4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="54"/>
+      <c r="AX4" s="49"/>
       <c r="BB4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="58" t="s">
+      <c r="BC4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="58"/>
-      <c r="BE4" s="58"/>
-      <c r="BF4" s="58"/>
+      <c r="BD4" s="54"/>
+      <c r="BE4" s="54"/>
+      <c r="BF4" s="54"/>
     </row>
     <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
@@ -1273,14 +1285,14 @@
         <v>33</v>
       </c>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="60" t="s">
+      <c r="AM5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="59" t="s">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="59"/>
+      <c r="AP5" s="55"/>
       <c r="AQ5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1308,21 +1320,21 @@
       <c r="BB5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="58" t="s">
+      <c r="BC5" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="58"/>
-      <c r="BE5" s="58"/>
-      <c r="BF5" s="58"/>
+      <c r="BD5" s="54"/>
+      <c r="BE5" s="54"/>
+      <c r="BF5" s="54"/>
     </row>
     <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="59" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1435,8 +1447,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="49"/>
-      <c r="J7" s="51"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="60"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1495,8 +1507,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="51"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="60"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1535,8 +1547,8 @@
       </c>
     </row>
     <row r="9" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I9" s="49"/>
-      <c r="J9" s="51"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="60"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1575,7 +1587,7 @@
       </c>
     </row>
     <row r="10" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I10" s="49"/>
+      <c r="I10" s="58"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1608,7 +1620,7 @@
       </c>
     </row>
     <row r="11" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I11" s="49"/>
+      <c r="I11" s="58"/>
       <c r="AK11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1637,7 +1649,7 @@
       </c>
     </row>
     <row r="12" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I12" s="49"/>
+      <c r="I12" s="58"/>
       <c r="AK12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1666,7 +1678,7 @@
       </c>
     </row>
     <row r="13" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I13" s="49"/>
+      <c r="I13" s="58"/>
       <c r="AK13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1695,7 +1707,7 @@
       </c>
     </row>
     <row r="14" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I14" s="49"/>
+      <c r="I14" s="58"/>
       <c r="AK14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1722,7 +1734,7 @@
       </c>
     </row>
     <row r="15" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I15" s="49"/>
+      <c r="I15" s="58"/>
       <c r="AK15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1749,7 +1761,7 @@
       </c>
     </row>
     <row r="16" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I16" s="49"/>
+      <c r="I16" s="58"/>
       <c r="AK16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1776,7 +1788,7 @@
       </c>
     </row>
     <row r="17" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I17" s="49"/>
+      <c r="I17" s="58"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1821,7 @@
       </c>
     </row>
     <row r="18" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I18" s="49"/>
+      <c r="I18" s="58"/>
       <c r="AK18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1832,7 +1844,7 @@
       </c>
     </row>
     <row r="19" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I19" s="49"/>
+      <c r="I19" s="58"/>
       <c r="AK19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1849,7 +1861,7 @@
       </c>
     </row>
     <row r="20" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I20" s="49"/>
+      <c r="I20" s="58"/>
       <c r="AK20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1866,7 +1878,7 @@
       </c>
     </row>
     <row r="21" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I21" s="49"/>
+      <c r="I21" s="58"/>
       <c r="AM21" s="17"/>
       <c r="AN21" s="17"/>
       <c r="AO21" s="20" t="s">
@@ -1879,14 +1891,22 @@
     <row r="22" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM22" s="33"/>
       <c r="AN22" s="33"/>
-      <c r="AO22" s="33"/>
-      <c r="AP22" s="33"/>
+      <c r="AO22" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP22" s="65">
+        <v>2500</v>
+      </c>
     </row>
     <row r="23" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM23" s="17"/>
       <c r="AN23" s="17"/>
-      <c r="AO23" s="17"/>
-      <c r="AP23" s="17"/>
+      <c r="AO23" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP23" s="20">
+        <v>2501</v>
+      </c>
     </row>
     <row r="24" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM24" s="17"/>
@@ -1974,16 +1994,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AK4:AP4"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BF5"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -1996,6 +2006,16 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AK4:AP4"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AM5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2020,12 +2040,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="62" t="s">
@@ -2285,11 +2305,11 @@
       <c r="B4" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add Tail Attack animations for Raccoon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774BAA6-5DC6-4558-A290-B797C70317FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F823D2E7-EDE9-4021-BE86-AEA7152B0A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2289" yWindow="3711" windowWidth="20871" windowHeight="10895" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="17" yWindow="17" windowWidth="17820" windowHeight="11880" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Flying Left</t>
+  </si>
+  <si>
+    <t>Attack Right</t>
+  </si>
+  <si>
+    <t>Attck Left</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1089,7 @@
   <dimension ref="B4:BF37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AJ13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AT23" sqref="AT23"/>
+      <selection activeCell="AQ24" sqref="AQ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1911,14 +1917,22 @@
     <row r="24" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM24" s="17"/>
       <c r="AN24" s="17"/>
-      <c r="AO24" s="17"/>
-      <c r="AP24" s="17"/>
+      <c r="AO24" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP24" s="20">
+        <v>2600</v>
+      </c>
     </row>
     <row r="25" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM25" s="17"/>
       <c r="AN25" s="17"/>
-      <c r="AO25" s="17"/>
-      <c r="AP25" s="17"/>
+      <c r="AO25" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP25" s="20">
+        <v>2601</v>
+      </c>
     </row>
     <row r="26" spans="9:56" x14ac:dyDescent="0.3">
       <c r="AM26" s="17"/>

</xml_diff>

<commit_message>
Create Breakable Brick with basic feature - rendering
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F823D2E7-EDE9-4021-BE86-AEA7152B0A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A264686-D0BD-4F53-90C7-802D28743D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17" yWindow="17" windowWidth="17820" windowHeight="11880" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>Attck Left</t>
+  </si>
+  <si>
+    <t>Breakable Brick</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -718,6 +721,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,14 +752,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,28 +773,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,41 +1092,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BF37"/>
+  <dimension ref="B4:BH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AQ24" sqref="AQ24"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20:AI21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.07421875" customWidth="1"/>
     <col min="6" max="8" width="16" customWidth="1"/>
-    <col min="12" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="18" max="22" width="12.77734375" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" customWidth="1"/>
-    <col min="25" max="25" width="17.5546875" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="33" max="33" width="15.88671875" customWidth="1"/>
-    <col min="35" max="35" width="10.44140625" customWidth="1"/>
-    <col min="37" max="37" width="15.33203125" customWidth="1"/>
-    <col min="38" max="38" width="9.21875" customWidth="1"/>
-    <col min="39" max="39" width="14.109375" customWidth="1"/>
-    <col min="41" max="41" width="14.88671875" customWidth="1"/>
-    <col min="45" max="45" width="9.33203125" customWidth="1"/>
-    <col min="47" max="47" width="10.88671875" customWidth="1"/>
-    <col min="49" max="49" width="9.77734375" customWidth="1"/>
-    <col min="50" max="50" width="8.44140625" customWidth="1"/>
-    <col min="51" max="51" width="5.6640625" customWidth="1"/>
-    <col min="52" max="53" width="7.77734375" customWidth="1"/>
-    <col min="54" max="54" width="11.6640625" customWidth="1"/>
-    <col min="55" max="56" width="13.44140625" customWidth="1"/>
-    <col min="57" max="57" width="13.109375" customWidth="1"/>
+    <col min="12" max="13" width="11.69140625" customWidth="1"/>
+    <col min="14" max="14" width="12.69140625" customWidth="1"/>
+    <col min="18" max="22" width="12.765625" customWidth="1"/>
+    <col min="23" max="23" width="12.3046875" customWidth="1"/>
+    <col min="25" max="25" width="17.53515625" customWidth="1"/>
+    <col min="26" max="26" width="8.84375" customWidth="1"/>
+    <col min="33" max="33" width="15.84375" customWidth="1"/>
+    <col min="35" max="35" width="13.07421875" customWidth="1"/>
+    <col min="37" max="37" width="10.4609375" customWidth="1"/>
+    <col min="39" max="39" width="15.3046875" customWidth="1"/>
+    <col min="40" max="40" width="9.23046875" customWidth="1"/>
+    <col min="41" max="41" width="14.07421875" customWidth="1"/>
+    <col min="43" max="43" width="14.84375" customWidth="1"/>
+    <col min="47" max="47" width="9.3046875" customWidth="1"/>
+    <col min="49" max="49" width="10.84375" customWidth="1"/>
+    <col min="51" max="51" width="9.765625" customWidth="1"/>
+    <col min="52" max="52" width="8.4609375" customWidth="1"/>
+    <col min="53" max="53" width="5.69140625" customWidth="1"/>
+    <col min="54" max="55" width="7.765625" customWidth="1"/>
+    <col min="56" max="56" width="11.69140625" customWidth="1"/>
+    <col min="57" max="58" width="13.4609375" customWidth="1"/>
+    <col min="59" max="59" width="13.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:60" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,88 +1138,92 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="61" t="s">
+      <c r="K4" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61" t="s">
+      <c r="L4" s="58"/>
+      <c r="M4" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="61"/>
+      <c r="N4" s="58"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="50" t="s">
+      <c r="S4" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50" t="s">
+      <c r="T4" s="55"/>
+      <c r="U4" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50" t="s">
+      <c r="V4" s="55"/>
+      <c r="W4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50" t="s">
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="48" t="s">
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="48" t="s">
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="49"/>
-      <c r="AE4" s="48" t="s">
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="49"/>
-      <c r="AG4" s="48" t="s">
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="49"/>
-      <c r="AI4" s="48" t="s">
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="49"/>
-      <c r="AK4" s="51" t="s">
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="53"/>
-      <c r="AN4" s="53"/>
-      <c r="AO4" s="53"/>
-      <c r="AP4" s="49"/>
-      <c r="AQ4" s="48" t="s">
+      <c r="AN4" s="51"/>
+      <c r="AO4" s="60"/>
+      <c r="AP4" s="60"/>
+      <c r="AQ4" s="60"/>
+      <c r="AR4" s="57"/>
+      <c r="AS4" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="49"/>
-      <c r="AS4" s="48" t="s">
+      <c r="AT4" s="57"/>
+      <c r="AU4" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="AT4" s="49"/>
-      <c r="AU4" s="48" t="s">
+      <c r="AV4" s="57"/>
+      <c r="AW4" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="AV4" s="49"/>
-      <c r="AW4" s="48" t="s">
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="49"/>
-      <c r="BB4" s="38" t="s">
+      <c r="AZ4" s="57"/>
+      <c r="BD4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BC4" s="54" t="s">
+      <c r="BE4" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="BD4" s="54"/>
-      <c r="BE4" s="54"/>
-      <c r="BF4" s="54"/>
-    </row>
-    <row r="5" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BF4" s="61"/>
+      <c r="BG4" s="61"/>
+      <c r="BH4" s="61"/>
+    </row>
+    <row r="5" spans="2:60" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1281,34 +1292,34 @@
       <c r="AH5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AI5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="29" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="34" t="s">
+      <c r="AK5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL5" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM5" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="AL5" s="35"/>
-      <c r="AM5" s="56" t="s">
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="55" t="s">
+      <c r="AP5" s="64"/>
+      <c r="AQ5" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="AP5" s="55"/>
-      <c r="AQ5" s="6" t="s">
+      <c r="AR5" s="62"/>
+      <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AR5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AT5" s="7" t="s">
+      <c r="AT5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="AU5" s="7" t="s">
@@ -1323,24 +1334,30 @@
       <c r="AX5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BB5" s="38" t="s">
+      <c r="AY5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BC5" s="54" t="s">
+      <c r="BE5" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="BD5" s="54"/>
-      <c r="BE5" s="54"/>
-      <c r="BF5" s="54"/>
-    </row>
-    <row r="6" spans="2:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BF5" s="61"/>
+      <c r="BG5" s="61"/>
+      <c r="BH5" s="61"/>
+    </row>
+    <row r="6" spans="2:60" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="53" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1389,72 +1406,78 @@
         <v>37</v>
       </c>
       <c r="AH6" s="12">
-        <v>10500</v>
-      </c>
-      <c r="AI6" t="s">
+        <v>10100</v>
+      </c>
+      <c r="AI6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ6" s="9">
+        <v>10200</v>
+      </c>
+      <c r="AK6" t="s">
         <v>39</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>12000</v>
-      </c>
-      <c r="AK6" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL6" s="37">
-        <v>400</v>
       </c>
       <c r="AM6" s="36" t="s">
         <v>20</v>
       </c>
       <c r="AN6" s="37">
+        <v>400</v>
+      </c>
+      <c r="AO6" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP6" s="37">
         <v>1100</v>
       </c>
-      <c r="AO6" s="17" t="s">
+      <c r="AQ6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AP6" s="20">
+      <c r="AR6" s="20">
         <v>1700</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AT6" s="9">
+      <c r="AV6" s="9">
         <v>11000</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AV6" s="9">
+      <c r="AX6" s="9">
         <v>13000</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AX6" s="9">
+      <c r="AZ6" s="9">
         <v>14000</v>
       </c>
-      <c r="BC6" s="39" t="s">
+      <c r="BE6" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="BD6" s="39" t="s">
+      <c r="BF6" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="BE6" s="31" t="s">
+      <c r="BG6" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="BF6" s="31" t="s">
+      <c r="BH6" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="2:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:60" x14ac:dyDescent="0.4">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="60"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="54"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1479,42 +1502,44 @@
         <v>38</v>
       </c>
       <c r="AH7" s="14">
-        <v>10600</v>
-      </c>
-      <c r="AK7" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL7" s="37">
-        <v>401</v>
-      </c>
+        <v>10150</v>
+      </c>
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="17"/>
       <c r="AM7" s="36" t="s">
         <v>19</v>
       </c>
       <c r="AN7" s="37">
+        <v>401</v>
+      </c>
+      <c r="AO7" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP7" s="37">
         <v>1102</v>
       </c>
-      <c r="AO7" s="17" t="s">
+      <c r="AQ7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AP7" s="20">
+      <c r="AR7" s="20">
         <v>1701</v>
       </c>
-      <c r="BC7" s="36" t="s">
+      <c r="BE7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="BD7" s="37">
+      <c r="BF7" s="37">
         <v>1100</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:60" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="60"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="54"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1527,34 +1552,34 @@
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AK8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL8" s="37">
-        <v>500</v>
-      </c>
       <c r="AM8" s="36" t="s">
         <v>21</v>
       </c>
       <c r="AN8" s="37">
+        <v>500</v>
+      </c>
+      <c r="AO8" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP8" s="37">
         <v>1200</v>
       </c>
-      <c r="AO8" s="17" t="s">
+      <c r="AQ8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>1800</v>
       </c>
-      <c r="BC8" s="36" t="s">
+      <c r="BE8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="BD8" s="37">
+      <c r="BF8" s="37">
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I9" s="58"/>
-      <c r="J9" s="60"/>
+    <row r="9" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I9" s="52"/>
+      <c r="J9" s="54"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1567,451 +1592,464 @@
       <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AK9" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL9" s="37">
-        <v>501</v>
-      </c>
       <c r="AM9" s="36" t="s">
         <v>22</v>
       </c>
       <c r="AN9" s="37">
+        <v>501</v>
+      </c>
+      <c r="AO9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP9" s="37">
         <v>1201</v>
       </c>
-      <c r="AO9" s="17" t="s">
+      <c r="AQ9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>1801</v>
       </c>
-      <c r="BC9" s="36" t="s">
+      <c r="BE9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="BD9" s="37">
+      <c r="BF9" s="37">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I10" s="58"/>
+    <row r="10" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I10" s="52"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="4">
         <v>6004</v>
       </c>
-      <c r="AK10" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL10" s="37">
-        <v>600</v>
-      </c>
       <c r="AM10" s="36" t="s">
         <v>23</v>
       </c>
       <c r="AN10" s="37">
+        <v>600</v>
+      </c>
+      <c r="AO10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP10" s="37">
         <v>1300</v>
       </c>
-      <c r="AO10" s="17" t="s">
+      <c r="AQ10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="AP10">
+      <c r="AR10">
         <v>1900</v>
       </c>
-      <c r="BC10" s="36" t="s">
+      <c r="BE10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="BD10" s="37">
+      <c r="BF10" s="37">
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I11" s="58"/>
-      <c r="AK11" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL11" s="37">
-        <v>601</v>
-      </c>
+    <row r="11" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I11" s="52"/>
       <c r="AM11" s="36" t="s">
         <v>24</v>
       </c>
       <c r="AN11" s="37">
+        <v>601</v>
+      </c>
+      <c r="AO11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP11" s="37">
         <v>1301</v>
       </c>
-      <c r="AO11" s="17" t="s">
+      <c r="AQ11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="AP11">
+      <c r="AR11">
         <v>1901</v>
       </c>
-      <c r="AR11" s="19"/>
-      <c r="AS11" s="19"/>
-      <c r="BC11" s="36" t="s">
+      <c r="AT11" s="19"/>
+      <c r="AU11" s="19"/>
+      <c r="BE11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="BD11" s="37">
+      <c r="BF11" s="37">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I12" s="58"/>
-      <c r="AK12" s="36" t="s">
+    <row r="12" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I12" s="52"/>
+      <c r="AM12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AL12" s="37">
+      <c r="AN12" s="37">
         <v>700</v>
       </c>
-      <c r="AM12" s="36" t="s">
+      <c r="AO12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AN12" s="37">
+      <c r="AP12" s="37">
         <v>1400</v>
       </c>
-      <c r="AO12" s="17" t="s">
+      <c r="AQ12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="AP12">
+      <c r="AR12">
         <v>2000</v>
       </c>
-      <c r="AR12" s="22"/>
-      <c r="AS12" s="22"/>
-      <c r="BC12" s="36" t="s">
+      <c r="AT12" s="22"/>
+      <c r="AU12" s="22"/>
+      <c r="BE12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="BD12" s="37">
+      <c r="BF12" s="37">
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I13" s="58"/>
-      <c r="AK13" s="36" t="s">
+    <row r="13" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I13" s="52"/>
+      <c r="AM13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AL13" s="37">
+      <c r="AN13" s="37">
         <v>701</v>
       </c>
-      <c r="AM13" s="36" t="s">
+      <c r="AO13" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AN13" s="37">
+      <c r="AP13" s="37">
         <v>1401</v>
       </c>
-      <c r="AO13" s="17" t="s">
+      <c r="AQ13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AP13">
+      <c r="AR13">
         <v>2001</v>
       </c>
-      <c r="AR13" s="17"/>
-      <c r="AS13" s="17"/>
-      <c r="BC13" s="36" t="s">
+      <c r="AT13" s="17"/>
+      <c r="AU13" s="17"/>
+      <c r="BE13" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="BD13" s="37">
+      <c r="BF13" s="37">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I14" s="58"/>
-      <c r="AK14" s="36" t="s">
+    <row r="14" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I14" s="52"/>
+      <c r="AM14" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AL14" s="37">
+      <c r="AN14" s="37">
         <v>800</v>
       </c>
-      <c r="AM14" s="36" t="s">
+      <c r="AO14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AN14" s="37">
+      <c r="AP14" s="37">
         <v>1500</v>
       </c>
-      <c r="AO14" s="17" t="s">
+      <c r="AQ14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AP14">
+      <c r="AR14">
         <v>2100</v>
       </c>
-      <c r="BC14" s="36" t="s">
+      <c r="BE14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BD14" s="37">
+      <c r="BF14" s="37">
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I15" s="58"/>
-      <c r="AK15" s="36" t="s">
+    <row r="15" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I15" s="52"/>
+      <c r="AM15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AL15" s="37">
+      <c r="AN15" s="37">
         <v>801</v>
       </c>
-      <c r="AM15" s="36" t="s">
+      <c r="AO15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AN15" s="37">
+      <c r="AP15" s="37">
         <v>1501</v>
       </c>
-      <c r="AO15" s="17" t="s">
+      <c r="AQ15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AP15">
+      <c r="AR15">
         <v>2101</v>
       </c>
-      <c r="BC15" s="36" t="s">
+      <c r="BE15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="BD15" s="37">
+      <c r="BF15" s="37">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:58" x14ac:dyDescent="0.3">
-      <c r="I16" s="58"/>
-      <c r="AK16" s="36" t="s">
+    <row r="16" spans="2:60" x14ac:dyDescent="0.4">
+      <c r="I16" s="52"/>
+      <c r="AM16" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="AL16" s="37">
+      <c r="AN16" s="37">
         <v>900</v>
       </c>
-      <c r="AM16" s="36" t="s">
+      <c r="AO16" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AN16" s="37">
+      <c r="AP16" s="37">
         <v>1600</v>
       </c>
-      <c r="AO16" s="17" t="s">
+      <c r="AQ16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AP16">
+      <c r="AR16">
         <v>2200</v>
       </c>
-      <c r="BC16" s="36" t="s">
+      <c r="BE16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="BD16" s="37">
+      <c r="BF16" s="37">
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I17" s="58"/>
+    <row r="17" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="I17" s="52"/>
       <c r="AG17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="AH17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AK17" s="36" t="s">
+      <c r="AI17" s="48"/>
+      <c r="AJ17" s="48"/>
+      <c r="AM17" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="AL17" s="37">
+      <c r="AN17" s="37">
         <v>901</v>
       </c>
-      <c r="AM17" s="36" t="s">
+      <c r="AO17" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AN17" s="37">
+      <c r="AP17" s="37">
         <v>1601</v>
       </c>
-      <c r="AO17" s="17" t="s">
+      <c r="AQ17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AP17">
+      <c r="AR17">
         <v>2201</v>
       </c>
-      <c r="BC17" s="36" t="s">
+      <c r="BE17" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="BD17" s="37">
+      <c r="BF17" s="37">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I18" s="58"/>
-      <c r="AK18" s="36" t="s">
+    <row r="18" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="I18" s="52"/>
+      <c r="AM18" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AL18" s="37">
+      <c r="AN18" s="37">
         <v>1000</v>
       </c>
-      <c r="AM18" s="13"/>
-      <c r="AN18" s="14"/>
-      <c r="AO18" s="17" t="s">
+      <c r="AO18" s="13"/>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AP18">
+      <c r="AR18">
         <v>2300</v>
       </c>
-      <c r="BC18" s="36" t="s">
+      <c r="BE18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="BD18" s="37">
+      <c r="BF18" s="37">
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I19" s="58"/>
-      <c r="AK19" s="36" t="s">
+    <row r="19" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="I19" s="52"/>
+      <c r="AM19" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AL19" s="37">
+      <c r="AN19" s="37">
         <v>1001</v>
       </c>
-      <c r="AM19" s="17"/>
-      <c r="AN19" s="17"/>
-      <c r="AO19" s="10" t="s">
+      <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
+      <c r="AQ19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AP19">
+      <c r="AR19">
         <v>2301</v>
       </c>
     </row>
-    <row r="20" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I20" s="58"/>
-      <c r="AK20" s="13" t="s">
+    <row r="20" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="I20" s="52"/>
+      <c r="AM20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AL20" s="14">
+      <c r="AN20" s="14">
         <v>999</v>
       </c>
-      <c r="AM20" s="17"/>
-      <c r="AN20" s="17"/>
-      <c r="AO20" s="20" t="s">
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="AP20" s="17">
+      <c r="AR20" s="17">
         <v>2400</v>
       </c>
     </row>
-    <row r="21" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="I21" s="58"/>
-      <c r="AM21" s="17"/>
-      <c r="AN21" s="17"/>
-      <c r="AO21" s="20" t="s">
+    <row r="21" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="I21" s="52"/>
+      <c r="AO21" s="17"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="AP21" s="20">
+      <c r="AR21" s="20">
         <v>2401</v>
       </c>
     </row>
-    <row r="22" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM22" s="33"/>
-      <c r="AN22" s="33"/>
-      <c r="AO22" s="64" t="s">
+    <row r="22" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="AO22" s="33"/>
+      <c r="AP22" s="33"/>
+      <c r="AQ22" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="AP22" s="65">
+      <c r="AR22" s="50">
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM23" s="17"/>
-      <c r="AN23" s="17"/>
-      <c r="AO23" s="20" t="s">
+    <row r="23" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="AO23" s="17"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="AP23" s="20">
+      <c r="AR23" s="20">
         <v>2501</v>
       </c>
     </row>
-    <row r="24" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM24" s="17"/>
-      <c r="AN24" s="17"/>
-      <c r="AO24" s="20" t="s">
+    <row r="24" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="AO24" s="17"/>
+      <c r="AP24" s="17"/>
+      <c r="AQ24" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="AP24" s="20">
+      <c r="AR24" s="20">
         <v>2600</v>
       </c>
     </row>
-    <row r="25" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM25" s="17"/>
-      <c r="AN25" s="17"/>
-      <c r="AO25" s="20" t="s">
+    <row r="25" spans="9:58" x14ac:dyDescent="0.4">
+      <c r="AO25" s="17"/>
+      <c r="AP25" s="17"/>
+      <c r="AQ25" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="AP25" s="20">
+      <c r="AR25" s="20">
         <v>2601</v>
       </c>
     </row>
-    <row r="26" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM26" s="17"/>
-      <c r="AN26" s="17"/>
+    <row r="26" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO26" s="17"/>
       <c r="AP26" s="17"/>
-    </row>
-    <row r="27" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM27" s="17"/>
-      <c r="AN27" s="17"/>
+      <c r="AQ26" s="17"/>
+      <c r="AR26" s="17"/>
+    </row>
+    <row r="27" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO27" s="17"/>
       <c r="AP27" s="17"/>
-    </row>
-    <row r="28" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM28" s="17"/>
-      <c r="AN28" s="17"/>
+      <c r="AQ27" s="17"/>
+      <c r="AR27" s="17"/>
+    </row>
+    <row r="28" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO28" s="17"/>
       <c r="AP28" s="17"/>
-    </row>
-    <row r="29" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM29" s="17"/>
-      <c r="AN29" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+    </row>
+    <row r="29" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO29" s="17"/>
       <c r="AP29" s="17"/>
-    </row>
-    <row r="30" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM30" s="17"/>
-      <c r="AN30" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="17"/>
+    </row>
+    <row r="30" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO30" s="17"/>
       <c r="AP30" s="17"/>
-    </row>
-    <row r="31" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM31" s="17"/>
-      <c r="AN31" s="17"/>
+      <c r="AQ30" s="17"/>
+      <c r="AR30" s="17"/>
+    </row>
+    <row r="31" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO31" s="17"/>
       <c r="AP31" s="17"/>
-    </row>
-    <row r="32" spans="9:56" x14ac:dyDescent="0.3">
-      <c r="AM32" s="17"/>
-      <c r="AN32" s="17"/>
+      <c r="AQ31" s="17"/>
+      <c r="AR31" s="17"/>
+    </row>
+    <row r="32" spans="9:58" x14ac:dyDescent="0.4">
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
-    </row>
-    <row r="33" spans="39:42" x14ac:dyDescent="0.3">
-      <c r="AM33" s="17"/>
-      <c r="AN33" s="17"/>
+      <c r="AQ32" s="17"/>
+      <c r="AR32" s="17"/>
+    </row>
+    <row r="33" spans="41:44" x14ac:dyDescent="0.4">
       <c r="AO33" s="17"/>
       <c r="AP33" s="17"/>
-    </row>
-    <row r="34" spans="39:42" x14ac:dyDescent="0.3">
-      <c r="AM34" s="17"/>
-      <c r="AN34" s="17"/>
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+    </row>
+    <row r="34" spans="41:44" x14ac:dyDescent="0.4">
       <c r="AO34" s="17"/>
       <c r="AP34" s="17"/>
-    </row>
-    <row r="35" spans="39:42" x14ac:dyDescent="0.3">
-      <c r="AM35" s="32"/>
-      <c r="AN35" s="32"/>
+      <c r="AQ34" s="17"/>
+      <c r="AR34" s="17"/>
+    </row>
+    <row r="35" spans="41:44" x14ac:dyDescent="0.4">
       <c r="AO35" s="32"/>
       <c r="AP35" s="32"/>
-    </row>
-    <row r="36" spans="39:42" x14ac:dyDescent="0.3">
-      <c r="AM36" s="20"/>
-      <c r="AN36" s="20"/>
+      <c r="AQ35" s="32"/>
+      <c r="AR35" s="32"/>
+    </row>
+    <row r="36" spans="41:44" x14ac:dyDescent="0.4">
       <c r="AO36" s="20"/>
       <c r="AP36" s="20"/>
-    </row>
-    <row r="37" spans="39:42" x14ac:dyDescent="0.3">
-      <c r="AM37" s="20"/>
-      <c r="AN37" s="20"/>
+      <c r="AQ36" s="20"/>
+      <c r="AR36" s="20"/>
+    </row>
+    <row r="37" spans="41:44" x14ac:dyDescent="0.4">
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
+      <c r="AQ37" s="20"/>
+      <c r="AR37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="BE4:BH4"/>
+    <mergeCell ref="BE5:BH5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="K4:L4"/>
@@ -2020,16 +2058,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AK4:AP4"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BF5"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2044,35 +2072,35 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.69140625" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
+    <col min="7" max="7" width="16.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B2" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2095,7 +2123,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -2116,7 +2144,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -2135,7 +2163,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -2154,7 +2182,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A8" s="42">
         <v>4</v>
       </c>
@@ -2177,7 +2205,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -2198,7 +2226,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="46">
         <v>6</v>
       </c>
@@ -2216,73 +2244,73 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -2306,26 +2334,26 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="23.69140625" customWidth="1"/>
+    <col min="4" max="4" width="56.23046875" customWidth="1"/>
+    <col min="5" max="5" width="12.23046875" customWidth="1"/>
+    <col min="6" max="6" width="15.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="63" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B4" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
@@ -2339,7 +2367,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -2351,7 +2379,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -2363,7 +2391,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="D8" s="24" t="s">
         <v>90</v>
       </c>
@@ -2384,19 +2412,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.21875" style="40"/>
-    <col min="3" max="3" width="40.88671875" customWidth="1"/>
-    <col min="4" max="4" width="55.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.23046875" style="40"/>
+    <col min="3" max="3" width="40.84375" customWidth="1"/>
+    <col min="4" max="4" width="55.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
@@ -2407,7 +2435,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B5" s="45">
         <v>1</v>
       </c>
@@ -2418,7 +2446,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="45">
         <v>2</v>
       </c>
@@ -2429,47 +2457,47 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B7" s="45"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="45"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B9" s="45"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B10" s="45"/>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="45"/>
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B12" s="45"/>
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B13" s="45"/>
       <c r="C13" s="44"/>
       <c r="D13" s="44"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B14" s="45"/>
       <c r="C14" s="44"/>
       <c r="D14" s="44"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B15" s="45"/>
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>

</xml_diff>

<commit_message>
Create basic Hidden Coin Area scene for scece 1-1
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A264686-D0BD-4F53-90C7-802D28743D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F5732-0233-4259-871F-9780D3B18BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -1095,7 +1095,7 @@
   <dimension ref="B4:BH37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20:AI21"/>
+      <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1820,12 +1820,8 @@
     </row>
     <row r="17" spans="9:58" x14ac:dyDescent="0.4">
       <c r="I17" s="52"/>
-      <c r="AG17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH17" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="AG17" s="48"/>
+      <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
       <c r="AJ17" s="48"/>
       <c r="AM17" s="36" t="s">

</xml_diff>

<commit_message>
Create PipeGate class to help Mario teleports between different location
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F5732-0233-4259-871F-9780D3B18BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFF8577-579F-4B92-90A1-AB9025114DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -385,6 +385,24 @@
   </si>
   <si>
     <t>Breakable Brick</t>
+  </si>
+  <si>
+    <r>
+      <t>Pipe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HiddenZone</t>
+    </r>
+  </si>
+  <si>
+    <t>PipeHZ Green</t>
   </si>
 </sst>
 </file>
@@ -730,9 +748,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,33 +788,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1092,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BH37"/>
+  <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BB13" sqref="BB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1120,14 +1138,16 @@
     <col min="49" max="49" width="10.84375" customWidth="1"/>
     <col min="51" max="51" width="9.765625" customWidth="1"/>
     <col min="52" max="52" width="8.4609375" customWidth="1"/>
-    <col min="53" max="53" width="5.69140625" customWidth="1"/>
-    <col min="54" max="55" width="7.765625" customWidth="1"/>
-    <col min="56" max="56" width="11.69140625" customWidth="1"/>
-    <col min="57" max="58" width="13.4609375" customWidth="1"/>
-    <col min="59" max="59" width="13.07421875" customWidth="1"/>
+    <col min="53" max="53" width="12.07421875" customWidth="1"/>
+    <col min="54" max="54" width="8.4609375" customWidth="1"/>
+    <col min="55" max="55" width="5.69140625" customWidth="1"/>
+    <col min="56" max="57" width="7.765625" customWidth="1"/>
+    <col min="58" max="58" width="11.69140625" customWidth="1"/>
+    <col min="59" max="60" width="13.4609375" customWidth="1"/>
+    <col min="61" max="61" width="13.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:60" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:62" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1138,92 +1158,96 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58" t="s">
+      <c r="L4" s="64"/>
+      <c r="M4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="58"/>
+      <c r="N4" s="64"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="55" t="s">
+      <c r="S4" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55" t="s">
+      <c r="T4" s="53"/>
+      <c r="U4" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55" t="s">
+      <c r="V4" s="53"/>
+      <c r="W4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55" t="s">
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="56" t="s">
+      <c r="Z4" s="53"/>
+      <c r="AA4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="56" t="s">
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="56" t="s">
+      <c r="AD4" s="52"/>
+      <c r="AE4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="56" t="s">
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="56" t="s">
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="56" t="s">
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="59" t="s">
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="51"/>
-      <c r="AO4" s="60"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="57"/>
-      <c r="AS4" s="56" t="s">
+      <c r="AN4" s="55"/>
+      <c r="AO4" s="56"/>
+      <c r="AP4" s="56"/>
+      <c r="AQ4" s="56"/>
+      <c r="AR4" s="52"/>
+      <c r="AS4" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="56" t="s">
+      <c r="AT4" s="52"/>
+      <c r="AU4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="57"/>
-      <c r="AW4" s="56" t="s">
+      <c r="AV4" s="52"/>
+      <c r="AW4" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="56" t="s">
+      <c r="AX4" s="52"/>
+      <c r="AY4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="57"/>
-      <c r="BD4" s="38" t="s">
+      <c r="AZ4" s="52"/>
+      <c r="BA4" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="BB4" s="52"/>
+      <c r="BF4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BE4" s="61" t="s">
+      <c r="BG4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="BF4" s="61"/>
-      <c r="BG4" s="61"/>
-      <c r="BH4" s="61"/>
-    </row>
-    <row r="5" spans="2:60" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BH4" s="57"/>
+      <c r="BI4" s="57"/>
+      <c r="BJ4" s="57"/>
+    </row>
+    <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1308,14 +1332,14 @@
         <v>33</v>
       </c>
       <c r="AN5" s="35"/>
-      <c r="AO5" s="63" t="s">
+      <c r="AO5" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="64"/>
-      <c r="AQ5" s="62" t="s">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="AR5" s="62"/>
+      <c r="AR5" s="58"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1340,24 +1364,30 @@
       <c r="AZ5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BD5" s="38" t="s">
+      <c r="BA5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BF5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BE5" s="61" t="s">
+      <c r="BG5" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="61"/>
-    </row>
-    <row r="6" spans="2:60" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BH5" s="57"/>
+      <c r="BI5" s="57"/>
+      <c r="BJ5" s="57"/>
+    </row>
+    <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="62" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1456,28 +1486,34 @@
       <c r="AZ6" s="9">
         <v>14000</v>
       </c>
-      <c r="BE6" s="39" t="s">
+      <c r="BA6" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB6" s="9">
+        <v>14010</v>
+      </c>
+      <c r="BG6" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="BF6" s="39" t="s">
+      <c r="BH6" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="BG6" s="31" t="s">
+      <c r="BI6" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="BH6" s="31" t="s">
+      <c r="BJ6" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="2:60" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="54"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="63"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1524,22 +1560,23 @@
       <c r="AR7" s="20">
         <v>1701</v>
       </c>
-      <c r="BE7" s="36" t="s">
+      <c r="BA7" s="9"/>
+      <c r="BG7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="BF7" s="37">
+      <c r="BH7" s="37">
         <v>1100</v>
       </c>
-      <c r="BG7">
+      <c r="BI7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:60" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:62" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="54"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="63"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1570,16 +1607,16 @@
       <c r="AR8">
         <v>1800</v>
       </c>
-      <c r="BE8" s="36" t="s">
+      <c r="BG8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="BF8" s="37">
+      <c r="BH8" s="37">
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I9" s="52"/>
-      <c r="J9" s="54"/>
+    <row r="9" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I9" s="61"/>
+      <c r="J9" s="63"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1610,15 +1647,15 @@
       <c r="AR9">
         <v>1801</v>
       </c>
-      <c r="BE9" s="36" t="s">
+      <c r="BG9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="BF9" s="37">
+      <c r="BH9" s="37">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I10" s="52"/>
+    <row r="10" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I10" s="61"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1643,15 +1680,15 @@
       <c r="AR10">
         <v>1900</v>
       </c>
-      <c r="BE10" s="36" t="s">
+      <c r="BG10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="BF10" s="37">
+      <c r="BH10" s="37">
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I11" s="52"/>
+    <row r="11" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I11" s="61"/>
       <c r="AM11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1672,15 +1709,15 @@
       </c>
       <c r="AT11" s="19"/>
       <c r="AU11" s="19"/>
-      <c r="BE11" s="36" t="s">
+      <c r="BG11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="BF11" s="37">
+      <c r="BH11" s="37">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I12" s="52"/>
+    <row r="12" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I12" s="61"/>
       <c r="AM12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1701,15 +1738,15 @@
       </c>
       <c r="AT12" s="22"/>
       <c r="AU12" s="22"/>
-      <c r="BE12" s="36" t="s">
+      <c r="BG12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="BF12" s="37">
+      <c r="BH12" s="37">
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I13" s="52"/>
+    <row r="13" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I13" s="61"/>
       <c r="AM13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1730,15 +1767,15 @@
       </c>
       <c r="AT13" s="17"/>
       <c r="AU13" s="17"/>
-      <c r="BE13" s="36" t="s">
+      <c r="BG13" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="BF13" s="37">
+      <c r="BH13" s="37">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I14" s="52"/>
+    <row r="14" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I14" s="61"/>
       <c r="AM14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1757,15 +1794,15 @@
       <c r="AR14">
         <v>2100</v>
       </c>
-      <c r="BE14" s="36" t="s">
+      <c r="BG14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BF14" s="37">
+      <c r="BH14" s="37">
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I15" s="52"/>
+    <row r="15" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I15" s="61"/>
       <c r="AM15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1784,15 +1821,15 @@
       <c r="AR15">
         <v>2101</v>
       </c>
-      <c r="BE15" s="36" t="s">
+      <c r="BG15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="BF15" s="37">
+      <c r="BH15" s="37">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:60" x14ac:dyDescent="0.4">
-      <c r="I16" s="52"/>
+    <row r="16" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I16" s="61"/>
       <c r="AM16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1811,15 +1848,15 @@
       <c r="AR16">
         <v>2200</v>
       </c>
-      <c r="BE16" s="36" t="s">
+      <c r="BG16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="BF16" s="37">
+      <c r="BH16" s="37">
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:58" x14ac:dyDescent="0.4">
-      <c r="I17" s="52"/>
+    <row r="17" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I17" s="61"/>
       <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
@@ -1842,15 +1879,15 @@
       <c r="AR17">
         <v>2201</v>
       </c>
-      <c r="BE17" s="36" t="s">
+      <c r="BG17" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="BF17" s="37">
+      <c r="BH17" s="37">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:58" x14ac:dyDescent="0.4">
-      <c r="I18" s="52"/>
+    <row r="18" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I18" s="61"/>
       <c r="AM18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1865,15 +1902,15 @@
       <c r="AR18">
         <v>2300</v>
       </c>
-      <c r="BE18" s="36" t="s">
+      <c r="BG18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="BF18" s="37">
+      <c r="BH18" s="37">
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:58" x14ac:dyDescent="0.4">
-      <c r="I19" s="52"/>
+    <row r="19" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I19" s="61"/>
       <c r="AM19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1889,8 +1926,8 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="20" spans="9:58" x14ac:dyDescent="0.4">
-      <c r="I20" s="52"/>
+    <row r="20" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I20" s="61"/>
       <c r="AM20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1906,8 +1943,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="21" spans="9:58" x14ac:dyDescent="0.4">
-      <c r="I21" s="52"/>
+    <row r="21" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I21" s="61"/>
       <c r="AO21" s="17"/>
       <c r="AP21" s="17"/>
       <c r="AQ21" s="20" t="s">
@@ -1917,7 +1954,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="22" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="22" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO22" s="33"/>
       <c r="AP22" s="33"/>
       <c r="AQ22" s="49" t="s">
@@ -1927,7 +1964,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="23" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO23" s="17"/>
       <c r="AP23" s="17"/>
       <c r="AQ23" s="20" t="s">
@@ -1937,7 +1974,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="24" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="24" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO24" s="17"/>
       <c r="AP24" s="17"/>
       <c r="AQ24" s="20" t="s">
@@ -1947,7 +1984,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="25" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="25" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO25" s="17"/>
       <c r="AP25" s="17"/>
       <c r="AQ25" s="20" t="s">
@@ -1957,43 +1994,43 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="26" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="26" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO26" s="17"/>
       <c r="AP26" s="17"/>
       <c r="AQ26" s="17"/>
       <c r="AR26" s="17"/>
     </row>
-    <row r="27" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="27" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO27" s="17"/>
       <c r="AP27" s="17"/>
       <c r="AQ27" s="17"/>
       <c r="AR27" s="17"/>
     </row>
-    <row r="28" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="28" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO28" s="17"/>
       <c r="AP28" s="17"/>
       <c r="AQ28" s="17"/>
       <c r="AR28" s="17"/>
     </row>
-    <row r="29" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="29" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO29" s="17"/>
       <c r="AP29" s="17"/>
       <c r="AQ29" s="17"/>
       <c r="AR29" s="17"/>
     </row>
-    <row r="30" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="30" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO30" s="17"/>
       <c r="AP30" s="17"/>
       <c r="AQ30" s="17"/>
       <c r="AR30" s="17"/>
     </row>
-    <row r="31" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="31" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO31" s="17"/>
       <c r="AP31" s="17"/>
       <c r="AQ31" s="17"/>
       <c r="AR31" s="17"/>
     </row>
-    <row r="32" spans="9:58" x14ac:dyDescent="0.4">
+    <row r="32" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
       <c r="AQ32" s="17"/>
@@ -2030,18 +2067,7 @@
       <c r="AR37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AR4"/>
-    <mergeCell ref="BE4:BH4"/>
-    <mergeCell ref="BE5:BH5"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AI4:AJ4"/>
+  <mergeCells count="24">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2054,6 +2080,18 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="BG4:BJ4"/>
+    <mergeCell ref="BG5:BJ5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BA4:BB4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2078,12 +2116,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" s="65" t="s">
@@ -2343,11 +2381,11 @@
       <c r="B4" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add animation Idle Hold Koopa for Big Mario. And cause damage for Mario when hold Koopa until it get out of its shell
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFF8577-579F-4B92-90A1-AB9025114DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82D37D9-39CF-489B-975F-59F618D6CBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="121">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -403,6 +403,15 @@
   </si>
   <si>
     <t>PipeHZ Green</t>
+  </si>
+  <si>
+    <t>Jump Walk + Run Right</t>
+  </si>
+  <si>
+    <t>Jump Walk + Run Left</t>
+  </si>
+  <si>
+    <t>Mario Big Hold Koopa</t>
   </si>
 </sst>
 </file>
@@ -640,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -748,6 +757,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,14 +779,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -779,23 +800,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="BB13" sqref="BB13"/>
+    <sheetView tabSelected="1" topLeftCell="AG16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AQ27" sqref="AQ27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1130,7 +1141,7 @@
     <col min="33" max="33" width="15.84375" customWidth="1"/>
     <col min="35" max="35" width="13.07421875" customWidth="1"/>
     <col min="37" max="37" width="10.4609375" customWidth="1"/>
-    <col min="39" max="39" width="15.3046875" customWidth="1"/>
+    <col min="39" max="39" width="19.3828125" customWidth="1"/>
     <col min="40" max="40" width="9.23046875" customWidth="1"/>
     <col min="41" max="41" width="14.07421875" customWidth="1"/>
     <col min="43" max="43" width="14.84375" customWidth="1"/>
@@ -1158,94 +1169,94 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="64" t="s">
+      <c r="K4" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64" t="s">
+      <c r="L4" s="58"/>
+      <c r="M4" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="64"/>
+      <c r="N4" s="58"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53" t="s">
+      <c r="T4" s="55"/>
+      <c r="U4" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53" t="s">
+      <c r="V4" s="55"/>
+      <c r="W4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="53" t="s">
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="53"/>
-      <c r="AA4" s="51" t="s">
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="51" t="s">
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="51" t="s">
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="51" t="s">
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="51" t="s">
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="51" t="s">
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="54" t="s">
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="55"/>
-      <c r="AO4" s="56"/>
-      <c r="AP4" s="56"/>
-      <c r="AQ4" s="56"/>
-      <c r="AR4" s="52"/>
-      <c r="AS4" s="51" t="s">
+      <c r="AN4" s="51"/>
+      <c r="AO4" s="60"/>
+      <c r="AP4" s="60"/>
+      <c r="AQ4" s="60"/>
+      <c r="AR4" s="57"/>
+      <c r="AS4" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="52"/>
-      <c r="AU4" s="51" t="s">
+      <c r="AT4" s="57"/>
+      <c r="AU4" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="52"/>
-      <c r="AW4" s="51" t="s">
+      <c r="AV4" s="57"/>
+      <c r="AW4" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="AX4" s="52"/>
-      <c r="AY4" s="51" t="s">
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="52"/>
-      <c r="BA4" s="51" t="s">
+      <c r="AZ4" s="57"/>
+      <c r="BA4" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="BB4" s="52"/>
+      <c r="BB4" s="57"/>
       <c r="BF4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="BG4" s="57" t="s">
+      <c r="BG4" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="BH4" s="57"/>
-      <c r="BI4" s="57"/>
-      <c r="BJ4" s="57"/>
+      <c r="BH4" s="61"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
     </row>
     <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1332,14 +1343,14 @@
         <v>33</v>
       </c>
       <c r="AN5" s="35"/>
-      <c r="AO5" s="59" t="s">
+      <c r="AO5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="58" t="s">
+      <c r="AP5" s="64"/>
+      <c r="AQ5" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="AR5" s="58"/>
+      <c r="AR5" s="62"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1373,21 +1384,21 @@
       <c r="BF5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BG5" s="57" t="s">
+      <c r="BG5" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="BH5" s="57"/>
-      <c r="BI5" s="57"/>
-      <c r="BJ5" s="57"/>
+      <c r="BH5" s="61"/>
+      <c r="BI5" s="61"/>
+      <c r="BJ5" s="61"/>
     </row>
     <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="53" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1512,8 +1523,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="63"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="54"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1575,8 +1586,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="61"/>
-      <c r="J8" s="63"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="54"/>
       <c r="S8" s="28" t="s">
         <v>56</v>
       </c>
@@ -1615,8 +1626,8 @@
       </c>
     </row>
     <row r="9" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I9" s="61"/>
-      <c r="J9" s="63"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="54"/>
       <c r="S9" s="28" t="s">
         <v>57</v>
       </c>
@@ -1655,7 +1666,7 @@
       </c>
     </row>
     <row r="10" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I10" s="61"/>
+      <c r="I10" s="52"/>
       <c r="S10" s="28" t="s">
         <v>58</v>
       </c>
@@ -1688,7 +1699,7 @@
       </c>
     </row>
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I11" s="61"/>
+      <c r="I11" s="52"/>
       <c r="AM11" s="36" t="s">
         <v>24</v>
       </c>
@@ -1717,7 +1728,7 @@
       </c>
     </row>
     <row r="12" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I12" s="61"/>
+      <c r="I12" s="52"/>
       <c r="AM12" s="36" t="s">
         <v>25</v>
       </c>
@@ -1746,7 +1757,7 @@
       </c>
     </row>
     <row r="13" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I13" s="61"/>
+      <c r="I13" s="52"/>
       <c r="AM13" s="36" t="s">
         <v>26</v>
       </c>
@@ -1775,7 +1786,7 @@
       </c>
     </row>
     <row r="14" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I14" s="61"/>
+      <c r="I14" s="52"/>
       <c r="AM14" s="36" t="s">
         <v>27</v>
       </c>
@@ -1802,7 +1813,7 @@
       </c>
     </row>
     <row r="15" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I15" s="61"/>
+      <c r="I15" s="52"/>
       <c r="AM15" s="36" t="s">
         <v>28</v>
       </c>
@@ -1829,7 +1840,7 @@
       </c>
     </row>
     <row r="16" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I16" s="61"/>
+      <c r="I16" s="52"/>
       <c r="AM16" s="36" t="s">
         <v>29</v>
       </c>
@@ -1856,7 +1867,7 @@
       </c>
     </row>
     <row r="17" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I17" s="61"/>
+      <c r="I17" s="52"/>
       <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
@@ -1887,7 +1898,7 @@
       </c>
     </row>
     <row r="18" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I18" s="61"/>
+      <c r="I18" s="52"/>
       <c r="AM18" s="36" t="s">
         <v>31</v>
       </c>
@@ -1910,7 +1921,7 @@
       </c>
     </row>
     <row r="19" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I19" s="61"/>
+      <c r="I19" s="52"/>
       <c r="AM19" s="36" t="s">
         <v>32</v>
       </c>
@@ -1927,7 +1938,7 @@
       </c>
     </row>
     <row r="20" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I20" s="61"/>
+      <c r="I20" s="52"/>
       <c r="AM20" s="13" t="s">
         <v>14</v>
       </c>
@@ -1944,7 +1955,9 @@
       </c>
     </row>
     <row r="21" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I21" s="61"/>
+      <c r="I21" s="52"/>
+      <c r="AM21" s="67"/>
+      <c r="AN21" s="68"/>
       <c r="AO21" s="17"/>
       <c r="AP21" s="17"/>
       <c r="AQ21" s="20" t="s">
@@ -1955,6 +1968,10 @@
       </c>
     </row>
     <row r="22" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM22" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN22" s="61"/>
       <c r="AO22" s="33"/>
       <c r="AP22" s="33"/>
       <c r="AQ22" s="49" t="s">
@@ -1965,6 +1982,12 @@
       </c>
     </row>
     <row r="23" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM23" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN23" s="68">
+        <v>1010</v>
+      </c>
       <c r="AO23" s="17"/>
       <c r="AP23" s="17"/>
       <c r="AQ23" s="20" t="s">
@@ -1975,6 +1998,12 @@
       </c>
     </row>
     <row r="24" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM24" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN24" s="68">
+        <v>1011</v>
+      </c>
       <c r="AO24" s="17"/>
       <c r="AP24" s="17"/>
       <c r="AQ24" s="20" t="s">
@@ -2001,73 +2030,138 @@
       <c r="AR26" s="17"/>
     </row>
     <row r="27" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM27" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN27" s="37">
+        <v>500</v>
+      </c>
       <c r="AO27" s="17"/>
       <c r="AP27" s="17"/>
       <c r="AQ27" s="17"/>
       <c r="AR27" s="17"/>
     </row>
     <row r="28" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM28" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN28" s="37">
+        <v>501</v>
+      </c>
       <c r="AO28" s="17"/>
       <c r="AP28" s="17"/>
       <c r="AQ28" s="17"/>
       <c r="AR28" s="17"/>
     </row>
     <row r="29" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM29" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN29" s="37">
+        <v>600</v>
+      </c>
       <c r="AO29" s="17"/>
       <c r="AP29" s="17"/>
       <c r="AQ29" s="17"/>
       <c r="AR29" s="17"/>
     </row>
     <row r="30" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM30" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN30" s="37">
+        <v>601</v>
+      </c>
       <c r="AO30" s="17"/>
       <c r="AP30" s="17"/>
       <c r="AQ30" s="17"/>
       <c r="AR30" s="17"/>
     </row>
     <row r="31" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM31" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="AN31" s="37">
+        <v>700</v>
+      </c>
       <c r="AO31" s="17"/>
       <c r="AP31" s="17"/>
       <c r="AQ31" s="17"/>
       <c r="AR31" s="17"/>
     </row>
     <row r="32" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM32" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN32" s="37">
+        <v>701</v>
+      </c>
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
       <c r="AQ32" s="17"/>
       <c r="AR32" s="17"/>
     </row>
-    <row r="33" spans="41:44" x14ac:dyDescent="0.4">
+    <row r="33" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM33" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN33" s="37">
+        <v>800</v>
+      </c>
       <c r="AO33" s="17"/>
       <c r="AP33" s="17"/>
       <c r="AQ33" s="17"/>
       <c r="AR33" s="17"/>
     </row>
-    <row r="34" spans="41:44" x14ac:dyDescent="0.4">
+    <row r="34" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM34" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN34" s="37">
+        <v>801</v>
+      </c>
       <c r="AO34" s="17"/>
       <c r="AP34" s="17"/>
       <c r="AQ34" s="17"/>
       <c r="AR34" s="17"/>
     </row>
-    <row r="35" spans="41:44" x14ac:dyDescent="0.4">
+    <row r="35" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM35" s="36"/>
+      <c r="AN35" s="37"/>
       <c r="AO35" s="32"/>
       <c r="AP35" s="32"/>
       <c r="AQ35" s="32"/>
       <c r="AR35" s="32"/>
     </row>
-    <row r="36" spans="41:44" x14ac:dyDescent="0.4">
+    <row r="36" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM36" s="36"/>
+      <c r="AN36" s="37"/>
       <c r="AO36" s="20"/>
       <c r="AP36" s="20"/>
       <c r="AQ36" s="20"/>
       <c r="AR36" s="20"/>
     </row>
-    <row r="37" spans="41:44" x14ac:dyDescent="0.4">
+    <row r="37" spans="39:44" x14ac:dyDescent="0.4">
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
       <c r="AQ37" s="20"/>
       <c r="AR37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="BG4:BJ4"/>
+    <mergeCell ref="BG5:BJ5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BA4:BB4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2080,18 +2174,6 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AR4"/>
-    <mergeCell ref="BG4:BJ4"/>
-    <mergeCell ref="BG5:BJ5"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BA4:BB4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2116,12 +2198,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" s="65" t="s">
@@ -2381,11 +2463,11 @@
       <c r="B4" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add animation Go through Pipe for Big Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82D37D9-39CF-489B-975F-59F618D6CBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA54736-80AB-4E04-AAB6-01C94179AB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>Mario Big Hold Koopa</t>
+  </si>
+  <si>
+    <t>Thêm Animation cho Mario khi chui ống nữa</t>
+  </si>
+  <si>
+    <t>Go into + Get out of Pipe</t>
   </si>
 </sst>
 </file>
@@ -649,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -805,7 +811,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AQ27" sqref="AQ27"/>
+    <sheetView tabSelected="1" topLeftCell="AE3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1600,11 +1605,11 @@
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AM8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN8" s="37">
-        <v>500</v>
+      <c r="AM8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN8">
+        <v>410</v>
       </c>
       <c r="AO8" s="36" t="s">
         <v>21</v>
@@ -1641,10 +1646,10 @@
         <v>5530</v>
       </c>
       <c r="AM9" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AN9" s="37">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AO9" s="36" t="s">
         <v>22</v>
@@ -1674,10 +1679,10 @@
         <v>6004</v>
       </c>
       <c r="AM10" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AN10" s="37">
-        <v>600</v>
+        <v>501</v>
       </c>
       <c r="AO10" s="36" t="s">
         <v>23</v>
@@ -1701,10 +1706,10 @@
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I11" s="52"/>
       <c r="AM11" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AN11" s="37">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AO11" s="36" t="s">
         <v>24</v>
@@ -1730,10 +1735,10 @@
     <row r="12" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I12" s="52"/>
       <c r="AM12" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AN12" s="37">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="AO12" s="36" t="s">
         <v>31</v>
@@ -1759,10 +1764,10 @@
     <row r="13" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I13" s="52"/>
       <c r="AM13" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AN13" s="37">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AO13" s="36" t="s">
         <v>32</v>
@@ -1788,10 +1793,10 @@
     <row r="14" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I14" s="52"/>
       <c r="AM14" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AN14" s="37">
-        <v>800</v>
+        <v>701</v>
       </c>
       <c r="AO14" s="36" t="s">
         <v>25</v>
@@ -1815,10 +1820,10 @@
     <row r="15" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I15" s="52"/>
       <c r="AM15" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN15" s="37">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="AO15" s="36" t="s">
         <v>26</v>
@@ -1842,10 +1847,10 @@
     <row r="16" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I16" s="52"/>
       <c r="AM16" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AN16" s="37">
-        <v>900</v>
+        <v>801</v>
       </c>
       <c r="AO16" s="36" t="s">
         <v>27</v>
@@ -1873,10 +1878,10 @@
       <c r="AI17" s="48"/>
       <c r="AJ17" s="48"/>
       <c r="AM17" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AN17" s="37">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AO17" s="36" t="s">
         <v>28</v>
@@ -1900,10 +1905,10 @@
     <row r="18" spans="9:60" x14ac:dyDescent="0.4">
       <c r="I18" s="52"/>
       <c r="AM18" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AN18" s="37">
-        <v>1000</v>
+        <v>901</v>
       </c>
       <c r="AO18" s="13"/>
       <c r="AP18" s="14"/>
@@ -1923,10 +1928,10 @@
     <row r="19" spans="9:60" x14ac:dyDescent="0.4">
       <c r="I19" s="52"/>
       <c r="AM19" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AN19" s="37">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="AO19" s="17"/>
       <c r="AP19" s="17"/>
@@ -1939,11 +1944,11 @@
     </row>
     <row r="20" spans="9:60" x14ac:dyDescent="0.4">
       <c r="I20" s="52"/>
-      <c r="AM20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN20" s="14">
-        <v>999</v>
+      <c r="AM20" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN20" s="37">
+        <v>1001</v>
       </c>
       <c r="AO20" s="17"/>
       <c r="AP20" s="17"/>
@@ -1956,8 +1961,12 @@
     </row>
     <row r="21" spans="9:60" x14ac:dyDescent="0.4">
       <c r="I21" s="52"/>
-      <c r="AM21" s="67"/>
-      <c r="AN21" s="68"/>
+      <c r="AM21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN21" s="14">
+        <v>999</v>
+      </c>
       <c r="AO21" s="17"/>
       <c r="AP21" s="17"/>
       <c r="AQ21" s="20" t="s">
@@ -1968,10 +1977,6 @@
       </c>
     </row>
     <row r="22" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM22" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN22" s="61"/>
       <c r="AO22" s="33"/>
       <c r="AP22" s="33"/>
       <c r="AQ22" s="49" t="s">
@@ -1982,12 +1987,10 @@
       </c>
     </row>
     <row r="23" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM23" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN23" s="68">
-        <v>1010</v>
-      </c>
+      <c r="AM23" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN23" s="61"/>
       <c r="AO23" s="17"/>
       <c r="AP23" s="17"/>
       <c r="AQ23" s="20" t="s">
@@ -1999,10 +2002,10 @@
     </row>
     <row r="24" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM24" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN24" s="68">
-        <v>1011</v>
+        <v>20</v>
+      </c>
+      <c r="AN24" s="67">
+        <v>1010</v>
       </c>
       <c r="AO24" s="17"/>
       <c r="AP24" s="17"/>
@@ -2014,6 +2017,12 @@
       </c>
     </row>
     <row r="25" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM25" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN25" s="67">
+        <v>1011</v>
+      </c>
       <c r="AO25" s="17"/>
       <c r="AP25" s="17"/>
       <c r="AQ25" s="20" t="s">
@@ -2030,12 +2039,6 @@
       <c r="AR26" s="17"/>
     </row>
     <row r="27" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM27" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN27" s="37">
-        <v>500</v>
-      </c>
       <c r="AO27" s="17"/>
       <c r="AP27" s="17"/>
       <c r="AQ27" s="17"/>
@@ -2043,10 +2046,10 @@
     </row>
     <row r="28" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM28" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AN28" s="37">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AO28" s="17"/>
       <c r="AP28" s="17"/>
@@ -2055,10 +2058,10 @@
     </row>
     <row r="29" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM29" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AN29" s="37">
-        <v>600</v>
+        <v>501</v>
       </c>
       <c r="AO29" s="17"/>
       <c r="AP29" s="17"/>
@@ -2067,10 +2070,10 @@
     </row>
     <row r="30" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM30" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AN30" s="37">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AO30" s="17"/>
       <c r="AP30" s="17"/>
@@ -2079,10 +2082,10 @@
     </row>
     <row r="31" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM31" s="36" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="AN31" s="37">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="AO31" s="17"/>
       <c r="AP31" s="17"/>
@@ -2091,10 +2094,10 @@
     </row>
     <row r="32" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM32" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AN32" s="37">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
@@ -2103,10 +2106,10 @@
     </row>
     <row r="33" spans="39:44" x14ac:dyDescent="0.4">
       <c r="AM33" s="36" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="AN33" s="37">
-        <v>800</v>
+        <v>701</v>
       </c>
       <c r="AO33" s="17"/>
       <c r="AP33" s="17"/>
@@ -2115,10 +2118,10 @@
     </row>
     <row r="34" spans="39:44" x14ac:dyDescent="0.4">
       <c r="AM34" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN34" s="37">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="AO34" s="17"/>
       <c r="AP34" s="17"/>
@@ -2126,8 +2129,12 @@
       <c r="AR34" s="17"/>
     </row>
     <row r="35" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AM35" s="36"/>
-      <c r="AN35" s="37"/>
+      <c r="AM35" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN35" s="37">
+        <v>801</v>
+      </c>
       <c r="AO35" s="32"/>
       <c r="AP35" s="32"/>
       <c r="AQ35" s="32"/>
@@ -2137,7 +2144,9 @@
       <c r="AM36" s="36"/>
       <c r="AN36" s="37"/>
       <c r="AO36" s="20"/>
-      <c r="AP36" s="20"/>
+      <c r="AP36" s="20" t="s">
+        <v>121</v>
+      </c>
       <c r="AQ36" s="20"/>
       <c r="AR36" s="20"/>
     </row>
@@ -2149,7 +2158,7 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AM23:AN23"/>
     <mergeCell ref="AS4:AT4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="AM4:AR4"/>

</xml_diff>

<commit_message>
Add animation Go through Pipe for Small Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA54736-80AB-4E04-AAB6-01C94179AB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D092D7-003E-440F-81D8-FD8CBD9910B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -1129,7 +1129,7 @@
   <dimension ref="B4:BJ37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+      <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1146,9 +1146,9 @@
     <col min="33" max="33" width="15.84375" customWidth="1"/>
     <col min="35" max="35" width="13.07421875" customWidth="1"/>
     <col min="37" max="37" width="10.4609375" customWidth="1"/>
-    <col min="39" max="39" width="19.3828125" customWidth="1"/>
+    <col min="39" max="39" width="20.4609375" customWidth="1"/>
     <col min="40" max="40" width="9.23046875" customWidth="1"/>
-    <col min="41" max="41" width="14.07421875" customWidth="1"/>
+    <col min="41" max="41" width="20.4609375" customWidth="1"/>
     <col min="43" max="43" width="14.84375" customWidth="1"/>
     <col min="47" max="47" width="9.3046875" customWidth="1"/>
     <col min="49" max="49" width="10.84375" customWidth="1"/>
@@ -1611,11 +1611,11 @@
       <c r="AN8">
         <v>410</v>
       </c>
-      <c r="AO8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP8" s="37">
-        <v>1200</v>
+      <c r="AO8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="AP8">
+        <v>1110</v>
       </c>
       <c r="AQ8" s="17" t="s">
         <v>21</v>
@@ -1652,10 +1652,10 @@
         <v>500</v>
       </c>
       <c r="AO9" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AP9" s="37">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="AQ9" s="17" t="s">
         <v>22</v>
@@ -1685,10 +1685,10 @@
         <v>501</v>
       </c>
       <c r="AO10" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AP10" s="37">
-        <v>1300</v>
+        <v>1201</v>
       </c>
       <c r="AQ10" s="17" t="s">
         <v>23</v>
@@ -1712,10 +1712,10 @@
         <v>600</v>
       </c>
       <c r="AO11" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AP11" s="37">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="AQ11" s="17" t="s">
         <v>24</v>
@@ -1741,10 +1741,10 @@
         <v>601</v>
       </c>
       <c r="AO12" s="36" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="AP12" s="37">
-        <v>1400</v>
+        <v>1301</v>
       </c>
       <c r="AQ12" s="17" t="s">
         <v>25</v>
@@ -1770,10 +1770,10 @@
         <v>700</v>
       </c>
       <c r="AO13" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AP13" s="37">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="AQ13" s="17" t="s">
         <v>26</v>
@@ -1799,10 +1799,10 @@
         <v>701</v>
       </c>
       <c r="AO14" s="36" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AP14" s="37">
-        <v>1500</v>
+        <v>1401</v>
       </c>
       <c r="AQ14" s="17" t="s">
         <v>27</v>
@@ -1826,10 +1826,10 @@
         <v>800</v>
       </c>
       <c r="AO15" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AP15" s="37">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="AQ15" s="17" t="s">
         <v>28</v>
@@ -1853,10 +1853,10 @@
         <v>801</v>
       </c>
       <c r="AO16" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AP16" s="37">
-        <v>1600</v>
+        <v>1501</v>
       </c>
       <c r="AQ16" s="17" t="s">
         <v>29</v>
@@ -1884,10 +1884,10 @@
         <v>900</v>
       </c>
       <c r="AO17" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AP17" s="37">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="AQ17" s="17" t="s">
         <v>30</v>
@@ -1910,8 +1910,12 @@
       <c r="AN18" s="37">
         <v>901</v>
       </c>
-      <c r="AO18" s="13"/>
-      <c r="AP18" s="14"/>
+      <c r="AO18" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP18" s="37">
+        <v>1601</v>
+      </c>
       <c r="AQ18" s="17" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Add animation Go through Pipe for Raccoon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D092D7-003E-440F-81D8-FD8CBD9910B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D70BEE-FB7A-4ACB-92D0-459CB515880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="123">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -559,15 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -651,11 +642,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -676,7 +676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -720,14 +719,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -748,21 +741,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -787,31 +774,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+    <sheetView tabSelected="1" topLeftCell="AJ3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AT11" sqref="AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1149,7 +1149,7 @@
     <col min="39" max="39" width="20.4609375" customWidth="1"/>
     <col min="40" max="40" width="9.23046875" customWidth="1"/>
     <col min="41" max="41" width="20.4609375" customWidth="1"/>
-    <col min="43" max="43" width="14.84375" customWidth="1"/>
+    <col min="43" max="43" width="20.765625" customWidth="1"/>
     <col min="47" max="47" width="9.3046875" customWidth="1"/>
     <col min="49" max="49" width="10.84375" customWidth="1"/>
     <col min="51" max="51" width="9.765625" customWidth="1"/>
@@ -1172,103 +1172,103 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="58" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58" t="s">
+      <c r="L4" s="53"/>
+      <c r="M4" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="58"/>
+      <c r="N4" s="53"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="55" t="s">
+      <c r="S4" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55" t="s">
+      <c r="T4" s="50"/>
+      <c r="U4" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55" t="s">
+      <c r="V4" s="50"/>
+      <c r="W4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55" t="s">
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="56" t="s">
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="56" t="s">
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="56" t="s">
+      <c r="AD4" s="52"/>
+      <c r="AE4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="56" t="s">
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="56" t="s">
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="56" t="s">
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="59" t="s">
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="51"/>
-      <c r="AO4" s="60"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="57"/>
-      <c r="AS4" s="56" t="s">
+      <c r="AN4" s="46"/>
+      <c r="AO4" s="55"/>
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="55"/>
+      <c r="AR4" s="52"/>
+      <c r="AS4" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="56" t="s">
+      <c r="AT4" s="52"/>
+      <c r="AU4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="57"/>
-      <c r="AW4" s="56" t="s">
+      <c r="AV4" s="52"/>
+      <c r="AW4" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="56" t="s">
+      <c r="AX4" s="52"/>
+      <c r="AY4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="57"/>
-      <c r="BA4" s="56" t="s">
+      <c r="AZ4" s="52"/>
+      <c r="BA4" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="BB4" s="57"/>
-      <c r="BF4" s="38" t="s">
+      <c r="BB4" s="52"/>
+      <c r="BF4" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="BG4" s="61" t="s">
+      <c r="BG4" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="BH4" s="61"/>
-      <c r="BI4" s="61"/>
-      <c r="BJ4" s="61"/>
+      <c r="BH4" s="56"/>
+      <c r="BI4" s="56"/>
+      <c r="BJ4" s="56"/>
     </row>
     <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="N5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="S5" s="6" t="s">
@@ -1290,10 +1290,10 @@
       <c r="T5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="29" t="s">
+      <c r="V5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="W5" s="6" t="s">
@@ -1341,21 +1341,21 @@
       <c r="AK5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="29" t="s">
+      <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="34" t="s">
+      <c r="AM5" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="35"/>
-      <c r="AO5" s="63" t="s">
+      <c r="AN5" s="67"/>
+      <c r="AO5" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="64"/>
-      <c r="AQ5" s="62" t="s">
+      <c r="AP5" s="67"/>
+      <c r="AQ5" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="AR5" s="62"/>
+      <c r="AR5" s="69"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1386,24 +1386,24 @@
       <c r="BB5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BF5" s="38" t="s">
+      <c r="BF5" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BG5" s="61" t="s">
+      <c r="BG5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="BH5" s="61"/>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
+      <c r="BH5" s="56"/>
+      <c r="BI5" s="56"/>
+      <c r="BJ5" s="56"/>
     </row>
     <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="48" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1424,10 +1424,10 @@
       <c r="T6" s="4">
         <v>6000</v>
       </c>
-      <c r="U6" s="17" t="s">
+      <c r="U6" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="16">
         <v>7000</v>
       </c>
       <c r="W6" s="4" t="s">
@@ -1436,10 +1436,10 @@
       <c r="X6" s="4">
         <v>5000</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="16">
+      <c r="Z6" s="15">
         <v>5500</v>
       </c>
       <c r="AE6" s="8" t="s">
@@ -1448,10 +1448,10 @@
       <c r="AF6" s="9">
         <v>10000</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AG6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AH6" s="12">
+      <c r="AH6" s="11">
         <v>10100</v>
       </c>
       <c r="AI6" s="8" t="s">
@@ -1466,22 +1466,22 @@
       <c r="AL6">
         <v>12000</v>
       </c>
-      <c r="AM6" s="36" t="s">
+      <c r="AM6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="37">
+      <c r="AN6" s="34">
         <v>400</v>
       </c>
-      <c r="AO6" s="36" t="s">
+      <c r="AO6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AP6" s="37">
+      <c r="AP6" s="16">
         <v>1100</v>
       </c>
-      <c r="AQ6" s="17" t="s">
+      <c r="AQ6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AR6" s="20">
+      <c r="AR6" s="60">
         <v>1700</v>
       </c>
       <c r="AU6" s="9" t="s">
@@ -1508,16 +1508,16 @@
       <c r="BB6" s="9">
         <v>14010</v>
       </c>
-      <c r="BG6" s="39" t="s">
+      <c r="BG6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="BH6" s="39" t="s">
+      <c r="BH6" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="BI6" s="31" t="s">
+      <c r="BI6" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="BJ6" s="31" t="s">
+      <c r="BJ6" s="30" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1528,59 +1528,59 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="54"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="49"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="T7" s="4">
         <v>6001</v>
       </c>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
       <c r="W7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="X7" s="4">
         <v>5001</v>
       </c>
-      <c r="Y7" s="17" t="s">
+      <c r="Y7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="16">
         <v>5510</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AH7" s="14">
+      <c r="AH7" s="13">
         <v>10150</v>
       </c>
-      <c r="AI7" s="17"/>
-      <c r="AJ7" s="17"/>
-      <c r="AM7" s="36" t="s">
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AM7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AN7" s="37">
+      <c r="AN7" s="34">
         <v>401</v>
       </c>
-      <c r="AO7" s="36" t="s">
+      <c r="AO7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AP7" s="37">
+      <c r="AP7" s="16">
         <v>1102</v>
       </c>
-      <c r="AQ7" s="17" t="s">
+      <c r="AQ7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AR7" s="20">
+      <c r="AR7" s="60">
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
-      <c r="BG7" s="36" t="s">
+      <c r="BG7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="BH7" s="37">
+      <c r="BH7" s="34">
         <v>1100</v>
       </c>
       <c r="BI7">
@@ -1591,578 +1591,583 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="54"/>
-      <c r="S8" s="28" t="s">
+      <c r="I8" s="47"/>
+      <c r="J8" s="49"/>
+      <c r="S8" s="27" t="s">
         <v>56</v>
       </c>
       <c r="T8" s="4">
         <v>6002</v>
       </c>
-      <c r="Y8" s="20" t="s">
+      <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AM8" s="20" t="s">
+      <c r="AM8" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="AN8">
+      <c r="AN8" s="34">
         <v>410</v>
       </c>
-      <c r="AO8" s="20" t="s">
+      <c r="AO8" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="AP8">
+      <c r="AP8" s="16">
         <v>1110</v>
       </c>
-      <c r="AQ8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="AR8">
-        <v>1800</v>
-      </c>
-      <c r="BG8" s="36" t="s">
+      <c r="AQ8" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR8" s="34">
+        <v>1710</v>
+      </c>
+      <c r="BG8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="BH8" s="37">
+      <c r="BH8" s="34">
         <v>1102</v>
       </c>
     </row>
     <row r="9" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I9" s="52"/>
-      <c r="J9" s="54"/>
-      <c r="S9" s="28" t="s">
+      <c r="I9" s="47"/>
+      <c r="J9" s="49"/>
+      <c r="S9" s="27" t="s">
         <v>57</v>
       </c>
       <c r="T9" s="4">
         <v>6003</v>
       </c>
-      <c r="Y9" s="20" t="s">
+      <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AM9" s="36" t="s">
+      <c r="AM9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AN9" s="37">
+      <c r="AN9" s="34">
         <v>500</v>
       </c>
-      <c r="AO9" s="36" t="s">
+      <c r="AO9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AP9" s="37">
+      <c r="AP9" s="16">
         <v>1200</v>
       </c>
-      <c r="AQ9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR9">
-        <v>1801</v>
-      </c>
-      <c r="BG9" s="36" t="s">
+      <c r="AQ9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="BH9" s="37">
+      <c r="AR9" s="34">
+        <v>1800</v>
+      </c>
+      <c r="BG9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="BH9" s="34">
         <v>1200</v>
       </c>
     </row>
     <row r="10" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I10" s="52"/>
-      <c r="S10" s="28" t="s">
+      <c r="I10" s="47"/>
+      <c r="S10" s="27" t="s">
         <v>58</v>
       </c>
       <c r="T10" s="4">
         <v>6004</v>
       </c>
-      <c r="AM10" s="36" t="s">
+      <c r="AM10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="AN10" s="37">
+      <c r="AN10" s="34">
         <v>501</v>
       </c>
-      <c r="AO10" s="36" t="s">
+      <c r="AO10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="AP10" s="37">
+      <c r="AP10" s="16">
         <v>1201</v>
       </c>
-      <c r="AQ10" s="17" t="s">
+      <c r="AQ10" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR10" s="34">
+        <v>1801</v>
+      </c>
+      <c r="BG10" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH10" s="34">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="11" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I11" s="47"/>
+      <c r="AM11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AR10">
+      <c r="AN11" s="34">
+        <v>600</v>
+      </c>
+      <c r="AO11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP11" s="16">
+        <v>1300</v>
+      </c>
+      <c r="AQ11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR11" s="34">
         <v>1900</v>
       </c>
-      <c r="BG10" s="36" t="s">
+      <c r="AT11" s="18"/>
+      <c r="AU11" s="18"/>
+      <c r="BG11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="BH11" s="34">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="12" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I12" s="47"/>
+      <c r="AM12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN12" s="34">
+        <v>601</v>
+      </c>
+      <c r="AO12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP12" s="16">
+        <v>1301</v>
+      </c>
+      <c r="AQ12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR12" s="34">
+        <v>1901</v>
+      </c>
+      <c r="AT12" s="21"/>
+      <c r="AU12" s="21"/>
+      <c r="BG12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="BH12" s="34">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="13" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I13" s="47"/>
+      <c r="AM13" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN13" s="34">
+        <v>700</v>
+      </c>
+      <c r="AO13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP13" s="16">
+        <v>1400</v>
+      </c>
+      <c r="AQ13" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR13" s="34">
+        <v>2000</v>
+      </c>
+      <c r="AT13" s="16"/>
+      <c r="AU13" s="16"/>
+      <c r="BG13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="BH13" s="34">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I14" s="47"/>
+      <c r="AM14" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN14" s="34">
+        <v>701</v>
+      </c>
+      <c r="AO14" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP14" s="16">
+        <v>1401</v>
+      </c>
+      <c r="AQ14" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR14" s="34">
+        <v>2001</v>
+      </c>
+      <c r="BG14" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="BH14" s="34">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="15" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I15" s="47"/>
+      <c r="AM15" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN15" s="34">
+        <v>800</v>
+      </c>
+      <c r="AO15" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP15" s="16">
+        <v>1500</v>
+      </c>
+      <c r="AQ15" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR15" s="34">
+        <v>2100</v>
+      </c>
+      <c r="BG15" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH15" s="34">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="2:62" x14ac:dyDescent="0.4">
+      <c r="I16" s="47"/>
+      <c r="AM16" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN16" s="34">
+        <v>801</v>
+      </c>
+      <c r="AO16" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP16" s="16">
+        <v>1501</v>
+      </c>
+      <c r="AQ16" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR16" s="34">
+        <v>2101</v>
+      </c>
+      <c r="BG16" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="BH16" s="34">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="17" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I17" s="47"/>
+      <c r="AG17" s="45"/>
+      <c r="AH17" s="45"/>
+      <c r="AI17" s="45"/>
+      <c r="AJ17" s="45"/>
+      <c r="AM17" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN17" s="34">
+        <v>900</v>
+      </c>
+      <c r="AO17" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP17" s="16">
+        <v>1600</v>
+      </c>
+      <c r="AQ17" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR17" s="34">
+        <v>2200</v>
+      </c>
+      <c r="BG17" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH17" s="34">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="18" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I18" s="47"/>
+      <c r="AM18" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN18" s="34">
+        <v>901</v>
+      </c>
+      <c r="AO18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP18" s="61">
+        <v>1601</v>
+      </c>
+      <c r="AQ18" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR18" s="34">
+        <v>2201</v>
+      </c>
+      <c r="BG18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH18" s="34">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="19" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I19" s="47"/>
+      <c r="AM19" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN19" s="34">
+        <v>1000</v>
+      </c>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16"/>
+      <c r="AQ19" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR19" s="34">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="20" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I20" s="47"/>
+      <c r="AM20" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN20" s="34">
+        <v>1001</v>
+      </c>
+      <c r="AO20" s="16"/>
+      <c r="AP20" s="16"/>
+      <c r="AQ20" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR20" s="34">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="21" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="I21" s="47"/>
+      <c r="AM21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN21" s="13">
+        <v>999</v>
+      </c>
+      <c r="AO21" s="16"/>
+      <c r="AP21" s="16"/>
+      <c r="AQ21" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR21" s="34">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="22" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AO22" s="32"/>
+      <c r="AP22" s="32"/>
+      <c r="AQ22" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR22" s="60">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="23" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM23" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN23" s="56"/>
+      <c r="AO23" s="16"/>
+      <c r="AP23" s="16"/>
+      <c r="AQ23" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR23" s="63">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="24" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM24" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN24" s="60">
+        <v>1010</v>
+      </c>
+      <c r="AO24" s="16"/>
+      <c r="AP24" s="16"/>
+      <c r="AQ24" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR24" s="60">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="25" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM25" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN25" s="60">
+        <v>1011</v>
+      </c>
+      <c r="AO25" s="16"/>
+      <c r="AP25" s="16"/>
+      <c r="AQ25" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="AR25" s="60">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="26" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AO26" s="16"/>
+      <c r="AP26" s="16"/>
+      <c r="AQ26" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="AR26" s="65">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="27" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="16"/>
+      <c r="AR27" s="16"/>
+    </row>
+    <row r="28" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM28" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN28" s="34">
+        <v>500</v>
+      </c>
+      <c r="AO28" s="16"/>
+      <c r="AP28" s="16"/>
+      <c r="AQ28" s="16"/>
+      <c r="AR28" s="16"/>
+    </row>
+    <row r="29" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM29" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="BH10" s="37">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="11" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I11" s="52"/>
-      <c r="AM11" s="36" t="s">
+      <c r="AN29" s="34">
+        <v>501</v>
+      </c>
+      <c r="AO29" s="16"/>
+      <c r="AP29" s="16"/>
+      <c r="AQ29" s="16"/>
+      <c r="AR29" s="16"/>
+    </row>
+    <row r="30" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM30" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AN11" s="37">
+      <c r="AN30" s="34">
         <v>600</v>
       </c>
-      <c r="AO11" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP11" s="37">
-        <v>1300</v>
-      </c>
-      <c r="AQ11" s="17" t="s">
+      <c r="AO30" s="16"/>
+      <c r="AP30" s="16"/>
+      <c r="AQ30" s="16"/>
+      <c r="AR30" s="16"/>
+    </row>
+    <row r="31" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM31" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AR11">
-        <v>1901</v>
-      </c>
-      <c r="AT11" s="19"/>
-      <c r="AU11" s="19"/>
-      <c r="BG11" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="BH11" s="37">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="12" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I12" s="52"/>
-      <c r="AM12" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AN12" s="37">
+      <c r="AN31" s="34">
         <v>601</v>
       </c>
-      <c r="AO12" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP12" s="37">
-        <v>1301</v>
-      </c>
-      <c r="AQ12" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="AR12">
-        <v>2000</v>
-      </c>
-      <c r="AT12" s="22"/>
-      <c r="AU12" s="22"/>
-      <c r="BG12" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="BH12" s="37">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="13" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I13" s="52"/>
-      <c r="AM13" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN13" s="37">
+      <c r="AO31" s="16"/>
+      <c r="AP31" s="16"/>
+      <c r="AQ31" s="16"/>
+      <c r="AR31" s="16"/>
+    </row>
+    <row r="32" spans="9:60" x14ac:dyDescent="0.4">
+      <c r="AM32" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="AN32" s="34">
         <v>700</v>
       </c>
-      <c r="AO13" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP13" s="37">
-        <v>1400</v>
-      </c>
-      <c r="AQ13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR13">
-        <v>2001</v>
-      </c>
-      <c r="AT13" s="17"/>
-      <c r="AU13" s="17"/>
-      <c r="BG13" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="BH13" s="37">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="14" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I14" s="52"/>
-      <c r="AM14" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN14" s="37">
+      <c r="AO32" s="16"/>
+      <c r="AP32" s="16"/>
+      <c r="AQ32" s="16"/>
+      <c r="AR32" s="16"/>
+    </row>
+    <row r="33" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM33" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN33" s="34">
         <v>701</v>
       </c>
-      <c r="AO14" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP14" s="37">
-        <v>1401</v>
-      </c>
-      <c r="AQ14" s="17" t="s">
+      <c r="AO33" s="16"/>
+      <c r="AP33" s="16"/>
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+    </row>
+    <row r="34" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM34" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AR14">
-        <v>2100</v>
-      </c>
-      <c r="BG14" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="BH14" s="37">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="15" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I15" s="52"/>
-      <c r="AM15" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="AN15" s="37">
+      <c r="AN34" s="34">
         <v>800</v>
       </c>
-      <c r="AO15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="AP15" s="37">
-        <v>1500</v>
-      </c>
-      <c r="AQ15" s="17" t="s">
+      <c r="AO34" s="16"/>
+      <c r="AP34" s="16"/>
+      <c r="AQ34" s="16"/>
+      <c r="AR34" s="16"/>
+    </row>
+    <row r="35" spans="39:44" x14ac:dyDescent="0.4">
+      <c r="AM35" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="AR15">
-        <v>2101</v>
-      </c>
-      <c r="BG15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="BH15" s="37">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="16" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I16" s="52"/>
-      <c r="AM16" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN16" s="37">
+      <c r="AN35" s="34">
         <v>801</v>
       </c>
-      <c r="AO16" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP16" s="37">
-        <v>1501</v>
-      </c>
-      <c r="AQ16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR16">
-        <v>2200</v>
-      </c>
-      <c r="BG16" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="BH16" s="37">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="17" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I17" s="52"/>
-      <c r="AG17" s="48"/>
-      <c r="AH17" s="48"/>
-      <c r="AI17" s="48"/>
-      <c r="AJ17" s="48"/>
-      <c r="AM17" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN17" s="37">
-        <v>900</v>
-      </c>
-      <c r="AO17" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP17" s="37">
-        <v>1600</v>
-      </c>
-      <c r="AQ17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR17">
-        <v>2201</v>
-      </c>
-      <c r="BG17" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="BH17" s="37">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="18" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I18" s="52"/>
-      <c r="AM18" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN18" s="37">
-        <v>901</v>
-      </c>
-      <c r="AO18" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP18" s="37">
-        <v>1601</v>
-      </c>
-      <c r="AQ18" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR18">
-        <v>2300</v>
-      </c>
-      <c r="BG18" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="BH18" s="37">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="19" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I19" s="52"/>
-      <c r="AM19" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN19" s="37">
-        <v>1000</v>
-      </c>
-      <c r="AO19" s="17"/>
-      <c r="AP19" s="17"/>
-      <c r="AQ19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR19">
-        <v>2301</v>
-      </c>
-    </row>
-    <row r="20" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I20" s="52"/>
-      <c r="AM20" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN20" s="37">
-        <v>1001</v>
-      </c>
-      <c r="AO20" s="17"/>
-      <c r="AP20" s="17"/>
-      <c r="AQ20" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="AR20" s="17">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="21" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I21" s="52"/>
-      <c r="AM21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN21" s="14">
-        <v>999</v>
-      </c>
-      <c r="AO21" s="17"/>
-      <c r="AP21" s="17"/>
-      <c r="AQ21" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR21" s="20">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="22" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AO22" s="33"/>
-      <c r="AP22" s="33"/>
-      <c r="AQ22" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="AR22" s="50">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="23" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM23" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN23" s="61"/>
-      <c r="AO23" s="17"/>
-      <c r="AP23" s="17"/>
-      <c r="AQ23" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="AR23" s="20">
-        <v>2501</v>
-      </c>
-    </row>
-    <row r="24" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM24" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN24" s="67">
-        <v>1010</v>
-      </c>
-      <c r="AO24" s="17"/>
-      <c r="AP24" s="17"/>
-      <c r="AQ24" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="AR24" s="20">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="25" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM25" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN25" s="67">
-        <v>1011</v>
-      </c>
-      <c r="AO25" s="17"/>
-      <c r="AP25" s="17"/>
-      <c r="AQ25" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="AR25" s="20">
-        <v>2601</v>
-      </c>
-    </row>
-    <row r="26" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AO26" s="17"/>
-      <c r="AP26" s="17"/>
-      <c r="AQ26" s="17"/>
-      <c r="AR26" s="17"/>
-    </row>
-    <row r="27" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="17"/>
-      <c r="AR27" s="17"/>
-    </row>
-    <row r="28" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM28" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN28" s="37">
-        <v>500</v>
-      </c>
-      <c r="AO28" s="17"/>
-      <c r="AP28" s="17"/>
-      <c r="AQ28" s="17"/>
-      <c r="AR28" s="17"/>
-    </row>
-    <row r="29" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM29" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AN29" s="37">
-        <v>501</v>
-      </c>
-      <c r="AO29" s="17"/>
-      <c r="AP29" s="17"/>
-      <c r="AQ29" s="17"/>
-      <c r="AR29" s="17"/>
-    </row>
-    <row r="30" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM30" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="AN30" s="37">
-        <v>600</v>
-      </c>
-      <c r="AO30" s="17"/>
-      <c r="AP30" s="17"/>
-      <c r="AQ30" s="17"/>
-      <c r="AR30" s="17"/>
-    </row>
-    <row r="31" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM31" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AN31" s="37">
-        <v>601</v>
-      </c>
-      <c r="AO31" s="17"/>
-      <c r="AP31" s="17"/>
-      <c r="AQ31" s="17"/>
-      <c r="AR31" s="17"/>
-    </row>
-    <row r="32" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM32" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN32" s="37">
-        <v>700</v>
-      </c>
-      <c r="AO32" s="17"/>
-      <c r="AP32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="17"/>
-    </row>
-    <row r="33" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AM33" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN33" s="37">
-        <v>701</v>
-      </c>
-      <c r="AO33" s="17"/>
-      <c r="AP33" s="17"/>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-    </row>
-    <row r="34" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AM34" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="AN34" s="37">
-        <v>800</v>
-      </c>
-      <c r="AO34" s="17"/>
-      <c r="AP34" s="17"/>
-      <c r="AQ34" s="17"/>
-      <c r="AR34" s="17"/>
-    </row>
-    <row r="35" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AM35" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN35" s="37">
-        <v>801</v>
-      </c>
-      <c r="AO35" s="32"/>
-      <c r="AP35" s="32"/>
-      <c r="AQ35" s="32"/>
-      <c r="AR35" s="32"/>
+      <c r="AO35" s="31"/>
+      <c r="AP35" s="31"/>
+      <c r="AQ35" s="31"/>
+      <c r="AR35" s="31"/>
     </row>
     <row r="36" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AM36" s="36"/>
-      <c r="AN36" s="37"/>
-      <c r="AO36" s="20"/>
-      <c r="AP36" s="20" t="s">
+      <c r="AM36" s="33"/>
+      <c r="AN36" s="34"/>
+      <c r="AO36" s="19"/>
+      <c r="AP36" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="AQ36" s="20"/>
-      <c r="AR36" s="20"/>
+      <c r="AQ36" s="19"/>
+      <c r="AR36" s="19"/>
     </row>
     <row r="37" spans="39:44" x14ac:dyDescent="0.4">
-      <c r="AO37" s="20"/>
-      <c r="AP37" s="20"/>
-      <c r="AQ37" s="20"/>
-      <c r="AR37" s="20"/>
+      <c r="AO37" s="19"/>
+      <c r="AP37" s="19"/>
+      <c r="AQ37" s="19"/>
+      <c r="AR37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
     <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="AS4:AT4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="AM4:AR4"/>
@@ -2211,23 +2216,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="F3" s="25"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
@@ -2239,7 +2244,7 @@
       <c r="C4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -2256,19 +2261,19 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="4"/>
@@ -2277,17 +2282,17 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="4"/>
@@ -2296,41 +2301,41 @@
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29" t="s">
         <v>79</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A8" s="42">
+      <c r="A8" s="39">
         <v>4</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="40" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2338,112 +2343,112 @@
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="40" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="46">
+      <c r="A10" s="43">
         <v>6</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="47" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2473,26 +2478,26 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2501,10 +2506,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2513,15 +2518,15 @@
         <v>2</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2543,93 +2548,93 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.23046875" style="40"/>
+    <col min="2" max="2" width="9.23046875" style="37"/>
     <col min="3" max="3" width="40.84375" customWidth="1"/>
     <col min="4" max="4" width="55.23046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="37" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="38" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="B5" s="45">
+      <c r="B5" s="42">
         <v>1</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="41" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B6" s="45">
+      <c r="B6" s="42">
         <v>2</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="41" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B7" s="45"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="45"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B9" s="45"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B10" s="45"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B11" s="45"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B12" s="45"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B13" s="45"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B14" s="45"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B15" s="45"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create class Tail for Mario's attack, just have basic class structure
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D70BEE-FB7A-4ACB-92D0-459CB515880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286BD5D9-0D30-43CD-B26F-1EEDD6BE21D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-77" yWindow="-77" windowWidth="33068" windowHeight="18223" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="127">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -418,6 +418,18 @@
   </si>
   <si>
     <t>Go into + Get out of Pipe</t>
+  </si>
+  <si>
+    <t>Mario bị kẹt khi chui xuống Hidden Zone</t>
+  </si>
+  <si>
+    <t>Mario đứng ở rìa bên trái của cái pipe_gate</t>
+  </si>
+  <si>
+    <t>Mới chỉ phát hiện được một lần gần đây, chưa test đủ nhiều để biết được tần suất</t>
+  </si>
+  <si>
+    <t>Ani khi chui vào Hidden Zone bị lòi ra một chút bên ngoài pipe_gate</t>
   </si>
 </sst>
 </file>
@@ -463,7 +475,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -624,17 +636,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -655,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -741,12 +742,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,7 +786,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1128,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="AJ3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AT11" sqref="AT11"/>
     </sheetView>
   </sheetViews>
@@ -1174,94 +1169,94 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="53"/>
+      <c r="N4" s="51"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="50" t="s">
+      <c r="S4" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50" t="s">
+      <c r="T4" s="48"/>
+      <c r="U4" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50" t="s">
+      <c r="V4" s="48"/>
+      <c r="W4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50" t="s">
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="51" t="s">
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="51" t="s">
+      <c r="AB4" s="50"/>
+      <c r="AC4" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="51" t="s">
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="51" t="s">
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="51" t="s">
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="51" t="s">
+      <c r="AJ4" s="50"/>
+      <c r="AK4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="54" t="s">
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="46"/>
-      <c r="AO4" s="55"/>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="55"/>
-      <c r="AR4" s="52"/>
-      <c r="AS4" s="51" t="s">
+      <c r="AN4" s="44"/>
+      <c r="AO4" s="53"/>
+      <c r="AP4" s="53"/>
+      <c r="AQ4" s="53"/>
+      <c r="AR4" s="50"/>
+      <c r="AS4" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="52"/>
-      <c r="AU4" s="51" t="s">
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="52"/>
-      <c r="AW4" s="51" t="s">
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="AX4" s="52"/>
-      <c r="AY4" s="51" t="s">
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="52"/>
-      <c r="BA4" s="51" t="s">
+      <c r="AZ4" s="50"/>
+      <c r="BA4" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="BB4" s="52"/>
+      <c r="BB4" s="50"/>
       <c r="BF4" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="BG4" s="56" t="s">
+      <c r="BG4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="BH4" s="56"/>
-      <c r="BI4" s="56"/>
-      <c r="BJ4" s="56"/>
+      <c r="BH4" s="54"/>
+      <c r="BI4" s="54"/>
+      <c r="BJ4" s="54"/>
     </row>
     <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1344,18 +1339,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="66" t="s">
+      <c r="AM5" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="67"/>
-      <c r="AO5" s="66" t="s">
+      <c r="AN5" s="65"/>
+      <c r="AO5" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="67"/>
-      <c r="AQ5" s="68" t="s">
+      <c r="AP5" s="65"/>
+      <c r="AQ5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="AR5" s="69"/>
+      <c r="AR5" s="67"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1389,21 +1384,21 @@
       <c r="BF5" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BG5" s="56" t="s">
+      <c r="BG5" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="BH5" s="56"/>
-      <c r="BI5" s="56"/>
-      <c r="BJ5" s="56"/>
+      <c r="BH5" s="54"/>
+      <c r="BI5" s="54"/>
+      <c r="BJ5" s="54"/>
     </row>
     <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="48" t="s">
+      <c r="J6" s="46" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1481,7 +1476,7 @@
       <c r="AQ6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AR6" s="60">
+      <c r="AR6" s="58">
         <v>1700</v>
       </c>
       <c r="AU6" s="9" t="s">
@@ -1528,8 +1523,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="49"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="47"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1573,7 +1568,7 @@
       <c r="AQ7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AR7" s="60">
+      <c r="AR7" s="58">
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
@@ -1591,8 +1586,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="49"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="47"/>
       <c r="S8" s="27" t="s">
         <v>56</v>
       </c>
@@ -1605,19 +1600,19 @@
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AM8" s="59" t="s">
+      <c r="AM8" s="57" t="s">
         <v>122</v>
       </c>
       <c r="AN8" s="34">
         <v>410</v>
       </c>
-      <c r="AO8" s="59" t="s">
+      <c r="AO8" s="57" t="s">
         <v>122</v>
       </c>
       <c r="AP8" s="16">
         <v>1110</v>
       </c>
-      <c r="AQ8" s="59" t="s">
+      <c r="AQ8" s="57" t="s">
         <v>122</v>
       </c>
       <c r="AR8" s="34">
@@ -1631,8 +1626,8 @@
       </c>
     </row>
     <row r="9" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I9" s="47"/>
-      <c r="J9" s="49"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="47"/>
       <c r="S9" s="27" t="s">
         <v>57</v>
       </c>
@@ -1671,7 +1666,7 @@
       </c>
     </row>
     <row r="10" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I10" s="47"/>
+      <c r="I10" s="45"/>
       <c r="S10" s="27" t="s">
         <v>58</v>
       </c>
@@ -1704,7 +1699,7 @@
       </c>
     </row>
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I11" s="47"/>
+      <c r="I11" s="45"/>
       <c r="AM11" s="33" t="s">
         <v>23</v>
       </c>
@@ -1733,7 +1728,7 @@
       </c>
     </row>
     <row r="12" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I12" s="47"/>
+      <c r="I12" s="45"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1762,7 +1757,7 @@
       </c>
     </row>
     <row r="13" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I13" s="47"/>
+      <c r="I13" s="45"/>
       <c r="AM13" s="33" t="s">
         <v>25</v>
       </c>
@@ -1791,7 +1786,7 @@
       </c>
     </row>
     <row r="14" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I14" s="47"/>
+      <c r="I14" s="45"/>
       <c r="AM14" s="33" t="s">
         <v>26</v>
       </c>
@@ -1818,7 +1813,7 @@
       </c>
     </row>
     <row r="15" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I15" s="47"/>
+      <c r="I15" s="45"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
       </c>
@@ -1845,7 +1840,7 @@
       </c>
     </row>
     <row r="16" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I16" s="47"/>
+      <c r="I16" s="45"/>
       <c r="AM16" s="33" t="s">
         <v>28</v>
       </c>
@@ -1872,11 +1867,11 @@
       </c>
     </row>
     <row r="17" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I17" s="47"/>
-      <c r="AG17" s="45"/>
-      <c r="AH17" s="45"/>
-      <c r="AI17" s="45"/>
-      <c r="AJ17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="AG17" s="43"/>
+      <c r="AH17" s="43"/>
+      <c r="AI17" s="43"/>
+      <c r="AJ17" s="43"/>
       <c r="AM17" s="33" t="s">
         <v>29</v>
       </c>
@@ -1903,7 +1898,7 @@
       </c>
     </row>
     <row r="18" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I18" s="47"/>
+      <c r="I18" s="45"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
       </c>
@@ -1913,7 +1908,7 @@
       <c r="AO18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AP18" s="61">
+      <c r="AP18" s="59">
         <v>1601</v>
       </c>
       <c r="AQ18" s="33" t="s">
@@ -1930,7 +1925,7 @@
       </c>
     </row>
     <row r="19" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I19" s="47"/>
+      <c r="I19" s="45"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
       </c>
@@ -1947,7 +1942,7 @@
       </c>
     </row>
     <row r="20" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I20" s="47"/>
+      <c r="I20" s="45"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
       </c>
@@ -1964,7 +1959,7 @@
       </c>
     </row>
     <row r="21" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I21" s="47"/>
+      <c r="I21" s="45"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1973,7 +1968,7 @@
       </c>
       <c r="AO21" s="16"/>
       <c r="AP21" s="16"/>
-      <c r="AQ21" s="59" t="s">
+      <c r="AQ21" s="57" t="s">
         <v>109</v>
       </c>
       <c r="AR21" s="34">
@@ -1983,24 +1978,24 @@
     <row r="22" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
-      <c r="AQ22" s="59" t="s">
+      <c r="AQ22" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="AR22" s="60">
+      <c r="AR22" s="58">
         <v>2401</v>
       </c>
     </row>
     <row r="23" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM23" s="56" t="s">
+      <c r="AM23" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="AN23" s="56"/>
+      <c r="AN23" s="54"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
-      <c r="AQ23" s="62" t="s">
+      <c r="AQ23" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="AR23" s="63">
+      <c r="AR23" s="61">
         <v>2500</v>
       </c>
     </row>
@@ -2008,15 +2003,15 @@
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AN24" s="60">
+      <c r="AN24" s="58">
         <v>1010</v>
       </c>
       <c r="AO24" s="16"/>
       <c r="AP24" s="16"/>
-      <c r="AQ24" s="59" t="s">
+      <c r="AQ24" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="AR24" s="60">
+      <c r="AR24" s="58">
         <v>2501</v>
       </c>
     </row>
@@ -2024,25 +2019,25 @@
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AN25" s="60">
+      <c r="AN25" s="58">
         <v>1011</v>
       </c>
       <c r="AO25" s="16"/>
       <c r="AP25" s="16"/>
-      <c r="AQ25" s="59" t="s">
+      <c r="AQ25" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="AR25" s="60">
+      <c r="AR25" s="58">
         <v>2600</v>
       </c>
     </row>
     <row r="26" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
-      <c r="AQ26" s="64" t="s">
+      <c r="AQ26" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="AR26" s="65">
+      <c r="AR26" s="63">
         <v>2601</v>
       </c>
     </row>
@@ -2202,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2216,20 +2211,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="24"/>
@@ -2361,34 +2356,61 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="43">
+      <c r="A10" s="39">
         <v>6</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="44" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="39">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A12" s="39">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B13" s="25"/>
@@ -2478,14 +2500,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Adjust animations for Raccoon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286BD5D9-0D30-43CD-B26F-1EEDD6BE21D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA18CA6-6749-409D-A30C-10E023D59B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="33068" windowHeight="18223" activeTab="1" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="126">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -412,9 +412,6 @@
   </si>
   <si>
     <t>Mario Big Hold Koopa</t>
-  </si>
-  <si>
-    <t>Thêm Animation cho Mario khi chui ống nữa</t>
   </si>
   <si>
     <t>Go into + Get out of Pipe</t>
@@ -745,45 +742,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -795,16 +753,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1123,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AT11" sqref="AT11"/>
+    <sheetView tabSelected="1" topLeftCell="AJ6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AR35" sqref="AR35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1169,94 +1166,94 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51" t="s">
+      <c r="L4" s="65"/>
+      <c r="M4" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="51"/>
+      <c r="N4" s="65"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="S4" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48" t="s">
+      <c r="T4" s="56"/>
+      <c r="U4" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48" t="s">
+      <c r="V4" s="56"/>
+      <c r="W4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48" t="s">
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="49" t="s">
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="49" t="s">
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="49" t="s">
+      <c r="AD4" s="55"/>
+      <c r="AE4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="49" t="s">
+      <c r="AF4" s="55"/>
+      <c r="AG4" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="49" t="s">
+      <c r="AH4" s="55"/>
+      <c r="AI4" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="49" t="s">
+      <c r="AJ4" s="55"/>
+      <c r="AK4" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="52" t="s">
+      <c r="AL4" s="55"/>
+      <c r="AM4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="44"/>
-      <c r="AO4" s="53"/>
-      <c r="AP4" s="53"/>
-      <c r="AQ4" s="53"/>
-      <c r="AR4" s="50"/>
-      <c r="AS4" s="49" t="s">
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59"/>
+      <c r="AR4" s="55"/>
+      <c r="AS4" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="50"/>
-      <c r="AU4" s="49" t="s">
+      <c r="AT4" s="55"/>
+      <c r="AU4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="50"/>
-      <c r="AW4" s="49" t="s">
+      <c r="AV4" s="55"/>
+      <c r="AW4" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="AX4" s="50"/>
-      <c r="AY4" s="49" t="s">
+      <c r="AX4" s="55"/>
+      <c r="AY4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="50"/>
-      <c r="BA4" s="49" t="s">
+      <c r="AZ4" s="55"/>
+      <c r="BA4" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="BB4" s="50"/>
+      <c r="BB4" s="55"/>
       <c r="BF4" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="BG4" s="54" t="s">
+      <c r="BG4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="BH4" s="54"/>
-      <c r="BI4" s="54"/>
-      <c r="BJ4" s="54"/>
+      <c r="BH4" s="51"/>
+      <c r="BI4" s="51"/>
+      <c r="BJ4" s="51"/>
     </row>
     <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
@@ -1339,18 +1336,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="64" t="s">
+      <c r="AM5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="64" t="s">
+      <c r="AN5" s="53"/>
+      <c r="AO5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="66" t="s">
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="AR5" s="67"/>
+      <c r="AR5" s="61"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1384,21 +1381,21 @@
       <c r="BF5" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BG5" s="54" t="s">
+      <c r="BG5" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="BH5" s="54"/>
-      <c r="BI5" s="54"/>
-      <c r="BJ5" s="54"/>
+      <c r="BH5" s="51"/>
+      <c r="BI5" s="51"/>
+      <c r="BJ5" s="51"/>
     </row>
     <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="63" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1476,7 +1473,7 @@
       <c r="AQ6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AR6" s="58">
+      <c r="AR6" s="45">
         <v>1700</v>
       </c>
       <c r="AU6" s="9" t="s">
@@ -1523,8 +1520,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="47"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="64"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1568,7 +1565,7 @@
       <c r="AQ7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AR7" s="58">
+      <c r="AR7" s="45">
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
@@ -1586,8 +1583,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="47"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="64"/>
       <c r="S8" s="27" t="s">
         <v>56</v>
       </c>
@@ -1600,20 +1597,20 @@
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AM8" s="57" t="s">
-        <v>122</v>
+      <c r="AM8" s="44" t="s">
+        <v>121</v>
       </c>
       <c r="AN8" s="34">
         <v>410</v>
       </c>
-      <c r="AO8" s="57" t="s">
-        <v>122</v>
+      <c r="AO8" s="44" t="s">
+        <v>121</v>
       </c>
       <c r="AP8" s="16">
         <v>1110</v>
       </c>
-      <c r="AQ8" s="57" t="s">
-        <v>122</v>
+      <c r="AQ8" s="44" t="s">
+        <v>121</v>
       </c>
       <c r="AR8" s="34">
         <v>1710</v>
@@ -1626,8 +1623,8 @@
       </c>
     </row>
     <row r="9" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I9" s="45"/>
-      <c r="J9" s="47"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="64"/>
       <c r="S9" s="27" t="s">
         <v>57</v>
       </c>
@@ -1666,7 +1663,7 @@
       </c>
     </row>
     <row r="10" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I10" s="45"/>
+      <c r="I10" s="62"/>
       <c r="S10" s="27" t="s">
         <v>58</v>
       </c>
@@ -1699,7 +1696,7 @@
       </c>
     </row>
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I11" s="45"/>
+      <c r="I11" s="62"/>
       <c r="AM11" s="33" t="s">
         <v>23</v>
       </c>
@@ -1728,7 +1725,7 @@
       </c>
     </row>
     <row r="12" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I12" s="45"/>
+      <c r="I12" s="62"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1757,7 +1754,7 @@
       </c>
     </row>
     <row r="13" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I13" s="45"/>
+      <c r="I13" s="62"/>
       <c r="AM13" s="33" t="s">
         <v>25</v>
       </c>
@@ -1786,7 +1783,7 @@
       </c>
     </row>
     <row r="14" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I14" s="45"/>
+      <c r="I14" s="62"/>
       <c r="AM14" s="33" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1810,7 @@
       </c>
     </row>
     <row r="15" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I15" s="45"/>
+      <c r="I15" s="62"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
       </c>
@@ -1840,7 +1837,7 @@
       </c>
     </row>
     <row r="16" spans="2:62" x14ac:dyDescent="0.4">
-      <c r="I16" s="45"/>
+      <c r="I16" s="62"/>
       <c r="AM16" s="33" t="s">
         <v>28</v>
       </c>
@@ -1867,7 +1864,7 @@
       </c>
     </row>
     <row r="17" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I17" s="45"/>
+      <c r="I17" s="62"/>
       <c r="AG17" s="43"/>
       <c r="AH17" s="43"/>
       <c r="AI17" s="43"/>
@@ -1898,7 +1895,7 @@
       </c>
     </row>
     <row r="18" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I18" s="45"/>
+      <c r="I18" s="62"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
       </c>
@@ -1908,7 +1905,7 @@
       <c r="AO18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AP18" s="59">
+      <c r="AP18" s="46">
         <v>1601</v>
       </c>
       <c r="AQ18" s="33" t="s">
@@ -1925,7 +1922,7 @@
       </c>
     </row>
     <row r="19" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I19" s="45"/>
+      <c r="I19" s="62"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
       </c>
@@ -1942,7 +1939,7 @@
       </c>
     </row>
     <row r="20" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I20" s="45"/>
+      <c r="I20" s="62"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
       </c>
@@ -1959,7 +1956,7 @@
       </c>
     </row>
     <row r="21" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="I21" s="45"/>
+      <c r="I21" s="62"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -1968,7 +1965,7 @@
       </c>
       <c r="AO21" s="16"/>
       <c r="AP21" s="16"/>
-      <c r="AQ21" s="57" t="s">
+      <c r="AQ21" s="44" t="s">
         <v>109</v>
       </c>
       <c r="AR21" s="34">
@@ -1978,24 +1975,24 @@
     <row r="22" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
-      <c r="AQ22" s="57" t="s">
+      <c r="AQ22" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="AR22" s="58">
+      <c r="AR22" s="45">
         <v>2401</v>
       </c>
     </row>
     <row r="23" spans="9:60" x14ac:dyDescent="0.4">
-      <c r="AM23" s="54" t="s">
+      <c r="AM23" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="AN23" s="54"/>
+      <c r="AN23" s="51"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
-      <c r="AQ23" s="60" t="s">
+      <c r="AQ23" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="AR23" s="61">
+      <c r="AR23" s="48">
         <v>2500</v>
       </c>
     </row>
@@ -2003,15 +2000,15 @@
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AN24" s="58">
+      <c r="AN24" s="45">
         <v>1010</v>
       </c>
       <c r="AO24" s="16"/>
       <c r="AP24" s="16"/>
-      <c r="AQ24" s="57" t="s">
+      <c r="AQ24" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="AR24" s="58">
+      <c r="AR24" s="45">
         <v>2501</v>
       </c>
     </row>
@@ -2019,25 +2016,25 @@
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AN25" s="58">
+      <c r="AN25" s="45">
         <v>1011</v>
       </c>
       <c r="AO25" s="16"/>
       <c r="AP25" s="16"/>
-      <c r="AQ25" s="57" t="s">
+      <c r="AQ25" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="AR25" s="58">
+      <c r="AR25" s="45">
         <v>2600</v>
       </c>
     </row>
     <row r="26" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
-      <c r="AQ26" s="62" t="s">
+      <c r="AQ26" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="AR26" s="63">
+      <c r="AR26" s="50">
         <v>2601</v>
       </c>
     </row>
@@ -2147,9 +2144,7 @@
       <c r="AM36" s="33"/>
       <c r="AN36" s="34"/>
       <c r="AO36" s="19"/>
-      <c r="AP36" s="19" t="s">
-        <v>121</v>
-      </c>
+      <c r="AP36" s="19"/>
       <c r="AQ36" s="19"/>
       <c r="AR36" s="19"/>
     </row>
@@ -2161,20 +2156,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AR4"/>
-    <mergeCell ref="BG4:BJ4"/>
-    <mergeCell ref="BG5:BJ5"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BA4:BB4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2187,6 +2168,20 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="BG4:BJ4"/>
+    <mergeCell ref="BG5:BJ5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2197,7 +2192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -2211,20 +2206,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="24"/>
@@ -2379,13 +2374,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="D11" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>125</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="40" t="s">
@@ -2398,13 +2393,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>125</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="40" t="s">
@@ -2500,14 +2495,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Modifying and adding animations for Koopa
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA18CA6-6749-409D-A30C-10E023D59B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEDBA62-EF88-4AB4-9D5F-C7A4FAAAA9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18274" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="127">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Ani khi chui vào Hidden Zone bị lòi ra một chút bên ngoài pipe_gate</t>
+  </si>
+  <si>
+    <t>Shelling Up</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -649,11 +652,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -804,6 +818,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1120,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AR35" sqref="AR35"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1697,6 +1712,12 @@
     </row>
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I11" s="62"/>
+      <c r="S11" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="T11" s="68">
+        <v>6005</v>
+      </c>
       <c r="AM11" s="33" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Add animations Spin Shell Up for Koopa
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEDBA62-EF88-4AB4-9D5F-C7A4FAAAA9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F8C67-B7DF-4DD6-AC5D-FD82588EF3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-144" yWindow="-144" windowWidth="23328" windowHeight="12792" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Thiếu "break" khi tạo object ở chỗ switch case trong Playscene.cpp</t>
-  </si>
-  <si>
-    <t>Shelling</t>
   </si>
   <si>
     <t>Spin Shell Left</t>
@@ -430,6 +427,15 @@
   </si>
   <si>
     <t>Shelling Up</t>
+  </si>
+  <si>
+    <t>Shelling Down</t>
+  </si>
+  <si>
+    <t>Spin Down</t>
+  </si>
+  <si>
+    <t>Spin Up</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,6 +825,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13:V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1197,7 +1209,7 @@
       </c>
       <c r="T4" s="56"/>
       <c r="U4" s="56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V4" s="56"/>
       <c r="W4" s="56" t="s">
@@ -1225,7 +1237,7 @@
       </c>
       <c r="AH4" s="55"/>
       <c r="AI4" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ4" s="55"/>
       <c r="AK4" s="54" t="s">
@@ -1249,7 +1261,7 @@
       </c>
       <c r="AV4" s="55"/>
       <c r="AW4" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AX4" s="55"/>
       <c r="AY4" s="54" t="s">
@@ -1257,11 +1269,11 @@
       </c>
       <c r="AZ4" s="55"/>
       <c r="BA4" s="54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB4" s="55"/>
       <c r="BF4" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="BG4" s="51" t="s">
         <v>18</v>
@@ -1360,7 +1372,7 @@
       </c>
       <c r="AP5" s="53"/>
       <c r="AQ5" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AR5" s="61"/>
       <c r="AS5" s="6" t="s">
@@ -1394,7 +1406,7 @@
         <v>12</v>
       </c>
       <c r="BF5" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BG5" s="51" t="s">
         <v>34</v>
@@ -1432,7 +1444,7 @@
         <v>6000</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V6" s="16">
         <v>7000</v>
@@ -1462,7 +1474,7 @@
         <v>10100</v>
       </c>
       <c r="AI6" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ6" s="9">
         <v>10200</v>
@@ -1498,7 +1510,7 @@
         <v>11000</v>
       </c>
       <c r="AW6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AX6" s="9">
         <v>13000</v>
@@ -1510,22 +1522,22 @@
         <v>14000</v>
       </c>
       <c r="BA6" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BB6" s="9">
         <v>14010</v>
       </c>
       <c r="BG6" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="BH6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="BH6" s="36" t="s">
-        <v>89</v>
-      </c>
       <c r="BI6" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="BJ6" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -1600,12 +1612,6 @@
       </c>
       <c r="I8" s="62"/>
       <c r="J8" s="64"/>
-      <c r="S8" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="T8" s="4">
-        <v>6002</v>
-      </c>
       <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1613,19 +1619,19 @@
         <v>5520</v>
       </c>
       <c r="AM8" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AN8" s="34">
         <v>410</v>
       </c>
       <c r="AO8" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AP8" s="16">
         <v>1110</v>
       </c>
       <c r="AQ8" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AR8" s="34">
         <v>1710</v>
@@ -1640,12 +1646,10 @@
     <row r="9" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I9" s="62"/>
       <c r="J9" s="64"/>
-      <c r="S9" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="T9" s="4">
-        <v>6003</v>
-      </c>
+      <c r="S9" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="T9" s="69"/>
       <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
@@ -1680,10 +1684,10 @@
     <row r="10" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I10" s="62"/>
       <c r="S10" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T10" s="4">
-        <v>6004</v>
+        <v>6010</v>
       </c>
       <c r="AM10" s="33" t="s">
         <v>22</v>
@@ -1712,11 +1716,11 @@
     </row>
     <row r="11" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I11" s="62"/>
-      <c r="S11" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="68">
-        <v>6005</v>
+      <c r="S11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="T11" s="4">
+        <v>6011</v>
       </c>
       <c r="AM11" s="33" t="s">
         <v>23</v>
@@ -1747,6 +1751,10 @@
     </row>
     <row r="12" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I12" s="62"/>
+      <c r="S12" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="T12" s="70"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1776,6 +1784,12 @@
     </row>
     <row r="13" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I13" s="62"/>
+      <c r="S13" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="T13" s="4">
+        <v>6015</v>
+      </c>
       <c r="AM13" s="33" t="s">
         <v>25</v>
       </c>
@@ -1805,6 +1819,12 @@
     </row>
     <row r="14" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I14" s="62"/>
+      <c r="S14" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" s="4">
+        <v>6016</v>
+      </c>
       <c r="AM14" s="33" t="s">
         <v>26</v>
       </c>
@@ -1859,6 +1879,12 @@
     </row>
     <row r="16" spans="2:62" x14ac:dyDescent="0.4">
       <c r="I16" s="62"/>
+      <c r="S16" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="T16" s="4">
+        <v>6020</v>
+      </c>
       <c r="AM16" s="33" t="s">
         <v>28</v>
       </c>
@@ -1886,6 +1912,12 @@
     </row>
     <row r="17" spans="9:60" x14ac:dyDescent="0.4">
       <c r="I17" s="62"/>
+      <c r="S17" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="T17" s="68">
+        <v>6021</v>
+      </c>
       <c r="AG17" s="43"/>
       <c r="AH17" s="43"/>
       <c r="AI17" s="43"/>
@@ -1987,7 +2019,7 @@
       <c r="AO21" s="16"/>
       <c r="AP21" s="16"/>
       <c r="AQ21" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AR21" s="34">
         <v>2400</v>
@@ -1997,7 +2029,7 @@
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
       <c r="AQ22" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AR22" s="45">
         <v>2401</v>
@@ -2005,13 +2037,13 @@
     </row>
     <row r="23" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM23" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AN23" s="51"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
       <c r="AQ23" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AR23" s="48">
         <v>2500</v>
@@ -2027,7 +2059,7 @@
       <c r="AO24" s="16"/>
       <c r="AP24" s="16"/>
       <c r="AQ24" s="44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AR24" s="45">
         <v>2501</v>
@@ -2043,7 +2075,7 @@
       <c r="AO25" s="16"/>
       <c r="AP25" s="16"/>
       <c r="AQ25" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AR25" s="45">
         <v>2600</v>
@@ -2053,7 +2085,7 @@
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AR26" s="50">
         <v>2601</v>
@@ -2115,7 +2147,7 @@
     </row>
     <row r="32" spans="9:60" x14ac:dyDescent="0.4">
       <c r="AM32" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AN32" s="34">
         <v>700</v>
@@ -2127,7 +2159,7 @@
     </row>
     <row r="33" spans="39:44" x14ac:dyDescent="0.4">
       <c r="AM33" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AN33" s="34">
         <v>701</v>
@@ -2176,7 +2208,7 @@
       <c r="AR37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2189,6 +2221,8 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S12:T12"/>
     <mergeCell ref="BG4:BJ4"/>
     <mergeCell ref="BG5:BJ5"/>
     <mergeCell ref="AW4:AX4"/>
@@ -2228,7 +2262,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B1" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -2236,7 +2270,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B2" s="66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -2247,25 +2281,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
@@ -2273,19 +2307,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>65</v>
-      </c>
       <c r="F5" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2294,17 +2328,17 @@
         <v>2</v>
       </c>
       <c r="B6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="D6" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2313,17 +2347,17 @@
         <v>3</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>78</v>
-      </c>
       <c r="D7" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2332,22 +2366,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="40" t="s">
+      <c r="E8" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="F8" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="G8" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -2355,19 +2389,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="D9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>93</v>
-      </c>
       <c r="F9" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2376,17 +2410,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>106</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2395,17 +2429,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="D11" s="29" t="s">
         <v>123</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>124</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2414,17 +2448,17 @@
         <v>8</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>123</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>124</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -2517,7 +2551,7 @@
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B4" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
@@ -2527,7 +2561,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>12</v>
@@ -2557,15 +2591,15 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="D8" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2593,18 +2627,18 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B3" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
@@ -2612,10 +2646,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.4">
@@ -2623,10 +2657,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add Crumb object for Breakable brick when it is breaked
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F8C67-B7DF-4DD6-AC5D-FD82588EF3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8973F55A-E7C6-4F95-9C65-A3B8A876A212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Spin Up</t>
+  </si>
+  <si>
+    <t>Crumb</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BJ37"/>
+  <dimension ref="B4:BL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13:V14"/>
+    <sheetView tabSelected="1" topLeftCell="AR3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BE9" sqref="BE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1174,15 +1177,15 @@
     <col min="51" max="51" width="9.765625" customWidth="1"/>
     <col min="52" max="52" width="8.4609375" customWidth="1"/>
     <col min="53" max="53" width="12.07421875" customWidth="1"/>
-    <col min="54" max="54" width="8.4609375" customWidth="1"/>
-    <col min="55" max="55" width="5.69140625" customWidth="1"/>
-    <col min="56" max="57" width="7.765625" customWidth="1"/>
-    <col min="58" max="58" width="11.69140625" customWidth="1"/>
-    <col min="59" max="60" width="13.4609375" customWidth="1"/>
-    <col min="61" max="61" width="13.07421875" customWidth="1"/>
+    <col min="54" max="56" width="8.4609375" customWidth="1"/>
+    <col min="57" max="57" width="5.69140625" customWidth="1"/>
+    <col min="58" max="59" width="7.765625" customWidth="1"/>
+    <col min="60" max="60" width="11.69140625" customWidth="1"/>
+    <col min="61" max="62" width="13.4609375" customWidth="1"/>
+    <col min="63" max="63" width="13.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:64" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,17 +1275,21 @@
         <v>115</v>
       </c>
       <c r="BB4" s="55"/>
-      <c r="BF4" s="35" t="s">
+      <c r="BC4" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD4" s="55"/>
+      <c r="BH4" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BG4" s="51" t="s">
+      <c r="BI4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="BH4" s="51"/>
-      <c r="BI4" s="51"/>
       <c r="BJ4" s="51"/>
-    </row>
-    <row r="5" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BK4" s="51"/>
+      <c r="BL4" s="51"/>
+    </row>
+    <row r="5" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1405,17 +1412,23 @@
       <c r="BB5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BF5" s="35" t="s">
+      <c r="BC5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="BG5" s="51" t="s">
+      <c r="BI5" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="BH5" s="51"/>
-      <c r="BI5" s="51"/>
       <c r="BJ5" s="51"/>
-    </row>
-    <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BK5" s="51"/>
+      <c r="BL5" s="51"/>
+    </row>
+    <row r="6" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -1527,20 +1540,26 @@
       <c r="BB6" s="9">
         <v>14010</v>
       </c>
-      <c r="BG6" s="36" t="s">
+      <c r="BC6" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD6" s="9">
+        <v>15000</v>
+      </c>
+      <c r="BI6" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="BH6" s="36" t="s">
+      <c r="BJ6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="BI6" s="30" t="s">
+      <c r="BK6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="BJ6" s="30" t="s">
+      <c r="BL6" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1596,17 +1615,17 @@
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
-      <c r="BG7" s="33" t="s">
+      <c r="BI7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="BH7" s="34">
+      <c r="BJ7" s="34">
         <v>1100</v>
       </c>
-      <c r="BI7">
+      <c r="BK7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:64" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -1636,14 +1655,14 @@
       <c r="AR8" s="34">
         <v>1710</v>
       </c>
-      <c r="BG8" s="33" t="s">
+      <c r="BI8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="BH8" s="34">
+      <c r="BJ8" s="34">
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I9" s="62"/>
       <c r="J9" s="64"/>
       <c r="S9" s="69" t="s">
@@ -1674,14 +1693,14 @@
       <c r="AR9" s="34">
         <v>1800</v>
       </c>
-      <c r="BG9" s="33" t="s">
+      <c r="BI9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="BH9" s="34">
+      <c r="BJ9" s="34">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I10" s="62"/>
       <c r="S10" s="27" t="s">
         <v>56</v>
@@ -1707,14 +1726,14 @@
       <c r="AR10" s="34">
         <v>1801</v>
       </c>
-      <c r="BG10" s="33" t="s">
+      <c r="BI10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="BH10" s="34">
+      <c r="BJ10" s="34">
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I11" s="62"/>
       <c r="S11" s="27" t="s">
         <v>57</v>
@@ -1742,14 +1761,14 @@
       </c>
       <c r="AT11" s="18"/>
       <c r="AU11" s="18"/>
-      <c r="BG11" s="33" t="s">
+      <c r="BI11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BH11" s="34">
+      <c r="BJ11" s="34">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I12" s="62"/>
       <c r="S12" s="70" t="s">
         <v>128</v>
@@ -1775,14 +1794,14 @@
       </c>
       <c r="AT12" s="21"/>
       <c r="AU12" s="21"/>
-      <c r="BG12" s="33" t="s">
+      <c r="BI12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="BH12" s="34">
+      <c r="BJ12" s="34">
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I13" s="62"/>
       <c r="S13" s="27" t="s">
         <v>56</v>
@@ -1810,14 +1829,14 @@
       </c>
       <c r="AT13" s="16"/>
       <c r="AU13" s="16"/>
-      <c r="BG13" s="33" t="s">
+      <c r="BI13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="BH13" s="34">
+      <c r="BJ13" s="34">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I14" s="62"/>
       <c r="S14" s="27" t="s">
         <v>57</v>
@@ -1843,14 +1862,14 @@
       <c r="AR14" s="34">
         <v>2001</v>
       </c>
-      <c r="BG14" s="33" t="s">
+      <c r="BI14" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="BH14" s="34">
+      <c r="BJ14" s="34">
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I15" s="62"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
@@ -1870,14 +1889,14 @@
       <c r="AR15" s="34">
         <v>2100</v>
       </c>
-      <c r="BG15" s="33" t="s">
+      <c r="BI15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="BH15" s="34">
+      <c r="BJ15" s="34">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:62" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:64" x14ac:dyDescent="0.4">
       <c r="I16" s="62"/>
       <c r="S16" s="27" t="s">
         <v>126</v>
@@ -1903,14 +1922,14 @@
       <c r="AR16" s="34">
         <v>2101</v>
       </c>
-      <c r="BG16" s="33" t="s">
+      <c r="BI16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="BH16" s="34">
+      <c r="BJ16" s="34">
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="17" spans="9:62" x14ac:dyDescent="0.4">
       <c r="I17" s="62"/>
       <c r="S17" s="68" t="s">
         <v>125</v>
@@ -1940,14 +1959,14 @@
       <c r="AR17" s="34">
         <v>2200</v>
       </c>
-      <c r="BG17" s="33" t="s">
+      <c r="BI17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="BH17" s="34">
+      <c r="BJ17" s="34">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="18" spans="9:62" x14ac:dyDescent="0.4">
       <c r="I18" s="62"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
@@ -1967,14 +1986,14 @@
       <c r="AR18" s="34">
         <v>2201</v>
       </c>
-      <c r="BG18" s="33" t="s">
+      <c r="BI18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="BH18" s="34">
+      <c r="BJ18" s="34">
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="19" spans="9:62" x14ac:dyDescent="0.4">
       <c r="I19" s="62"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
@@ -1991,7 +2010,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="20" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="20" spans="9:62" x14ac:dyDescent="0.4">
       <c r="I20" s="62"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
@@ -2008,7 +2027,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="21" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="21" spans="9:62" x14ac:dyDescent="0.4">
       <c r="I21" s="62"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
@@ -2025,7 +2044,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="22" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="22" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
       <c r="AQ22" s="44" t="s">
@@ -2035,7 +2054,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="23" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="23" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM23" s="51" t="s">
         <v>119</v>
       </c>
@@ -2049,7 +2068,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="24" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
@@ -2065,7 +2084,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="25" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="25" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
@@ -2081,7 +2100,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="26" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="26" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
@@ -2091,13 +2110,13 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="27" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AO27" s="16"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="28" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM28" s="33" t="s">
         <v>21</v>
       </c>
@@ -2109,7 +2128,7 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="29" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM29" s="33" t="s">
         <v>22</v>
       </c>
@@ -2121,7 +2140,7 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="30" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM30" s="33" t="s">
         <v>23</v>
       </c>
@@ -2133,7 +2152,7 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="31" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM31" s="33" t="s">
         <v>24</v>
       </c>
@@ -2145,7 +2164,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" spans="9:60" x14ac:dyDescent="0.4">
+    <row r="32" spans="9:62" x14ac:dyDescent="0.4">
       <c r="AM32" s="33" t="s">
         <v>117</v>
       </c>
@@ -2208,7 +2227,7 @@
       <c r="AR37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2223,12 +2242,13 @@
     <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="S12:T12"/>
-    <mergeCell ref="BG4:BJ4"/>
-    <mergeCell ref="BG5:BJ5"/>
+    <mergeCell ref="BI4:BL4"/>
+    <mergeCell ref="BI5:BL5"/>
     <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="AU4:AV4"/>
     <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
     <mergeCell ref="AM23:AN23"/>
     <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="AS4:AT4"/>

</xml_diff>

<commit_message>
Push down Hidden Zone's postion a little bit
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8973F55A-E7C6-4F95-9C65-A3B8A876A212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4787683-0975-4077-8260-3090AA3BC1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -439,6 +439,18 @@
   </si>
   <si>
     <t>Crumb</t>
+  </si>
+  <si>
+    <t># Vertical Left</t>
+  </si>
+  <si>
+    <t># Vertical Right</t>
+  </si>
+  <si>
+    <t># Horizontal</t>
+  </si>
+  <si>
+    <t># Stairs</t>
   </si>
 </sst>
 </file>
@@ -776,6 +788,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,21 +828,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -810,28 +841,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1148,44 +1160,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BL37"/>
+  <dimension ref="B4:BL112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BE9" sqref="BE9"/>
+    <sheetView tabSelected="1" topLeftCell="W42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI109" sqref="AI109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.07421875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
     <col min="6" max="8" width="16" customWidth="1"/>
-    <col min="12" max="13" width="11.69140625" customWidth="1"/>
-    <col min="14" max="14" width="12.69140625" customWidth="1"/>
-    <col min="18" max="22" width="12.765625" customWidth="1"/>
-    <col min="23" max="23" width="12.3046875" customWidth="1"/>
-    <col min="25" max="25" width="17.53515625" customWidth="1"/>
-    <col min="26" max="26" width="8.84375" customWidth="1"/>
-    <col min="33" max="33" width="15.84375" customWidth="1"/>
-    <col min="35" max="35" width="13.07421875" customWidth="1"/>
-    <col min="37" max="37" width="10.4609375" customWidth="1"/>
-    <col min="39" max="39" width="20.4609375" customWidth="1"/>
-    <col min="40" max="40" width="9.23046875" customWidth="1"/>
-    <col min="41" max="41" width="20.4609375" customWidth="1"/>
-    <col min="43" max="43" width="20.765625" customWidth="1"/>
-    <col min="47" max="47" width="9.3046875" customWidth="1"/>
-    <col min="49" max="49" width="10.84375" customWidth="1"/>
-    <col min="51" max="51" width="9.765625" customWidth="1"/>
-    <col min="52" max="52" width="8.4609375" customWidth="1"/>
-    <col min="53" max="53" width="12.07421875" customWidth="1"/>
-    <col min="54" max="56" width="8.4609375" customWidth="1"/>
-    <col min="57" max="57" width="5.69140625" customWidth="1"/>
-    <col min="58" max="59" width="7.765625" customWidth="1"/>
-    <col min="60" max="60" width="11.69140625" customWidth="1"/>
-    <col min="61" max="62" width="13.4609375" customWidth="1"/>
-    <col min="63" max="63" width="13.07421875" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="18" max="22" width="12.77734375" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" customWidth="1"/>
+    <col min="35" max="35" width="13.109375" customWidth="1"/>
+    <col min="37" max="37" width="10.44140625" customWidth="1"/>
+    <col min="39" max="39" width="20.44140625" customWidth="1"/>
+    <col min="40" max="40" width="9.21875" customWidth="1"/>
+    <col min="41" max="41" width="20.44140625" customWidth="1"/>
+    <col min="43" max="43" width="20.77734375" customWidth="1"/>
+    <col min="47" max="47" width="9.33203125" customWidth="1"/>
+    <col min="49" max="49" width="10.88671875" customWidth="1"/>
+    <col min="51" max="51" width="9.77734375" customWidth="1"/>
+    <col min="52" max="52" width="8.44140625" customWidth="1"/>
+    <col min="53" max="53" width="12.109375" customWidth="1"/>
+    <col min="54" max="56" width="8.44140625" customWidth="1"/>
+    <col min="57" max="57" width="5.6640625" customWidth="1"/>
+    <col min="58" max="59" width="7.77734375" customWidth="1"/>
+    <col min="60" max="60" width="11.6640625" customWidth="1"/>
+    <col min="61" max="62" width="13.44140625" customWidth="1"/>
+    <col min="63" max="63" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:64" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:64" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1196,14 +1208,14 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65" t="s">
+      <c r="L4" s="59"/>
+      <c r="M4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="65"/>
+      <c r="N4" s="59"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1223,73 +1235,73 @@
         <v>47</v>
       </c>
       <c r="Z4" s="56"/>
-      <c r="AA4" s="54" t="s">
+      <c r="AA4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="54" t="s">
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="55"/>
-      <c r="AE4" s="54" t="s">
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="55"/>
-      <c r="AG4" s="54" t="s">
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="55"/>
-      <c r="AI4" s="54" t="s">
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="55"/>
-      <c r="AK4" s="54" t="s">
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="55"/>
-      <c r="AM4" s="57" t="s">
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59"/>
-      <c r="AR4" s="55"/>
-      <c r="AS4" s="54" t="s">
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="55"/>
-      <c r="AU4" s="54" t="s">
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="55"/>
-      <c r="AW4" s="54" t="s">
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="AX4" s="55"/>
-      <c r="AY4" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ4" s="55"/>
-      <c r="BA4" s="54" t="s">
+      <c r="AX4" s="58"/>
+      <c r="AY4" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="BB4" s="55"/>
-      <c r="BC4" s="54" t="s">
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="BD4" s="55"/>
+      <c r="BD4" s="58"/>
       <c r="BH4" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BI4" s="51" t="s">
+      <c r="BI4" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="BJ4" s="51"/>
-      <c r="BK4" s="51"/>
-      <c r="BL4" s="51"/>
-    </row>
-    <row r="5" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="62"/>
+    </row>
+    <row r="5" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1370,18 +1382,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="52" t="s">
+      <c r="AM5" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="53"/>
-      <c r="AO5" s="52" t="s">
+      <c r="AN5" s="64"/>
+      <c r="AO5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="53"/>
-      <c r="AQ5" s="60" t="s">
+      <c r="AP5" s="64"/>
+      <c r="AQ5" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="AR5" s="61"/>
+      <c r="AR5" s="68"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1421,21 +1433,21 @@
       <c r="BH5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="BI5" s="51" t="s">
+      <c r="BI5" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="51"/>
-    </row>
-    <row r="6" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="62"/>
+      <c r="BL5" s="62"/>
+    </row>
+    <row r="6" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="58" t="s">
+      <c r="I6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="63" t="s">
+      <c r="J6" s="54" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1559,15 +1571,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="64"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="55"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1625,12 +1637,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:64" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:64" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="64"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="55"/>
       <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1662,13 +1674,13 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I9" s="62"/>
-      <c r="J9" s="64"/>
-      <c r="S9" s="69" t="s">
+    <row r="9" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I9" s="53"/>
+      <c r="J9" s="55"/>
+      <c r="S9" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="T9" s="69"/>
+      <c r="T9" s="60"/>
       <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
@@ -1700,8 +1712,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I10" s="62"/>
+    <row r="10" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I10" s="53"/>
       <c r="S10" s="27" t="s">
         <v>56</v>
       </c>
@@ -1733,8 +1745,8 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I11" s="62"/>
+    <row r="11" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I11" s="53"/>
       <c r="S11" s="27" t="s">
         <v>57</v>
       </c>
@@ -1768,12 +1780,12 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I12" s="62"/>
-      <c r="S12" s="70" t="s">
+    <row r="12" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I12" s="53"/>
+      <c r="S12" s="61" t="s">
         <v>128</v>
       </c>
-      <c r="T12" s="70"/>
+      <c r="T12" s="61"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1801,8 +1813,8 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I13" s="62"/>
+    <row r="13" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I13" s="53"/>
       <c r="S13" s="27" t="s">
         <v>56</v>
       </c>
@@ -1836,8 +1848,8 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I14" s="62"/>
+    <row r="14" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I14" s="53"/>
       <c r="S14" s="27" t="s">
         <v>57</v>
       </c>
@@ -1869,8 +1881,8 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I15" s="62"/>
+    <row r="15" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I15" s="53"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
       </c>
@@ -1896,8 +1908,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:64" x14ac:dyDescent="0.4">
-      <c r="I16" s="62"/>
+    <row r="16" spans="2:64" x14ac:dyDescent="0.3">
+      <c r="I16" s="53"/>
       <c r="S16" s="27" t="s">
         <v>126</v>
       </c>
@@ -1929,12 +1941,12 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="I17" s="62"/>
-      <c r="S17" s="68" t="s">
+    <row r="17" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="I17" s="53"/>
+      <c r="S17" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="T17" s="68">
+      <c r="T17" s="51">
         <v>6021</v>
       </c>
       <c r="AG17" s="43"/>
@@ -1966,8 +1978,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="I18" s="62"/>
+    <row r="18" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="I18" s="53"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
       </c>
@@ -1993,8 +2005,8 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="I19" s="62"/>
+    <row r="19" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="I19" s="53"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
       </c>
@@ -2010,8 +2022,8 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="20" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="I20" s="62"/>
+    <row r="20" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="I20" s="53"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
       </c>
@@ -2027,8 +2039,8 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="21" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="I21" s="62"/>
+    <row r="21" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="I21" s="53"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2056,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="22" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="22" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
       <c r="AQ22" s="44" t="s">
@@ -2054,11 +2066,11 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="23" spans="9:62" x14ac:dyDescent="0.4">
-      <c r="AM23" s="51" t="s">
+    <row r="23" spans="9:62" x14ac:dyDescent="0.3">
+      <c r="AM23" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="AN23" s="51"/>
+      <c r="AN23" s="62"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
       <c r="AQ23" s="47" t="s">
@@ -2068,7 +2080,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="24" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="25" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="25" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="26" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="26" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
@@ -2110,13 +2122,13 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="27" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AO27" s="16"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="28" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM28" s="33" t="s">
         <v>21</v>
       </c>
@@ -2128,7 +2140,7 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="29" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM29" s="33" t="s">
         <v>22</v>
       </c>
@@ -2140,7 +2152,7 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="30" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM30" s="33" t="s">
         <v>23</v>
       </c>
@@ -2152,7 +2164,7 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="31" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM31" s="33" t="s">
         <v>24</v>
       </c>
@@ -2164,7 +2176,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" spans="9:62" x14ac:dyDescent="0.4">
+    <row r="32" spans="9:62" x14ac:dyDescent="0.3">
       <c r="AM32" s="33" t="s">
         <v>117</v>
       </c>
@@ -2176,7 +2188,7 @@
       <c r="AQ32" s="16"/>
       <c r="AR32" s="16"/>
     </row>
-    <row r="33" spans="39:44" x14ac:dyDescent="0.4">
+    <row r="33" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AM33" s="33" t="s">
         <v>118</v>
       </c>
@@ -2188,7 +2200,7 @@
       <c r="AQ33" s="16"/>
       <c r="AR33" s="16"/>
     </row>
-    <row r="34" spans="39:44" x14ac:dyDescent="0.4">
+    <row r="34" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AM34" s="33" t="s">
         <v>27</v>
       </c>
@@ -2200,7 +2212,7 @@
       <c r="AQ34" s="16"/>
       <c r="AR34" s="16"/>
     </row>
-    <row r="35" spans="39:44" x14ac:dyDescent="0.4">
+    <row r="35" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AM35" s="33" t="s">
         <v>28</v>
       </c>
@@ -2212,7 +2224,7 @@
       <c r="AQ35" s="31"/>
       <c r="AR35" s="31"/>
     </row>
-    <row r="36" spans="39:44" x14ac:dyDescent="0.4">
+    <row r="36" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AM36" s="33"/>
       <c r="AN36" s="34"/>
       <c r="AO36" s="19"/>
@@ -2220,14 +2232,1049 @@
       <c r="AQ36" s="19"/>
       <c r="AR36" s="19"/>
     </row>
-    <row r="37" spans="39:44" x14ac:dyDescent="0.4">
+    <row r="37" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AO37" s="19"/>
       <c r="AP37" s="19"/>
       <c r="AQ37" s="19"/>
       <c r="AR37" s="19"/>
     </row>
+    <row r="49" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB50">
+        <v>1</v>
+      </c>
+      <c r="AC50">
+        <v>2079</v>
+      </c>
+      <c r="AD50">
+        <v>433</v>
+      </c>
+      <c r="AG50">
+        <v>1</v>
+      </c>
+      <c r="AH50">
+        <f xml:space="preserve"> AC50</f>
+        <v>2079</v>
+      </c>
+      <c r="AI50">
+        <f>AD50+16*4</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="51" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB51">
+        <v>1</v>
+      </c>
+      <c r="AC51">
+        <v>2079</v>
+      </c>
+      <c r="AD51">
+        <v>449</v>
+      </c>
+      <c r="AG51">
+        <v>1</v>
+      </c>
+      <c r="AH51">
+        <v>2079</v>
+      </c>
+      <c r="AI51">
+        <f t="shared" ref="AI51:AI112" si="0">AD51+16*4</f>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="52" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB52">
+        <v>1</v>
+      </c>
+      <c r="AC52">
+        <v>2079</v>
+      </c>
+      <c r="AD52">
+        <v>465</v>
+      </c>
+      <c r="AG52">
+        <v>1</v>
+      </c>
+      <c r="AH52">
+        <v>2079</v>
+      </c>
+      <c r="AI52">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="53" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB53">
+        <v>1</v>
+      </c>
+      <c r="AC53">
+        <v>2079</v>
+      </c>
+      <c r="AD53">
+        <v>481</v>
+      </c>
+      <c r="AG53">
+        <v>1</v>
+      </c>
+      <c r="AH53">
+        <v>2079</v>
+      </c>
+      <c r="AI53">
+        <f t="shared" si="0"/>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB54">
+        <v>1</v>
+      </c>
+      <c r="AC54">
+        <v>2079</v>
+      </c>
+      <c r="AD54">
+        <v>497</v>
+      </c>
+      <c r="AG54">
+        <v>1</v>
+      </c>
+      <c r="AH54">
+        <v>2079</v>
+      </c>
+      <c r="AI54">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="56" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB56">
+        <v>1</v>
+      </c>
+      <c r="AC56">
+        <v>2079</v>
+      </c>
+      <c r="AD56">
+        <v>513</v>
+      </c>
+      <c r="AG56">
+        <v>1</v>
+      </c>
+      <c r="AH56">
+        <v>2079</v>
+      </c>
+      <c r="AI56">
+        <f t="shared" si="0"/>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="57" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB57">
+        <v>1</v>
+      </c>
+      <c r="AC57">
+        <v>2079</v>
+      </c>
+      <c r="AD57">
+        <v>529</v>
+      </c>
+      <c r="AG57">
+        <v>1</v>
+      </c>
+      <c r="AH57">
+        <v>2079</v>
+      </c>
+      <c r="AI57">
+        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="58" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB58">
+        <v>1</v>
+      </c>
+      <c r="AC58">
+        <v>2079</v>
+      </c>
+      <c r="AD58">
+        <v>545</v>
+      </c>
+      <c r="AG58">
+        <v>1</v>
+      </c>
+      <c r="AH58">
+        <v>2079</v>
+      </c>
+      <c r="AI58">
+        <f t="shared" si="0"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="59" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB59">
+        <v>1</v>
+      </c>
+      <c r="AC59">
+        <v>2079</v>
+      </c>
+      <c r="AD59">
+        <v>561</v>
+      </c>
+      <c r="AG59">
+        <v>1</v>
+      </c>
+      <c r="AH59">
+        <v>2079</v>
+      </c>
+      <c r="AI59">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="60" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB60">
+        <v>1</v>
+      </c>
+      <c r="AC60">
+        <v>2079</v>
+      </c>
+      <c r="AD60">
+        <v>577</v>
+      </c>
+      <c r="AG60">
+        <v>1</v>
+      </c>
+      <c r="AH60">
+        <v>2079</v>
+      </c>
+      <c r="AI60">
+        <f t="shared" si="0"/>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="62" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG62" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB63">
+        <v>1</v>
+      </c>
+      <c r="AC63">
+        <v>2351</v>
+      </c>
+      <c r="AD63">
+        <v>433</v>
+      </c>
+      <c r="AG63">
+        <v>1</v>
+      </c>
+      <c r="AH63">
+        <v>2351</v>
+      </c>
+      <c r="AI63">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="64" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB64">
+        <v>1</v>
+      </c>
+      <c r="AC64">
+        <v>2351</v>
+      </c>
+      <c r="AD64">
+        <v>449</v>
+      </c>
+      <c r="AG64">
+        <v>1</v>
+      </c>
+      <c r="AH64">
+        <v>2351</v>
+      </c>
+      <c r="AI64">
+        <f t="shared" si="0"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB65">
+        <v>1</v>
+      </c>
+      <c r="AC65">
+        <v>2351</v>
+      </c>
+      <c r="AD65">
+        <v>465</v>
+      </c>
+      <c r="AG65">
+        <v>1</v>
+      </c>
+      <c r="AH65">
+        <v>2351</v>
+      </c>
+      <c r="AI65">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="66" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB66">
+        <v>1</v>
+      </c>
+      <c r="AC66">
+        <v>2351</v>
+      </c>
+      <c r="AD66">
+        <v>481</v>
+      </c>
+      <c r="AG66">
+        <v>1</v>
+      </c>
+      <c r="AH66">
+        <v>2351</v>
+      </c>
+      <c r="AI66">
+        <f t="shared" si="0"/>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="67" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB67">
+        <v>1</v>
+      </c>
+      <c r="AC67">
+        <v>2351</v>
+      </c>
+      <c r="AD67">
+        <v>497</v>
+      </c>
+      <c r="AG67">
+        <v>1</v>
+      </c>
+      <c r="AH67">
+        <v>2351</v>
+      </c>
+      <c r="AI67">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="68" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB68">
+        <v>1</v>
+      </c>
+      <c r="AC68">
+        <v>2367</v>
+      </c>
+      <c r="AD68">
+        <v>433</v>
+      </c>
+      <c r="AG68">
+        <v>1</v>
+      </c>
+      <c r="AH68">
+        <v>2367</v>
+      </c>
+      <c r="AI68">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="69" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB69">
+        <v>1</v>
+      </c>
+      <c r="AC69">
+        <v>2367</v>
+      </c>
+      <c r="AD69">
+        <v>449</v>
+      </c>
+      <c r="AG69">
+        <v>1</v>
+      </c>
+      <c r="AH69">
+        <v>2367</v>
+      </c>
+      <c r="AI69">
+        <f t="shared" si="0"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="70" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB70">
+        <v>1</v>
+      </c>
+      <c r="AC70">
+        <v>2367</v>
+      </c>
+      <c r="AD70">
+        <v>465</v>
+      </c>
+      <c r="AG70">
+        <v>1</v>
+      </c>
+      <c r="AH70">
+        <v>2367</v>
+      </c>
+      <c r="AI70">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="71" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB71">
+        <v>1</v>
+      </c>
+      <c r="AC71">
+        <v>2367</v>
+      </c>
+      <c r="AD71">
+        <v>481</v>
+      </c>
+      <c r="AG71">
+        <v>1</v>
+      </c>
+      <c r="AH71">
+        <v>2367</v>
+      </c>
+      <c r="AI71">
+        <f t="shared" si="0"/>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="72" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB72">
+        <v>1</v>
+      </c>
+      <c r="AC72">
+        <v>2367</v>
+      </c>
+      <c r="AD72">
+        <v>497</v>
+      </c>
+      <c r="AG72">
+        <v>1</v>
+      </c>
+      <c r="AH72">
+        <v>2367</v>
+      </c>
+      <c r="AI72">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="75" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB75" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB76">
+        <v>1</v>
+      </c>
+      <c r="AC76">
+        <v>2127</v>
+      </c>
+      <c r="AD76">
+        <v>433</v>
+      </c>
+      <c r="AG76">
+        <v>1</v>
+      </c>
+      <c r="AH76">
+        <v>2127</v>
+      </c>
+      <c r="AI76">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="77" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB77">
+        <v>1</v>
+      </c>
+      <c r="AC77">
+        <v>2143</v>
+      </c>
+      <c r="AD77">
+        <v>433</v>
+      </c>
+      <c r="AG77">
+        <v>1</v>
+      </c>
+      <c r="AH77">
+        <v>2143</v>
+      </c>
+      <c r="AI77">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="78" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB78">
+        <v>1</v>
+      </c>
+      <c r="AC78">
+        <v>2159</v>
+      </c>
+      <c r="AD78">
+        <v>433</v>
+      </c>
+      <c r="AG78">
+        <v>1</v>
+      </c>
+      <c r="AH78">
+        <v>2159</v>
+      </c>
+      <c r="AI78">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="79" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB79">
+        <v>1</v>
+      </c>
+      <c r="AC79">
+        <v>2175</v>
+      </c>
+      <c r="AD79">
+        <v>433</v>
+      </c>
+      <c r="AG79">
+        <v>1</v>
+      </c>
+      <c r="AH79">
+        <v>2175</v>
+      </c>
+      <c r="AI79">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="80" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB80">
+        <v>1</v>
+      </c>
+      <c r="AC80">
+        <v>2191</v>
+      </c>
+      <c r="AD80">
+        <v>433</v>
+      </c>
+      <c r="AG80">
+        <v>1</v>
+      </c>
+      <c r="AH80">
+        <v>2191</v>
+      </c>
+      <c r="AI80">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="82" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB82">
+        <v>1</v>
+      </c>
+      <c r="AC82">
+        <v>2207</v>
+      </c>
+      <c r="AD82">
+        <v>433</v>
+      </c>
+      <c r="AG82">
+        <v>1</v>
+      </c>
+      <c r="AH82">
+        <v>2207</v>
+      </c>
+      <c r="AI82">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="83" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB83">
+        <v>1</v>
+      </c>
+      <c r="AC83">
+        <v>2223</v>
+      </c>
+      <c r="AD83">
+        <v>433</v>
+      </c>
+      <c r="AG83">
+        <v>1</v>
+      </c>
+      <c r="AH83">
+        <v>2223</v>
+      </c>
+      <c r="AI83">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="84" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB84">
+        <v>1</v>
+      </c>
+      <c r="AC84">
+        <v>2239</v>
+      </c>
+      <c r="AD84">
+        <v>433</v>
+      </c>
+      <c r="AG84">
+        <v>1</v>
+      </c>
+      <c r="AH84">
+        <v>2239</v>
+      </c>
+      <c r="AI84">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="85" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB85">
+        <v>1</v>
+      </c>
+      <c r="AC85">
+        <v>2255</v>
+      </c>
+      <c r="AD85">
+        <v>433</v>
+      </c>
+      <c r="AG85">
+        <v>1</v>
+      </c>
+      <c r="AH85">
+        <v>2255</v>
+      </c>
+      <c r="AI85">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="86" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB86">
+        <v>1</v>
+      </c>
+      <c r="AC86">
+        <v>2271</v>
+      </c>
+      <c r="AD86">
+        <v>433</v>
+      </c>
+      <c r="AG86">
+        <v>1</v>
+      </c>
+      <c r="AH86">
+        <v>2271</v>
+      </c>
+      <c r="AI86">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="88" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB88">
+        <v>1</v>
+      </c>
+      <c r="AC88">
+        <v>2287</v>
+      </c>
+      <c r="AD88">
+        <v>433</v>
+      </c>
+      <c r="AG88">
+        <v>1</v>
+      </c>
+      <c r="AH88">
+        <v>2287</v>
+      </c>
+      <c r="AI88">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="89" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB89">
+        <v>1</v>
+      </c>
+      <c r="AC89">
+        <v>2303</v>
+      </c>
+      <c r="AD89">
+        <v>433</v>
+      </c>
+      <c r="AG89">
+        <v>1</v>
+      </c>
+      <c r="AH89">
+        <v>2303</v>
+      </c>
+      <c r="AI89">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="91" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB91">
+        <v>1</v>
+      </c>
+      <c r="AC91">
+        <v>2351</v>
+      </c>
+      <c r="AD91">
+        <v>433</v>
+      </c>
+      <c r="AG91">
+        <v>1</v>
+      </c>
+      <c r="AH91">
+        <v>2351</v>
+      </c>
+      <c r="AI91">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="92" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB92">
+        <v>1</v>
+      </c>
+      <c r="AC92">
+        <v>2367</v>
+      </c>
+      <c r="AD92">
+        <v>433</v>
+      </c>
+      <c r="AG92">
+        <v>1</v>
+      </c>
+      <c r="AH92">
+        <v>2367</v>
+      </c>
+      <c r="AI92">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="94" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB94" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG94" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB95">
+        <v>1</v>
+      </c>
+      <c r="AC95">
+        <v>2223</v>
+      </c>
+      <c r="AD95">
+        <v>577</v>
+      </c>
+      <c r="AG95">
+        <v>1</v>
+      </c>
+      <c r="AH95">
+        <v>2223</v>
+      </c>
+      <c r="AI95">
+        <f t="shared" si="0"/>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="96" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB96">
+        <v>1</v>
+      </c>
+      <c r="AC96">
+        <v>2239</v>
+      </c>
+      <c r="AD96">
+        <v>577</v>
+      </c>
+      <c r="AG96">
+        <v>1</v>
+      </c>
+      <c r="AH96">
+        <v>2239</v>
+      </c>
+      <c r="AI96">
+        <f t="shared" si="0"/>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="98" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB98">
+        <v>1</v>
+      </c>
+      <c r="AC98">
+        <v>2239</v>
+      </c>
+      <c r="AD98">
+        <v>561</v>
+      </c>
+      <c r="AG98">
+        <v>1</v>
+      </c>
+      <c r="AH98">
+        <v>2239</v>
+      </c>
+      <c r="AI98">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="99" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB99">
+        <v>1</v>
+      </c>
+      <c r="AC99">
+        <v>2255</v>
+      </c>
+      <c r="AD99">
+        <v>561</v>
+      </c>
+      <c r="AG99">
+        <v>1</v>
+      </c>
+      <c r="AH99">
+        <v>2255</v>
+      </c>
+      <c r="AI99">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="101" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB101">
+        <v>1</v>
+      </c>
+      <c r="AC101">
+        <v>2255</v>
+      </c>
+      <c r="AD101">
+        <v>545</v>
+      </c>
+      <c r="AG101">
+        <v>1</v>
+      </c>
+      <c r="AH101">
+        <v>2255</v>
+      </c>
+      <c r="AI101">
+        <f t="shared" si="0"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="102" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB102">
+        <v>1</v>
+      </c>
+      <c r="AC102">
+        <v>2271</v>
+      </c>
+      <c r="AD102">
+        <v>545</v>
+      </c>
+      <c r="AG102">
+        <v>1</v>
+      </c>
+      <c r="AH102">
+        <v>2271</v>
+      </c>
+      <c r="AI102">
+        <f t="shared" si="0"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="104" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB104">
+        <v>1</v>
+      </c>
+      <c r="AC104">
+        <v>2271</v>
+      </c>
+      <c r="AD104">
+        <v>529</v>
+      </c>
+      <c r="AG104">
+        <v>1</v>
+      </c>
+      <c r="AH104">
+        <v>2271</v>
+      </c>
+      <c r="AI104">
+        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="105" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB105">
+        <v>1</v>
+      </c>
+      <c r="AC105">
+        <v>2287</v>
+      </c>
+      <c r="AD105">
+        <v>529</v>
+      </c>
+      <c r="AG105">
+        <v>1</v>
+      </c>
+      <c r="AH105">
+        <v>2287</v>
+      </c>
+      <c r="AI105">
+        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="107" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB107">
+        <v>1</v>
+      </c>
+      <c r="AC107">
+        <v>2287</v>
+      </c>
+      <c r="AD107">
+        <v>513</v>
+      </c>
+      <c r="AG107">
+        <v>1</v>
+      </c>
+      <c r="AH107">
+        <v>2287</v>
+      </c>
+      <c r="AI107">
+        <f t="shared" si="0"/>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="108" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB108">
+        <v>1</v>
+      </c>
+      <c r="AC108">
+        <v>2303</v>
+      </c>
+      <c r="AD108">
+        <v>513</v>
+      </c>
+      <c r="AG108">
+        <v>1</v>
+      </c>
+      <c r="AH108">
+        <v>2303</v>
+      </c>
+      <c r="AI108">
+        <f t="shared" si="0"/>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="110" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB110">
+        <v>1</v>
+      </c>
+      <c r="AC110">
+        <v>2303</v>
+      </c>
+      <c r="AD110">
+        <v>497</v>
+      </c>
+      <c r="AG110">
+        <v>1</v>
+      </c>
+      <c r="AH110">
+        <v>2303</v>
+      </c>
+      <c r="AI110">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="111" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB111">
+        <v>1</v>
+      </c>
+      <c r="AC111">
+        <v>2319</v>
+      </c>
+      <c r="AD111">
+        <v>497</v>
+      </c>
+      <c r="AG111">
+        <v>1</v>
+      </c>
+      <c r="AH111">
+        <v>2319</v>
+      </c>
+      <c r="AI111">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="112" spans="28:35" x14ac:dyDescent="0.3">
+      <c r="AB112">
+        <v>1</v>
+      </c>
+      <c r="AC112">
+        <v>2335</v>
+      </c>
+      <c r="AD112">
+        <v>497</v>
+      </c>
+      <c r="AG112">
+        <v>1</v>
+      </c>
+      <c r="AH112">
+        <v>2335</v>
+      </c>
+      <c r="AI112">
+        <f t="shared" si="0"/>
+        <v>561</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BI4:BL4"/>
+    <mergeCell ref="BI5:BL5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2242,21 +3289,6 @@
     <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="S12:T12"/>
-    <mergeCell ref="BI4:BL4"/>
-    <mergeCell ref="BI5:BL5"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AR4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AI4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2271,35 +3303,35 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.69140625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="11.69140625" customWidth="1"/>
-    <col min="7" max="7" width="16.3046875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B1" s="51" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="66" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
@@ -2322,7 +3354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -2343,7 +3375,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -2362,7 +3394,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -2381,7 +3413,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>4</v>
       </c>
@@ -2404,7 +3436,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -2425,7 +3457,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="39">
         <v>6</v>
       </c>
@@ -2444,7 +3476,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="39">
         <v>7</v>
       </c>
@@ -2463,7 +3495,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>8</v>
       </c>
@@ -2482,61 +3514,61 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -2560,26 +3592,26 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.84375" customWidth="1"/>
-    <col min="3" max="3" width="23.69140625" customWidth="1"/>
-    <col min="4" max="4" width="56.23046875" customWidth="1"/>
-    <col min="5" max="5" width="12.23046875" customWidth="1"/>
-    <col min="6" max="6" width="15.07421875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="67" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>65</v>
       </c>
@@ -2593,7 +3625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -2605,7 +3637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -2617,7 +3649,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="23" t="s">
         <v>89</v>
       </c>
@@ -2638,19 +3670,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.23046875" style="37"/>
-    <col min="3" max="3" width="40.84375" customWidth="1"/>
-    <col min="4" max="4" width="55.23046875" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="37"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="55.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="38" t="s">
         <v>65</v>
       </c>
@@ -2661,7 +3693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="42">
         <v>1</v>
       </c>
@@ -2672,7 +3704,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="42">
         <v>2</v>
       </c>
@@ -2683,47 +3715,47 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="42"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="42"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="42"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="42"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="42"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="42"/>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="42"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="42"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="42"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>

</xml_diff>

<commit_message>
Create HUD obejct with basic features: render, atached to camera's position
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4787683-0975-4077-8260-3090AA3BC1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC88A81-919C-4F12-98DB-A59659AC995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="131">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -441,16 +441,7 @@
     <t>Crumb</t>
   </si>
   <si>
-    <t># Vertical Left</t>
-  </si>
-  <si>
-    <t># Vertical Right</t>
-  </si>
-  <si>
-    <t># Horizontal</t>
-  </si>
-  <si>
-    <t># Stairs</t>
+    <t>HUD</t>
   </si>
 </sst>
 </file>
@@ -789,9 +780,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -802,42 +823,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1160,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BL112"/>
+  <dimension ref="B4:BN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI109" sqref="AI109"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BF6" sqref="BF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,15 +1180,15 @@
     <col min="51" max="51" width="9.77734375" customWidth="1"/>
     <col min="52" max="52" width="8.44140625" customWidth="1"/>
     <col min="53" max="53" width="12.109375" customWidth="1"/>
-    <col min="54" max="56" width="8.44140625" customWidth="1"/>
-    <col min="57" max="57" width="5.6640625" customWidth="1"/>
-    <col min="58" max="59" width="7.77734375" customWidth="1"/>
-    <col min="60" max="60" width="11.6640625" customWidth="1"/>
-    <col min="61" max="62" width="13.44140625" customWidth="1"/>
-    <col min="63" max="63" width="13.109375" customWidth="1"/>
+    <col min="54" max="58" width="8.44140625" customWidth="1"/>
+    <col min="59" max="59" width="5.6640625" customWidth="1"/>
+    <col min="60" max="61" width="7.77734375" customWidth="1"/>
+    <col min="62" max="62" width="11.6640625" customWidth="1"/>
+    <col min="63" max="64" width="13.44140625" customWidth="1"/>
+    <col min="65" max="65" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,100 +1199,104 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59" t="s">
+      <c r="L4" s="66"/>
+      <c r="M4" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="59"/>
+      <c r="N4" s="66"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="56" t="s">
+      <c r="S4" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56" t="s">
+      <c r="T4" s="57"/>
+      <c r="U4" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56" t="s">
+      <c r="V4" s="57"/>
+      <c r="W4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56" t="s">
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="57" t="s">
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="57" t="s">
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="57" t="s">
+      <c r="AD4" s="56"/>
+      <c r="AE4" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="57" t="s">
+      <c r="AF4" s="56"/>
+      <c r="AG4" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="57" t="s">
+      <c r="AH4" s="56"/>
+      <c r="AI4" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="57" t="s">
+      <c r="AJ4" s="56"/>
+      <c r="AK4" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="65" t="s">
+      <c r="AL4" s="56"/>
+      <c r="AM4" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="58"/>
-      <c r="AS4" s="57" t="s">
+      <c r="AN4" s="59"/>
+      <c r="AO4" s="60"/>
+      <c r="AP4" s="60"/>
+      <c r="AQ4" s="60"/>
+      <c r="AR4" s="56"/>
+      <c r="AS4" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="57" t="s">
+      <c r="AT4" s="56"/>
+      <c r="AU4" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="57" t="s">
+      <c r="AV4" s="56"/>
+      <c r="AW4" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="AX4" s="58"/>
-      <c r="AY4" s="57" t="s">
+      <c r="AX4" s="56"/>
+      <c r="AY4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="57" t="s">
+      <c r="AZ4" s="56"/>
+      <c r="BA4" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="57" t="s">
+      <c r="BB4" s="56"/>
+      <c r="BC4" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="BD4" s="58"/>
-      <c r="BH4" s="35" t="s">
+      <c r="BD4" s="56"/>
+      <c r="BE4" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF4" s="56"/>
+      <c r="BJ4" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BI4" s="62" t="s">
+      <c r="BK4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="BJ4" s="62"/>
-      <c r="BK4" s="62"/>
-      <c r="BL4" s="62"/>
-    </row>
-    <row r="5" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BL4" s="52"/>
+      <c r="BM4" s="52"/>
+      <c r="BN4" s="52"/>
+    </row>
+    <row r="5" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1382,18 +1377,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="63" t="s">
+      <c r="AM5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="64"/>
-      <c r="AO5" s="63" t="s">
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="64"/>
-      <c r="AQ5" s="67" t="s">
+      <c r="AP5" s="54"/>
+      <c r="AQ5" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="AR5" s="68"/>
+      <c r="AR5" s="62"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1430,24 +1425,30 @@
       <c r="BD5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BH5" s="35" t="s">
+      <c r="BE5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="BI5" s="62" t="s">
+      <c r="BK5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="BJ5" s="62"/>
-      <c r="BK5" s="62"/>
-      <c r="BL5" s="62"/>
-    </row>
-    <row r="6" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BL5" s="52"/>
+      <c r="BM5" s="52"/>
+      <c r="BN5" s="52"/>
+    </row>
+    <row r="6" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="64" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1558,28 +1559,34 @@
       <c r="BD6" s="9">
         <v>15000</v>
       </c>
-      <c r="BI6" s="36" t="s">
+      <c r="BE6" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF6" s="9">
+        <v>16000</v>
+      </c>
+      <c r="BK6" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="BJ6" s="36" t="s">
+      <c r="BL6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="BK6" s="30" t="s">
+      <c r="BM6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="BL6" s="30" t="s">
+      <c r="BN6" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="55"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="65"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1627,22 +1634,22 @@
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
-      <c r="BI7" s="33" t="s">
+      <c r="BK7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="BJ7" s="34">
+      <c r="BL7" s="34">
         <v>1100</v>
       </c>
-      <c r="BK7">
+      <c r="BM7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="55"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="65"/>
       <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1667,20 +1674,20 @@
       <c r="AR8" s="34">
         <v>1710</v>
       </c>
-      <c r="BI8" s="33" t="s">
+      <c r="BK8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="BJ8" s="34">
+      <c r="BL8" s="34">
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I9" s="53"/>
-      <c r="J9" s="55"/>
-      <c r="S9" s="60" t="s">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I9" s="63"/>
+      <c r="J9" s="65"/>
+      <c r="S9" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="T9" s="60"/>
+      <c r="T9" s="67"/>
       <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
@@ -1705,15 +1712,15 @@
       <c r="AR9" s="34">
         <v>1800</v>
       </c>
-      <c r="BI9" s="33" t="s">
+      <c r="BK9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="BJ9" s="34">
+      <c r="BL9" s="34">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I10" s="53"/>
+    <row r="10" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I10" s="63"/>
       <c r="S10" s="27" t="s">
         <v>56</v>
       </c>
@@ -1738,15 +1745,15 @@
       <c r="AR10" s="34">
         <v>1801</v>
       </c>
-      <c r="BI10" s="33" t="s">
+      <c r="BK10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="BJ10" s="34">
+      <c r="BL10" s="34">
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I11" s="53"/>
+    <row r="11" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I11" s="63"/>
       <c r="S11" s="27" t="s">
         <v>57</v>
       </c>
@@ -1773,19 +1780,19 @@
       </c>
       <c r="AT11" s="18"/>
       <c r="AU11" s="18"/>
-      <c r="BI11" s="33" t="s">
+      <c r="BK11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BJ11" s="34">
+      <c r="BL11" s="34">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I12" s="53"/>
-      <c r="S12" s="61" t="s">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I12" s="63"/>
+      <c r="S12" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="T12" s="61"/>
+      <c r="T12" s="68"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1806,15 +1813,15 @@
       </c>
       <c r="AT12" s="21"/>
       <c r="AU12" s="21"/>
-      <c r="BI12" s="33" t="s">
+      <c r="BK12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="BJ12" s="34">
+      <c r="BL12" s="34">
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I13" s="53"/>
+    <row r="13" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I13" s="63"/>
       <c r="S13" s="27" t="s">
         <v>56</v>
       </c>
@@ -1841,15 +1848,15 @@
       </c>
       <c r="AT13" s="16"/>
       <c r="AU13" s="16"/>
-      <c r="BI13" s="33" t="s">
+      <c r="BK13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="BJ13" s="34">
+      <c r="BL13" s="34">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I14" s="53"/>
+    <row r="14" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I14" s="63"/>
       <c r="S14" s="27" t="s">
         <v>57</v>
       </c>
@@ -1874,15 +1881,15 @@
       <c r="AR14" s="34">
         <v>2001</v>
       </c>
-      <c r="BI14" s="33" t="s">
+      <c r="BK14" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="BJ14" s="34">
+      <c r="BL14" s="34">
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I15" s="53"/>
+    <row r="15" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I15" s="63"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
       </c>
@@ -1901,15 +1908,15 @@
       <c r="AR15" s="34">
         <v>2100</v>
       </c>
-      <c r="BI15" s="33" t="s">
+      <c r="BK15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="BJ15" s="34">
+      <c r="BL15" s="34">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:64" x14ac:dyDescent="0.3">
-      <c r="I16" s="53"/>
+    <row r="16" spans="2:66" x14ac:dyDescent="0.3">
+      <c r="I16" s="63"/>
       <c r="S16" s="27" t="s">
         <v>126</v>
       </c>
@@ -1934,15 +1941,15 @@
       <c r="AR16" s="34">
         <v>2101</v>
       </c>
-      <c r="BI16" s="33" t="s">
+      <c r="BK16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="BJ16" s="34">
+      <c r="BL16" s="34">
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="I17" s="53"/>
+    <row r="17" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="I17" s="63"/>
       <c r="S17" s="51" t="s">
         <v>125</v>
       </c>
@@ -1971,15 +1978,15 @@
       <c r="AR17" s="34">
         <v>2200</v>
       </c>
-      <c r="BI17" s="33" t="s">
+      <c r="BK17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="BJ17" s="34">
+      <c r="BL17" s="34">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="I18" s="53"/>
+    <row r="18" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="I18" s="63"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
       </c>
@@ -1998,15 +2005,15 @@
       <c r="AR18" s="34">
         <v>2201</v>
       </c>
-      <c r="BI18" s="33" t="s">
+      <c r="BK18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="BJ18" s="34">
+      <c r="BL18" s="34">
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="I19" s="53"/>
+    <row r="19" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="I19" s="63"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
       </c>
@@ -2022,8 +2029,8 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="20" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="I20" s="53"/>
+    <row r="20" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="I20" s="63"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
       </c>
@@ -2039,8 +2046,8 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="21" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="I21" s="53"/>
+    <row r="21" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="I21" s="63"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2063,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="22" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
       <c r="AQ22" s="44" t="s">
@@ -2066,11 +2073,11 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="23" spans="9:62" x14ac:dyDescent="0.3">
-      <c r="AM23" s="62" t="s">
+    <row r="23" spans="9:64" x14ac:dyDescent="0.3">
+      <c r="AM23" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="AN23" s="62"/>
+      <c r="AN23" s="52"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
       <c r="AQ23" s="47" t="s">
@@ -2080,7 +2087,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="24" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
@@ -2096,7 +2103,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="25" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
@@ -2112,7 +2119,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="26" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="26" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
@@ -2122,13 +2129,13 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="27" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AO27" s="16"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM28" s="33" t="s">
         <v>21</v>
       </c>
@@ -2140,7 +2147,7 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="29" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM29" s="33" t="s">
         <v>22</v>
       </c>
@@ -2152,7 +2159,7 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="30" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM30" s="33" t="s">
         <v>23</v>
       </c>
@@ -2164,7 +2171,7 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="31" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM31" s="33" t="s">
         <v>24</v>
       </c>
@@ -2176,7 +2183,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" spans="9:62" x14ac:dyDescent="0.3">
+    <row r="32" spans="9:64" x14ac:dyDescent="0.3">
       <c r="AM32" s="33" t="s">
         <v>117</v>
       </c>
@@ -2238,1043 +2245,8 @@
       <c r="AQ37" s="19"/>
       <c r="AR37" s="19"/>
     </row>
-    <row r="49" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB49" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB50">
-        <v>1</v>
-      </c>
-      <c r="AC50">
-        <v>2079</v>
-      </c>
-      <c r="AD50">
-        <v>433</v>
-      </c>
-      <c r="AG50">
-        <v>1</v>
-      </c>
-      <c r="AH50">
-        <f xml:space="preserve"> AC50</f>
-        <v>2079</v>
-      </c>
-      <c r="AI50">
-        <f>AD50+16*4</f>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="51" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB51">
-        <v>1</v>
-      </c>
-      <c r="AC51">
-        <v>2079</v>
-      </c>
-      <c r="AD51">
-        <v>449</v>
-      </c>
-      <c r="AG51">
-        <v>1</v>
-      </c>
-      <c r="AH51">
-        <v>2079</v>
-      </c>
-      <c r="AI51">
-        <f t="shared" ref="AI51:AI112" si="0">AD51+16*4</f>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="52" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB52">
-        <v>1</v>
-      </c>
-      <c r="AC52">
-        <v>2079</v>
-      </c>
-      <c r="AD52">
-        <v>465</v>
-      </c>
-      <c r="AG52">
-        <v>1</v>
-      </c>
-      <c r="AH52">
-        <v>2079</v>
-      </c>
-      <c r="AI52">
-        <f t="shared" si="0"/>
-        <v>529</v>
-      </c>
-    </row>
-    <row r="53" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB53">
-        <v>1</v>
-      </c>
-      <c r="AC53">
-        <v>2079</v>
-      </c>
-      <c r="AD53">
-        <v>481</v>
-      </c>
-      <c r="AG53">
-        <v>1</v>
-      </c>
-      <c r="AH53">
-        <v>2079</v>
-      </c>
-      <c r="AI53">
-        <f t="shared" si="0"/>
-        <v>545</v>
-      </c>
-    </row>
-    <row r="54" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB54">
-        <v>1</v>
-      </c>
-      <c r="AC54">
-        <v>2079</v>
-      </c>
-      <c r="AD54">
-        <v>497</v>
-      </c>
-      <c r="AG54">
-        <v>1</v>
-      </c>
-      <c r="AH54">
-        <v>2079</v>
-      </c>
-      <c r="AI54">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
-    <row r="56" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB56">
-        <v>1</v>
-      </c>
-      <c r="AC56">
-        <v>2079</v>
-      </c>
-      <c r="AD56">
-        <v>513</v>
-      </c>
-      <c r="AG56">
-        <v>1</v>
-      </c>
-      <c r="AH56">
-        <v>2079</v>
-      </c>
-      <c r="AI56">
-        <f t="shared" si="0"/>
-        <v>577</v>
-      </c>
-    </row>
-    <row r="57" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB57">
-        <v>1</v>
-      </c>
-      <c r="AC57">
-        <v>2079</v>
-      </c>
-      <c r="AD57">
-        <v>529</v>
-      </c>
-      <c r="AG57">
-        <v>1</v>
-      </c>
-      <c r="AH57">
-        <v>2079</v>
-      </c>
-      <c r="AI57">
-        <f t="shared" si="0"/>
-        <v>593</v>
-      </c>
-    </row>
-    <row r="58" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB58">
-        <v>1</v>
-      </c>
-      <c r="AC58">
-        <v>2079</v>
-      </c>
-      <c r="AD58">
-        <v>545</v>
-      </c>
-      <c r="AG58">
-        <v>1</v>
-      </c>
-      <c r="AH58">
-        <v>2079</v>
-      </c>
-      <c r="AI58">
-        <f t="shared" si="0"/>
-        <v>609</v>
-      </c>
-    </row>
-    <row r="59" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB59">
-        <v>1</v>
-      </c>
-      <c r="AC59">
-        <v>2079</v>
-      </c>
-      <c r="AD59">
-        <v>561</v>
-      </c>
-      <c r="AG59">
-        <v>1</v>
-      </c>
-      <c r="AH59">
-        <v>2079</v>
-      </c>
-      <c r="AI59">
-        <f t="shared" si="0"/>
-        <v>625</v>
-      </c>
-    </row>
-    <row r="60" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB60">
-        <v>1</v>
-      </c>
-      <c r="AC60">
-        <v>2079</v>
-      </c>
-      <c r="AD60">
-        <v>577</v>
-      </c>
-      <c r="AG60">
-        <v>1</v>
-      </c>
-      <c r="AH60">
-        <v>2079</v>
-      </c>
-      <c r="AI60">
-        <f t="shared" si="0"/>
-        <v>641</v>
-      </c>
-    </row>
-    <row r="62" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB62" t="s">
-        <v>131</v>
-      </c>
-      <c r="AG62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB63">
-        <v>1</v>
-      </c>
-      <c r="AC63">
-        <v>2351</v>
-      </c>
-      <c r="AD63">
-        <v>433</v>
-      </c>
-      <c r="AG63">
-        <v>1</v>
-      </c>
-      <c r="AH63">
-        <v>2351</v>
-      </c>
-      <c r="AI63">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="64" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB64">
-        <v>1</v>
-      </c>
-      <c r="AC64">
-        <v>2351</v>
-      </c>
-      <c r="AD64">
-        <v>449</v>
-      </c>
-      <c r="AG64">
-        <v>1</v>
-      </c>
-      <c r="AH64">
-        <v>2351</v>
-      </c>
-      <c r="AI64">
-        <f t="shared" si="0"/>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="65" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB65">
-        <v>1</v>
-      </c>
-      <c r="AC65">
-        <v>2351</v>
-      </c>
-      <c r="AD65">
-        <v>465</v>
-      </c>
-      <c r="AG65">
-        <v>1</v>
-      </c>
-      <c r="AH65">
-        <v>2351</v>
-      </c>
-      <c r="AI65">
-        <f t="shared" si="0"/>
-        <v>529</v>
-      </c>
-    </row>
-    <row r="66" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB66">
-        <v>1</v>
-      </c>
-      <c r="AC66">
-        <v>2351</v>
-      </c>
-      <c r="AD66">
-        <v>481</v>
-      </c>
-      <c r="AG66">
-        <v>1</v>
-      </c>
-      <c r="AH66">
-        <v>2351</v>
-      </c>
-      <c r="AI66">
-        <f t="shared" si="0"/>
-        <v>545</v>
-      </c>
-    </row>
-    <row r="67" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB67">
-        <v>1</v>
-      </c>
-      <c r="AC67">
-        <v>2351</v>
-      </c>
-      <c r="AD67">
-        <v>497</v>
-      </c>
-      <c r="AG67">
-        <v>1</v>
-      </c>
-      <c r="AH67">
-        <v>2351</v>
-      </c>
-      <c r="AI67">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
-    <row r="68" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB68">
-        <v>1</v>
-      </c>
-      <c r="AC68">
-        <v>2367</v>
-      </c>
-      <c r="AD68">
-        <v>433</v>
-      </c>
-      <c r="AG68">
-        <v>1</v>
-      </c>
-      <c r="AH68">
-        <v>2367</v>
-      </c>
-      <c r="AI68">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="69" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB69">
-        <v>1</v>
-      </c>
-      <c r="AC69">
-        <v>2367</v>
-      </c>
-      <c r="AD69">
-        <v>449</v>
-      </c>
-      <c r="AG69">
-        <v>1</v>
-      </c>
-      <c r="AH69">
-        <v>2367</v>
-      </c>
-      <c r="AI69">
-        <f t="shared" si="0"/>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="70" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB70">
-        <v>1</v>
-      </c>
-      <c r="AC70">
-        <v>2367</v>
-      </c>
-      <c r="AD70">
-        <v>465</v>
-      </c>
-      <c r="AG70">
-        <v>1</v>
-      </c>
-      <c r="AH70">
-        <v>2367</v>
-      </c>
-      <c r="AI70">
-        <f t="shared" si="0"/>
-        <v>529</v>
-      </c>
-    </row>
-    <row r="71" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB71">
-        <v>1</v>
-      </c>
-      <c r="AC71">
-        <v>2367</v>
-      </c>
-      <c r="AD71">
-        <v>481</v>
-      </c>
-      <c r="AG71">
-        <v>1</v>
-      </c>
-      <c r="AH71">
-        <v>2367</v>
-      </c>
-      <c r="AI71">
-        <f t="shared" si="0"/>
-        <v>545</v>
-      </c>
-    </row>
-    <row r="72" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB72">
-        <v>1</v>
-      </c>
-      <c r="AC72">
-        <v>2367</v>
-      </c>
-      <c r="AD72">
-        <v>497</v>
-      </c>
-      <c r="AG72">
-        <v>1</v>
-      </c>
-      <c r="AH72">
-        <v>2367</v>
-      </c>
-      <c r="AI72">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
-    <row r="75" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB75" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG75" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB76">
-        <v>1</v>
-      </c>
-      <c r="AC76">
-        <v>2127</v>
-      </c>
-      <c r="AD76">
-        <v>433</v>
-      </c>
-      <c r="AG76">
-        <v>1</v>
-      </c>
-      <c r="AH76">
-        <v>2127</v>
-      </c>
-      <c r="AI76">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="77" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB77">
-        <v>1</v>
-      </c>
-      <c r="AC77">
-        <v>2143</v>
-      </c>
-      <c r="AD77">
-        <v>433</v>
-      </c>
-      <c r="AG77">
-        <v>1</v>
-      </c>
-      <c r="AH77">
-        <v>2143</v>
-      </c>
-      <c r="AI77">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="78" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB78">
-        <v>1</v>
-      </c>
-      <c r="AC78">
-        <v>2159</v>
-      </c>
-      <c r="AD78">
-        <v>433</v>
-      </c>
-      <c r="AG78">
-        <v>1</v>
-      </c>
-      <c r="AH78">
-        <v>2159</v>
-      </c>
-      <c r="AI78">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="79" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB79">
-        <v>1</v>
-      </c>
-      <c r="AC79">
-        <v>2175</v>
-      </c>
-      <c r="AD79">
-        <v>433</v>
-      </c>
-      <c r="AG79">
-        <v>1</v>
-      </c>
-      <c r="AH79">
-        <v>2175</v>
-      </c>
-      <c r="AI79">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="80" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB80">
-        <v>1</v>
-      </c>
-      <c r="AC80">
-        <v>2191</v>
-      </c>
-      <c r="AD80">
-        <v>433</v>
-      </c>
-      <c r="AG80">
-        <v>1</v>
-      </c>
-      <c r="AH80">
-        <v>2191</v>
-      </c>
-      <c r="AI80">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="82" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB82">
-        <v>1</v>
-      </c>
-      <c r="AC82">
-        <v>2207</v>
-      </c>
-      <c r="AD82">
-        <v>433</v>
-      </c>
-      <c r="AG82">
-        <v>1</v>
-      </c>
-      <c r="AH82">
-        <v>2207</v>
-      </c>
-      <c r="AI82">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="83" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB83">
-        <v>1</v>
-      </c>
-      <c r="AC83">
-        <v>2223</v>
-      </c>
-      <c r="AD83">
-        <v>433</v>
-      </c>
-      <c r="AG83">
-        <v>1</v>
-      </c>
-      <c r="AH83">
-        <v>2223</v>
-      </c>
-      <c r="AI83">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="84" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB84">
-        <v>1</v>
-      </c>
-      <c r="AC84">
-        <v>2239</v>
-      </c>
-      <c r="AD84">
-        <v>433</v>
-      </c>
-      <c r="AG84">
-        <v>1</v>
-      </c>
-      <c r="AH84">
-        <v>2239</v>
-      </c>
-      <c r="AI84">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="85" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB85">
-        <v>1</v>
-      </c>
-      <c r="AC85">
-        <v>2255</v>
-      </c>
-      <c r="AD85">
-        <v>433</v>
-      </c>
-      <c r="AG85">
-        <v>1</v>
-      </c>
-      <c r="AH85">
-        <v>2255</v>
-      </c>
-      <c r="AI85">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="86" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB86">
-        <v>1</v>
-      </c>
-      <c r="AC86">
-        <v>2271</v>
-      </c>
-      <c r="AD86">
-        <v>433</v>
-      </c>
-      <c r="AG86">
-        <v>1</v>
-      </c>
-      <c r="AH86">
-        <v>2271</v>
-      </c>
-      <c r="AI86">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="88" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB88">
-        <v>1</v>
-      </c>
-      <c r="AC88">
-        <v>2287</v>
-      </c>
-      <c r="AD88">
-        <v>433</v>
-      </c>
-      <c r="AG88">
-        <v>1</v>
-      </c>
-      <c r="AH88">
-        <v>2287</v>
-      </c>
-      <c r="AI88">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="89" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB89">
-        <v>1</v>
-      </c>
-      <c r="AC89">
-        <v>2303</v>
-      </c>
-      <c r="AD89">
-        <v>433</v>
-      </c>
-      <c r="AG89">
-        <v>1</v>
-      </c>
-      <c r="AH89">
-        <v>2303</v>
-      </c>
-      <c r="AI89">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="91" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB91">
-        <v>1</v>
-      </c>
-      <c r="AC91">
-        <v>2351</v>
-      </c>
-      <c r="AD91">
-        <v>433</v>
-      </c>
-      <c r="AG91">
-        <v>1</v>
-      </c>
-      <c r="AH91">
-        <v>2351</v>
-      </c>
-      <c r="AI91">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="92" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB92">
-        <v>1</v>
-      </c>
-      <c r="AC92">
-        <v>2367</v>
-      </c>
-      <c r="AD92">
-        <v>433</v>
-      </c>
-      <c r="AG92">
-        <v>1</v>
-      </c>
-      <c r="AH92">
-        <v>2367</v>
-      </c>
-      <c r="AI92">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="94" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB94" t="s">
-        <v>133</v>
-      </c>
-      <c r="AG94" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="95" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB95">
-        <v>1</v>
-      </c>
-      <c r="AC95">
-        <v>2223</v>
-      </c>
-      <c r="AD95">
-        <v>577</v>
-      </c>
-      <c r="AG95">
-        <v>1</v>
-      </c>
-      <c r="AH95">
-        <v>2223</v>
-      </c>
-      <c r="AI95">
-        <f t="shared" si="0"/>
-        <v>641</v>
-      </c>
-    </row>
-    <row r="96" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB96">
-        <v>1</v>
-      </c>
-      <c r="AC96">
-        <v>2239</v>
-      </c>
-      <c r="AD96">
-        <v>577</v>
-      </c>
-      <c r="AG96">
-        <v>1</v>
-      </c>
-      <c r="AH96">
-        <v>2239</v>
-      </c>
-      <c r="AI96">
-        <f t="shared" si="0"/>
-        <v>641</v>
-      </c>
-    </row>
-    <row r="98" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB98">
-        <v>1</v>
-      </c>
-      <c r="AC98">
-        <v>2239</v>
-      </c>
-      <c r="AD98">
-        <v>561</v>
-      </c>
-      <c r="AG98">
-        <v>1</v>
-      </c>
-      <c r="AH98">
-        <v>2239</v>
-      </c>
-      <c r="AI98">
-        <f t="shared" si="0"/>
-        <v>625</v>
-      </c>
-    </row>
-    <row r="99" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB99">
-        <v>1</v>
-      </c>
-      <c r="AC99">
-        <v>2255</v>
-      </c>
-      <c r="AD99">
-        <v>561</v>
-      </c>
-      <c r="AG99">
-        <v>1</v>
-      </c>
-      <c r="AH99">
-        <v>2255</v>
-      </c>
-      <c r="AI99">
-        <f t="shared" si="0"/>
-        <v>625</v>
-      </c>
-    </row>
-    <row r="101" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB101">
-        <v>1</v>
-      </c>
-      <c r="AC101">
-        <v>2255</v>
-      </c>
-      <c r="AD101">
-        <v>545</v>
-      </c>
-      <c r="AG101">
-        <v>1</v>
-      </c>
-      <c r="AH101">
-        <v>2255</v>
-      </c>
-      <c r="AI101">
-        <f t="shared" si="0"/>
-        <v>609</v>
-      </c>
-    </row>
-    <row r="102" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB102">
-        <v>1</v>
-      </c>
-      <c r="AC102">
-        <v>2271</v>
-      </c>
-      <c r="AD102">
-        <v>545</v>
-      </c>
-      <c r="AG102">
-        <v>1</v>
-      </c>
-      <c r="AH102">
-        <v>2271</v>
-      </c>
-      <c r="AI102">
-        <f t="shared" si="0"/>
-        <v>609</v>
-      </c>
-    </row>
-    <row r="104" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB104">
-        <v>1</v>
-      </c>
-      <c r="AC104">
-        <v>2271</v>
-      </c>
-      <c r="AD104">
-        <v>529</v>
-      </c>
-      <c r="AG104">
-        <v>1</v>
-      </c>
-      <c r="AH104">
-        <v>2271</v>
-      </c>
-      <c r="AI104">
-        <f t="shared" si="0"/>
-        <v>593</v>
-      </c>
-    </row>
-    <row r="105" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB105">
-        <v>1</v>
-      </c>
-      <c r="AC105">
-        <v>2287</v>
-      </c>
-      <c r="AD105">
-        <v>529</v>
-      </c>
-      <c r="AG105">
-        <v>1</v>
-      </c>
-      <c r="AH105">
-        <v>2287</v>
-      </c>
-      <c r="AI105">
-        <f t="shared" si="0"/>
-        <v>593</v>
-      </c>
-    </row>
-    <row r="107" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB107">
-        <v>1</v>
-      </c>
-      <c r="AC107">
-        <v>2287</v>
-      </c>
-      <c r="AD107">
-        <v>513</v>
-      </c>
-      <c r="AG107">
-        <v>1</v>
-      </c>
-      <c r="AH107">
-        <v>2287</v>
-      </c>
-      <c r="AI107">
-        <f t="shared" si="0"/>
-        <v>577</v>
-      </c>
-    </row>
-    <row r="108" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB108">
-        <v>1</v>
-      </c>
-      <c r="AC108">
-        <v>2303</v>
-      </c>
-      <c r="AD108">
-        <v>513</v>
-      </c>
-      <c r="AG108">
-        <v>1</v>
-      </c>
-      <c r="AH108">
-        <v>2303</v>
-      </c>
-      <c r="AI108">
-        <f t="shared" si="0"/>
-        <v>577</v>
-      </c>
-    </row>
-    <row r="110" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB110">
-        <v>1</v>
-      </c>
-      <c r="AC110">
-        <v>2303</v>
-      </c>
-      <c r="AD110">
-        <v>497</v>
-      </c>
-      <c r="AG110">
-        <v>1</v>
-      </c>
-      <c r="AH110">
-        <v>2303</v>
-      </c>
-      <c r="AI110">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
-    <row r="111" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB111">
-        <v>1</v>
-      </c>
-      <c r="AC111">
-        <v>2319</v>
-      </c>
-      <c r="AD111">
-        <v>497</v>
-      </c>
-      <c r="AG111">
-        <v>1</v>
-      </c>
-      <c r="AH111">
-        <v>2319</v>
-      </c>
-      <c r="AI111">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
-    <row r="112" spans="28:35" x14ac:dyDescent="0.3">
-      <c r="AB112">
-        <v>1</v>
-      </c>
-      <c r="AC112">
-        <v>2335</v>
-      </c>
-      <c r="AD112">
-        <v>497</v>
-      </c>
-      <c r="AG112">
-        <v>1</v>
-      </c>
-      <c r="AH112">
-        <v>2335</v>
-      </c>
-      <c r="AI112">
-        <f t="shared" si="0"/>
-        <v>561</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="AM23:AN23"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AR4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BI4:BL4"/>
-    <mergeCell ref="BI5:BL5"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
+  <mergeCells count="30">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -3289,6 +2261,22 @@
     <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="S12:T12"/>
+    <mergeCell ref="BK4:BN4"/>
+    <mergeCell ref="BK5:BN5"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="AM23:AN23"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AR4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3299,7 +2287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4239-B81E-4CE7-883B-6C18963F977B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -3313,12 +2301,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="69" t="s">
@@ -3589,7 +2577,7 @@
   <dimension ref="A4:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3605,11 +2593,11 @@
       <c r="B4" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -3659,6 +2647,7 @@
     <mergeCell ref="B4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create P_button object with basic feature: render
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC88A81-919C-4F12-98DB-A59659AC995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E90ABC-95BB-4C61-B111-427111835740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>HUD</t>
+  </si>
+  <si>
+    <t>Pbutton</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>pressed</t>
   </si>
 </sst>
 </file>
@@ -679,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -780,6 +789,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1151,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BN37"/>
+  <dimension ref="B4:BP37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BF6" sqref="BF6"/>
+      <selection activeCell="BH7" sqref="BH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,13 +1197,13 @@
     <col min="53" max="53" width="12.109375" customWidth="1"/>
     <col min="54" max="58" width="8.44140625" customWidth="1"/>
     <col min="59" max="59" width="5.6640625" customWidth="1"/>
-    <col min="60" max="61" width="7.77734375" customWidth="1"/>
-    <col min="62" max="62" width="11.6640625" customWidth="1"/>
-    <col min="63" max="64" width="13.44140625" customWidth="1"/>
-    <col min="65" max="65" width="13.109375" customWidth="1"/>
+    <col min="60" max="63" width="7.77734375" customWidth="1"/>
+    <col min="64" max="64" width="11.6640625" customWidth="1"/>
+    <col min="65" max="66" width="13.44140625" customWidth="1"/>
+    <col min="67" max="67" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,104 +1214,110 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="66" t="s">
+      <c r="K4" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66" t="s">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="66"/>
+      <c r="N4" s="68"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="57" t="s">
+      <c r="S4" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57" t="s">
+      <c r="V4" s="59"/>
+      <c r="W4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57" t="s">
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="55" t="s">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="55" t="s">
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="56"/>
-      <c r="AE4" s="55" t="s">
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="55" t="s">
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="56"/>
-      <c r="AI4" s="55" t="s">
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="56"/>
-      <c r="AK4" s="55" t="s">
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="AL4" s="56"/>
-      <c r="AM4" s="58" t="s">
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="59"/>
-      <c r="AO4" s="60"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="56"/>
-      <c r="AS4" s="55" t="s">
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="62"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="AT4" s="56"/>
-      <c r="AU4" s="55" t="s">
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="AV4" s="56"/>
-      <c r="AW4" s="55" t="s">
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="AX4" s="56"/>
-      <c r="AY4" s="55" t="s">
+      <c r="AX4" s="58"/>
+      <c r="AY4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="AZ4" s="56"/>
-      <c r="BA4" s="55" t="s">
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="BB4" s="56"/>
-      <c r="BC4" s="55" t="s">
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="BD4" s="56"/>
-      <c r="BE4" s="55" t="s">
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="BF4" s="56"/>
-      <c r="BJ4" s="35" t="s">
+      <c r="BF4" s="58"/>
+      <c r="BG4" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH4" s="58"/>
+      <c r="BI4" s="52"/>
+      <c r="BJ4" s="52"/>
+      <c r="BL4" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="BK4" s="52" t="s">
+      <c r="BM4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="BL4" s="52"/>
-      <c r="BM4" s="52"/>
-      <c r="BN4" s="52"/>
-    </row>
-    <row r="5" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BN4" s="54"/>
+      <c r="BO4" s="54"/>
+      <c r="BP4" s="54"/>
+    </row>
+    <row r="5" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1377,18 +1398,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="53" t="s">
+      <c r="AM5" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="53" t="s">
+      <c r="AN5" s="56"/>
+      <c r="AO5" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="54"/>
-      <c r="AQ5" s="61" t="s">
+      <c r="AP5" s="56"/>
+      <c r="AQ5" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="AR5" s="62"/>
+      <c r="AR5" s="64"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1431,24 +1452,32 @@
       <c r="BF5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BJ5" s="35" t="s">
+      <c r="BG5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BL5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="BK5" s="52" t="s">
+      <c r="BM5" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="52"/>
-      <c r="BN5" s="52"/>
-    </row>
-    <row r="6" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BN5" s="54"/>
+      <c r="BO5" s="54"/>
+      <c r="BP5" s="54"/>
+    </row>
+    <row r="6" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="64" t="s">
+      <c r="J6" s="66" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1559,34 +1588,38 @@
       <c r="BD6" s="9">
         <v>15000</v>
       </c>
-      <c r="BE6" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="BF6" s="9">
+      <c r="BE6" s="9"/>
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="BH6" s="9">
         <v>16000</v>
       </c>
-      <c r="BK6" s="36" t="s">
+      <c r="BI6" s="16"/>
+      <c r="BJ6" s="16"/>
+      <c r="BM6" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="BL6" s="36" t="s">
+      <c r="BN6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="BM6" s="30" t="s">
+      <c r="BO6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="BN6" s="30" t="s">
+      <c r="BP6" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:66" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="67"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1634,22 +1667,28 @@
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
-      <c r="BK7" s="33" t="s">
+      <c r="BG7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH7">
+        <v>16001</v>
+      </c>
+      <c r="BM7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="BL7" s="34">
+      <c r="BN7" s="34">
         <v>1100</v>
       </c>
-      <c r="BM7">
+      <c r="BO7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:68" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="67"/>
       <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1674,20 +1713,20 @@
       <c r="AR8" s="34">
         <v>1710</v>
       </c>
-      <c r="BK8" s="33" t="s">
+      <c r="BM8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="BL8" s="34">
+      <c r="BN8" s="34">
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I9" s="63"/>
-      <c r="J9" s="65"/>
-      <c r="S9" s="67" t="s">
+    <row r="9" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I9" s="65"/>
+      <c r="J9" s="67"/>
+      <c r="S9" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="T9" s="67"/>
+      <c r="T9" s="69"/>
       <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
@@ -1712,15 +1751,15 @@
       <c r="AR9" s="34">
         <v>1800</v>
       </c>
-      <c r="BK9" s="33" t="s">
+      <c r="BM9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="BL9" s="34">
+      <c r="BN9" s="34">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I10" s="63"/>
+    <row r="10" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I10" s="65"/>
       <c r="S10" s="27" t="s">
         <v>56</v>
       </c>
@@ -1745,15 +1784,15 @@
       <c r="AR10" s="34">
         <v>1801</v>
       </c>
-      <c r="BK10" s="33" t="s">
+      <c r="BM10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="BL10" s="34">
+      <c r="BN10" s="34">
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I11" s="63"/>
+    <row r="11" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I11" s="65"/>
       <c r="S11" s="27" t="s">
         <v>57</v>
       </c>
@@ -1780,19 +1819,19 @@
       </c>
       <c r="AT11" s="18"/>
       <c r="AU11" s="18"/>
-      <c r="BK11" s="33" t="s">
+      <c r="BM11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BL11" s="34">
+      <c r="BN11" s="34">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I12" s="63"/>
-      <c r="S12" s="68" t="s">
+    <row r="12" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I12" s="65"/>
+      <c r="S12" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="T12" s="68"/>
+      <c r="T12" s="70"/>
       <c r="AM12" s="33" t="s">
         <v>24</v>
       </c>
@@ -1813,15 +1852,15 @@
       </c>
       <c r="AT12" s="21"/>
       <c r="AU12" s="21"/>
-      <c r="BK12" s="33" t="s">
+      <c r="BM12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="BL12" s="34">
+      <c r="BN12" s="34">
         <v>1301</v>
       </c>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I13" s="63"/>
+    <row r="13" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I13" s="65"/>
       <c r="S13" s="27" t="s">
         <v>56</v>
       </c>
@@ -1848,15 +1887,15 @@
       </c>
       <c r="AT13" s="16"/>
       <c r="AU13" s="16"/>
-      <c r="BK13" s="33" t="s">
+      <c r="BM13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="BL13" s="34">
+      <c r="BN13" s="34">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I14" s="63"/>
+    <row r="14" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I14" s="65"/>
       <c r="S14" s="27" t="s">
         <v>57</v>
       </c>
@@ -1881,15 +1920,15 @@
       <c r="AR14" s="34">
         <v>2001</v>
       </c>
-      <c r="BK14" s="33" t="s">
+      <c r="BM14" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="BL14" s="34">
+      <c r="BN14" s="34">
         <v>1401</v>
       </c>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I15" s="63"/>
+    <row r="15" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I15" s="65"/>
       <c r="AM15" s="33" t="s">
         <v>27</v>
       </c>
@@ -1908,15 +1947,15 @@
       <c r="AR15" s="34">
         <v>2100</v>
       </c>
-      <c r="BK15" s="33" t="s">
+      <c r="BM15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="BL15" s="34">
+      <c r="BN15" s="34">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.3">
-      <c r="I16" s="63"/>
+    <row r="16" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="I16" s="65"/>
       <c r="S16" s="27" t="s">
         <v>126</v>
       </c>
@@ -1941,15 +1980,15 @@
       <c r="AR16" s="34">
         <v>2101</v>
       </c>
-      <c r="BK16" s="33" t="s">
+      <c r="BM16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="BL16" s="34">
+      <c r="BN16" s="34">
         <v>1501</v>
       </c>
     </row>
-    <row r="17" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="I17" s="63"/>
+    <row r="17" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="I17" s="65"/>
       <c r="S17" s="51" t="s">
         <v>125</v>
       </c>
@@ -1978,15 +2017,15 @@
       <c r="AR17" s="34">
         <v>2200</v>
       </c>
-      <c r="BK17" s="33" t="s">
+      <c r="BM17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="BL17" s="34">
+      <c r="BN17" s="34">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="I18" s="63"/>
+    <row r="18" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="I18" s="65"/>
       <c r="AM18" s="33" t="s">
         <v>30</v>
       </c>
@@ -2005,15 +2044,15 @@
       <c r="AR18" s="34">
         <v>2201</v>
       </c>
-      <c r="BK18" s="33" t="s">
+      <c r="BM18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="BL18" s="34">
+      <c r="BN18" s="34">
         <v>1601</v>
       </c>
     </row>
-    <row r="19" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="I19" s="63"/>
+    <row r="19" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="I19" s="65"/>
       <c r="AM19" s="33" t="s">
         <v>31</v>
       </c>
@@ -2029,8 +2068,8 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="20" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="I20" s="63"/>
+    <row r="20" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="I20" s="65"/>
       <c r="AM20" s="33" t="s">
         <v>32</v>
       </c>
@@ -2046,8 +2085,8 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="21" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="I21" s="63"/>
+    <row r="21" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="I21" s="65"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -2063,7 +2102,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="22" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AO22" s="32"/>
       <c r="AP22" s="32"/>
       <c r="AQ22" s="44" t="s">
@@ -2073,11 +2112,11 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="23" spans="9:64" x14ac:dyDescent="0.3">
-      <c r="AM23" s="52" t="s">
+    <row r="23" spans="9:66" x14ac:dyDescent="0.3">
+      <c r="AM23" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="AN23" s="52"/>
+      <c r="AN23" s="54"/>
       <c r="AO23" s="16"/>
       <c r="AP23" s="16"/>
       <c r="AQ23" s="47" t="s">
@@ -2087,7 +2126,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM24" s="33" t="s">
         <v>20</v>
       </c>
@@ -2103,7 +2142,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="25" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM25" s="33" t="s">
         <v>19</v>
       </c>
@@ -2119,7 +2158,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="26" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="26" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AO26" s="16"/>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
@@ -2129,13 +2168,13 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="27" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AO27" s="16"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM28" s="33" t="s">
         <v>21</v>
       </c>
@@ -2147,7 +2186,7 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="29" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM29" s="33" t="s">
         <v>22</v>
       </c>
@@ -2159,7 +2198,7 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="30" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM30" s="33" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2210,7 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="31" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM31" s="33" t="s">
         <v>24</v>
       </c>
@@ -2183,7 +2222,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" spans="9:64" x14ac:dyDescent="0.3">
+    <row r="32" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM32" s="33" t="s">
         <v>117</v>
       </c>
@@ -2246,7 +2285,7 @@
       <c r="AR37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2261,14 +2300,15 @@
     <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="S12:T12"/>
-    <mergeCell ref="BK4:BN4"/>
-    <mergeCell ref="BK5:BN5"/>
+    <mergeCell ref="BM4:BP4"/>
+    <mergeCell ref="BM5:BP5"/>
     <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="AU4:AV4"/>
     <mergeCell ref="BA4:BB4"/>
     <mergeCell ref="BC4:BD4"/>
     <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BH4"/>
     <mergeCell ref="AM23:AN23"/>
     <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="AS4:AT4"/>
@@ -2301,20 +2341,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="24"/>
@@ -2590,14 +2630,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">

</xml_diff>

<commit_message>
Add animation Hold for small Mario: idle
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E90ABC-95BB-4C61-B111-427111835740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C2274-9388-4BCD-B4F1-F1E5B597E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="135">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>pressed</t>
+  </si>
+  <si>
+    <t>Mario Small Hold Koopa</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -850,6 +853,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1168,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BH7" sqref="BH7"/>
+    <sheetView tabSelected="1" topLeftCell="AD4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP25" sqref="AP25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2117,8 +2126,10 @@
         <v>119</v>
       </c>
       <c r="AN23" s="54"/>
-      <c r="AO23" s="16"/>
-      <c r="AP23" s="16"/>
+      <c r="AO23" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP23" s="74"/>
       <c r="AQ23" s="47" t="s">
         <v>110</v>
       </c>
@@ -2131,10 +2142,14 @@
         <v>20</v>
       </c>
       <c r="AN24" s="45">
-        <v>1010</v>
-      </c>
-      <c r="AO24" s="16"/>
-      <c r="AP24" s="16"/>
+        <v>450</v>
+      </c>
+      <c r="AO24" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP24" s="45">
+        <v>1150</v>
+      </c>
       <c r="AQ24" s="44" t="s">
         <v>111</v>
       </c>
@@ -2147,10 +2162,14 @@
         <v>19</v>
       </c>
       <c r="AN25" s="45">
-        <v>1011</v>
-      </c>
-      <c r="AO25" s="16"/>
-      <c r="AP25" s="16"/>
+        <v>451</v>
+      </c>
+      <c r="AO25" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP25" s="45">
+        <v>1151</v>
+      </c>
       <c r="AQ25" s="44" t="s">
         <v>112</v>
       </c>
@@ -2159,8 +2178,6 @@
       </c>
     </row>
     <row r="26" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AO26" s="16"/>
-      <c r="AP26" s="16"/>
       <c r="AQ26" s="49" t="s">
         <v>113</v>
       </c>
@@ -2169,8 +2186,6 @@
       </c>
     </row>
     <row r="27" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AO27" s="16"/>
-      <c r="AP27" s="16"/>
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
@@ -2181,8 +2196,12 @@
       <c r="AN28" s="34">
         <v>500</v>
       </c>
-      <c r="AO28" s="16"/>
-      <c r="AP28" s="16"/>
+      <c r="AO28" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP28" s="34">
+        <v>500</v>
+      </c>
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
@@ -2193,8 +2212,12 @@
       <c r="AN29" s="34">
         <v>501</v>
       </c>
-      <c r="AO29" s="16"/>
-      <c r="AP29" s="16"/>
+      <c r="AO29" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP29" s="34">
+        <v>501</v>
+      </c>
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
@@ -2205,8 +2228,12 @@
       <c r="AN30" s="34">
         <v>600</v>
       </c>
-      <c r="AO30" s="16"/>
-      <c r="AP30" s="16"/>
+      <c r="AO30" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP30" s="34">
+        <v>600</v>
+      </c>
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
@@ -2217,8 +2244,12 @@
       <c r="AN31" s="34">
         <v>601</v>
       </c>
-      <c r="AO31" s="16"/>
-      <c r="AP31" s="16"/>
+      <c r="AO31" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP31" s="34">
+        <v>601</v>
+      </c>
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
@@ -2229,8 +2260,12 @@
       <c r="AN32" s="34">
         <v>700</v>
       </c>
-      <c r="AO32" s="16"/>
-      <c r="AP32" s="16"/>
+      <c r="AO32" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP32" s="34">
+        <v>700</v>
+      </c>
       <c r="AQ32" s="16"/>
       <c r="AR32" s="16"/>
     </row>
@@ -2241,8 +2276,12 @@
       <c r="AN33" s="34">
         <v>701</v>
       </c>
-      <c r="AO33" s="16"/>
-      <c r="AP33" s="16"/>
+      <c r="AO33" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP33" s="34">
+        <v>701</v>
+      </c>
       <c r="AQ33" s="16"/>
       <c r="AR33" s="16"/>
     </row>
@@ -2253,8 +2292,12 @@
       <c r="AN34" s="34">
         <v>800</v>
       </c>
-      <c r="AO34" s="16"/>
-      <c r="AP34" s="16"/>
+      <c r="AO34" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP34" s="34">
+        <v>800</v>
+      </c>
       <c r="AQ34" s="16"/>
       <c r="AR34" s="16"/>
     </row>
@@ -2265,8 +2308,12 @@
       <c r="AN35" s="34">
         <v>801</v>
       </c>
-      <c r="AO35" s="31"/>
-      <c r="AP35" s="31"/>
+      <c r="AO35" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP35" s="34">
+        <v>801</v>
+      </c>
       <c r="AQ35" s="31"/>
       <c r="AR35" s="31"/>
     </row>
@@ -2285,7 +2332,7 @@
       <c r="AR37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2317,6 +2364,7 @@
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AO23:AP23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add animation Hold for raccoon Mario: idle
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C2274-9388-4BCD-B4F1-F1E5B597E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A656E000-17D2-4C37-B6BF-3B9E1BD54A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="136">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>Attack Right</t>
-  </si>
-  <si>
-    <t>Attck Left</t>
   </si>
   <si>
     <t>Breakable Brick</t>
@@ -454,6 +451,12 @@
   </si>
   <si>
     <t>Mario Small Hold Koopa</t>
+  </si>
+  <si>
+    <t>Mario Raccoon Hold</t>
+  </si>
+  <si>
+    <t>Attack Left</t>
   </si>
 </sst>
 </file>
@@ -749,9 +752,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,6 +859,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1175,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
-  <dimension ref="B4:BP37"/>
+  <dimension ref="B4:BP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP25" sqref="AP25"/>
+    <sheetView tabSelected="1" topLeftCell="AD13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR32" sqref="AR32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1223,108 +1226,108 @@
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="68"/>
+      <c r="N4" s="67"/>
       <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="59" t="s">
+      <c r="S4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59" t="s">
+      <c r="T4" s="58"/>
+      <c r="U4" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59" t="s">
+      <c r="V4" s="58"/>
+      <c r="W4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59" t="s">
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="57" t="s">
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="57" t="s">
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="57" t="s">
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="57" t="s">
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="57" t="s">
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN4" s="60"/>
+      <c r="AO4" s="61"/>
+      <c r="AP4" s="61"/>
+      <c r="AQ4" s="61"/>
+      <c r="AR4" s="57"/>
+      <c r="AS4" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT4" s="57"/>
+      <c r="AU4" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="AV4" s="57"/>
+      <c r="AW4" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ4" s="57"/>
+      <c r="BA4" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="60" t="s">
+      <c r="BB4" s="57"/>
+      <c r="BC4" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD4" s="57"/>
+      <c r="BE4" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="BF4" s="57"/>
+      <c r="BG4" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH4" s="57"/>
+      <c r="BI4" s="51"/>
+      <c r="BJ4" s="51"/>
+      <c r="BL4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM4" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="62"/>
-      <c r="AP4" s="62"/>
-      <c r="AQ4" s="62"/>
-      <c r="AR4" s="58"/>
-      <c r="AS4" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="AX4" s="58"/>
-      <c r="AY4" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="BD4" s="58"/>
-      <c r="BE4" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="BF4" s="58"/>
-      <c r="BG4" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH4" s="58"/>
-      <c r="BI4" s="52"/>
-      <c r="BJ4" s="52"/>
-      <c r="BL4" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="BM4" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="BN4" s="54"/>
-      <c r="BO4" s="54"/>
-      <c r="BP4" s="54"/>
+      <c r="BN4" s="53"/>
+      <c r="BO4" s="53"/>
+      <c r="BP4" s="53"/>
     </row>
     <row r="5" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
@@ -1407,18 +1410,18 @@
       <c r="AL5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="55" t="s">
+      <c r="AM5" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="55" t="s">
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="AP5" s="56"/>
-      <c r="AQ5" s="63" t="s">
+      <c r="AP5" s="55"/>
+      <c r="AQ5" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="AR5" s="64"/>
+      <c r="AR5" s="63"/>
       <c r="AS5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1467,26 +1470,26 @@
       <c r="BH5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BI5" s="53"/>
-      <c r="BJ5" s="53"/>
-      <c r="BL5" s="35" t="s">
+      <c r="BI5" s="52"/>
+      <c r="BJ5" s="52"/>
+      <c r="BL5" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="BM5" s="54" t="s">
+      <c r="BM5" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="BN5" s="54"/>
-      <c r="BO5" s="54"/>
-      <c r="BP5" s="54"/>
+      <c r="BN5" s="53"/>
+      <c r="BO5" s="53"/>
+      <c r="BP5" s="53"/>
     </row>
     <row r="6" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="66" t="s">
+      <c r="J6" s="65" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4">
@@ -1538,7 +1541,7 @@
         <v>10100</v>
       </c>
       <c r="AI6" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AJ6" s="9">
         <v>10200</v>
@@ -1549,22 +1552,22 @@
       <c r="AL6">
         <v>12000</v>
       </c>
-      <c r="AM6" s="33" t="s">
+      <c r="AM6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="34">
+      <c r="AN6" s="33">
         <v>400</v>
       </c>
-      <c r="AO6" s="33" t="s">
+      <c r="AO6" s="32" t="s">
         <v>20</v>
       </c>
       <c r="AP6" s="16">
         <v>1100</v>
       </c>
-      <c r="AQ6" s="33" t="s">
+      <c r="AQ6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="AR6" s="45">
+      <c r="AR6" s="44">
         <v>1700</v>
       </c>
       <c r="AU6" s="9" t="s">
@@ -1586,13 +1589,13 @@
         <v>14000</v>
       </c>
       <c r="BA6" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BB6" s="9">
         <v>14010</v>
       </c>
       <c r="BC6" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="BD6" s="9">
         <v>15000</v>
@@ -1600,17 +1603,17 @@
       <c r="BE6" s="9"/>
       <c r="BF6" s="9"/>
       <c r="BG6" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BH6" s="9">
         <v>16000</v>
       </c>
       <c r="BI6" s="16"/>
       <c r="BJ6" s="16"/>
-      <c r="BM6" s="36" t="s">
+      <c r="BM6" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="BN6" s="36" t="s">
+      <c r="BN6" s="35" t="s">
         <v>88</v>
       </c>
       <c r="BO6" s="30" t="s">
@@ -1627,8 +1630,8 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="65"/>
-      <c r="J7" s="67"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="66"/>
       <c r="S7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1657,35 +1660,35 @@
       </c>
       <c r="AI7" s="16"/>
       <c r="AJ7" s="16"/>
-      <c r="AM7" s="33" t="s">
+      <c r="AM7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AN7" s="34">
+      <c r="AN7" s="33">
         <v>401</v>
       </c>
-      <c r="AO7" s="33" t="s">
+      <c r="AO7" s="32" t="s">
         <v>19</v>
       </c>
       <c r="AP7" s="16">
         <v>1102</v>
       </c>
-      <c r="AQ7" s="33" t="s">
+      <c r="AQ7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AR7" s="45">
+      <c r="AR7" s="44">
         <v>1701</v>
       </c>
       <c r="BA7" s="9"/>
       <c r="BG7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BH7">
         <v>16001</v>
       </c>
-      <c r="BM7" s="33" t="s">
+      <c r="BM7" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="BN7" s="34">
+      <c r="BN7" s="33">
         <v>1100</v>
       </c>
       <c r="BO7">
@@ -1696,406 +1699,406 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="65"/>
-      <c r="J8" s="67"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="66"/>
       <c r="Y8" s="19" t="s">
         <v>50</v>
       </c>
       <c r="Z8">
         <v>5520</v>
       </c>
-      <c r="AM8" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN8" s="34">
+      <c r="AM8" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN8" s="33">
         <v>410</v>
       </c>
-      <c r="AO8" s="44" t="s">
-        <v>120</v>
+      <c r="AO8" s="43" t="s">
+        <v>119</v>
       </c>
       <c r="AP8" s="16">
         <v>1110</v>
       </c>
-      <c r="AQ8" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR8" s="34">
+      <c r="AQ8" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="AR8" s="33">
         <v>1710</v>
       </c>
-      <c r="BM8" s="33" t="s">
+      <c r="BM8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="BN8" s="34">
+      <c r="BN8" s="33">
         <v>1102</v>
       </c>
     </row>
     <row r="9" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I9" s="65"/>
-      <c r="J9" s="67"/>
-      <c r="S9" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="T9" s="69"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="66"/>
+      <c r="S9" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="T9" s="68"/>
       <c r="Y9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="Z9">
         <v>5530</v>
       </c>
-      <c r="AM9" s="33" t="s">
+      <c r="AM9" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AN9" s="34">
+      <c r="AN9" s="33">
         <v>500</v>
       </c>
-      <c r="AO9" s="33" t="s">
+      <c r="AO9" s="32" t="s">
         <v>21</v>
       </c>
       <c r="AP9" s="16">
         <v>1200</v>
       </c>
-      <c r="AQ9" s="33" t="s">
+      <c r="AQ9" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AR9" s="34">
+      <c r="AR9" s="33">
         <v>1800</v>
       </c>
-      <c r="BM9" s="33" t="s">
+      <c r="BM9" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="BN9" s="34">
+      <c r="BN9" s="33">
         <v>1200</v>
       </c>
     </row>
     <row r="10" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I10" s="65"/>
+      <c r="I10" s="64"/>
       <c r="S10" s="27" t="s">
         <v>56</v>
       </c>
       <c r="T10" s="4">
         <v>6010</v>
       </c>
-      <c r="AM10" s="33" t="s">
+      <c r="AM10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AN10" s="34">
+      <c r="AN10" s="33">
         <v>501</v>
       </c>
-      <c r="AO10" s="33" t="s">
+      <c r="AO10" s="32" t="s">
         <v>22</v>
       </c>
       <c r="AP10" s="16">
         <v>1201</v>
       </c>
-      <c r="AQ10" s="33" t="s">
+      <c r="AQ10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AR10" s="34">
+      <c r="AR10" s="33">
         <v>1801</v>
       </c>
-      <c r="BM10" s="33" t="s">
+      <c r="BM10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BN10" s="34">
+      <c r="BN10" s="33">
         <v>1201</v>
       </c>
     </row>
     <row r="11" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I11" s="65"/>
+      <c r="I11" s="64"/>
       <c r="S11" s="27" t="s">
         <v>57</v>
       </c>
       <c r="T11" s="4">
         <v>6011</v>
       </c>
-      <c r="AM11" s="33" t="s">
+      <c r="AM11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AN11" s="34">
+      <c r="AN11" s="33">
         <v>600</v>
       </c>
-      <c r="AO11" s="33" t="s">
+      <c r="AO11" s="32" t="s">
         <v>23</v>
       </c>
       <c r="AP11" s="16">
         <v>1300</v>
       </c>
-      <c r="AQ11" s="33" t="s">
+      <c r="AQ11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AR11" s="34">
+      <c r="AR11" s="33">
         <v>1900</v>
       </c>
       <c r="AT11" s="18"/>
       <c r="AU11" s="18"/>
-      <c r="BM11" s="33" t="s">
+      <c r="BM11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="BN11" s="34">
+      <c r="BN11" s="33">
         <v>1300</v>
       </c>
     </row>
     <row r="12" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I12" s="65"/>
-      <c r="S12" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="T12" s="70"/>
-      <c r="AM12" s="33" t="s">
+      <c r="I12" s="64"/>
+      <c r="S12" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="T12" s="69"/>
+      <c r="AM12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AN12" s="34">
+      <c r="AN12" s="33">
         <v>601</v>
       </c>
-      <c r="AO12" s="33" t="s">
+      <c r="AO12" s="32" t="s">
         <v>24</v>
       </c>
       <c r="AP12" s="16">
         <v>1301</v>
       </c>
-      <c r="AQ12" s="33" t="s">
+      <c r="AQ12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AR12" s="34">
+      <c r="AR12" s="33">
         <v>1901</v>
       </c>
       <c r="AT12" s="21"/>
       <c r="AU12" s="21"/>
-      <c r="BM12" s="33" t="s">
+      <c r="BM12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="BN12" s="34">
+      <c r="BN12" s="33">
         <v>1301</v>
       </c>
     </row>
     <row r="13" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I13" s="65"/>
+      <c r="I13" s="64"/>
       <c r="S13" s="27" t="s">
         <v>56</v>
       </c>
       <c r="T13" s="4">
         <v>6015</v>
       </c>
-      <c r="AM13" s="33" t="s">
+      <c r="AM13" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AN13" s="34">
+      <c r="AN13" s="33">
         <v>700</v>
       </c>
-      <c r="AO13" s="33" t="s">
+      <c r="AO13" s="32" t="s">
         <v>31</v>
       </c>
       <c r="AP13" s="16">
         <v>1400</v>
       </c>
-      <c r="AQ13" s="33" t="s">
+      <c r="AQ13" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AR13" s="34">
+      <c r="AR13" s="33">
         <v>2000</v>
       </c>
       <c r="AT13" s="16"/>
       <c r="AU13" s="16"/>
-      <c r="BM13" s="33" t="s">
+      <c r="BM13" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="BN13" s="34">
+      <c r="BN13" s="33">
         <v>1400</v>
       </c>
     </row>
     <row r="14" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I14" s="65"/>
+      <c r="I14" s="64"/>
       <c r="S14" s="27" t="s">
         <v>57</v>
       </c>
       <c r="T14" s="4">
         <v>6016</v>
       </c>
-      <c r="AM14" s="33" t="s">
+      <c r="AM14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="AN14" s="34">
+      <c r="AN14" s="33">
         <v>701</v>
       </c>
-      <c r="AO14" s="33" t="s">
+      <c r="AO14" s="32" t="s">
         <v>32</v>
       </c>
       <c r="AP14" s="16">
         <v>1401</v>
       </c>
-      <c r="AQ14" s="33" t="s">
+      <c r="AQ14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="AR14" s="34">
+      <c r="AR14" s="33">
         <v>2001</v>
       </c>
-      <c r="BM14" s="33" t="s">
+      <c r="BM14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="BN14" s="34">
+      <c r="BN14" s="33">
         <v>1401</v>
       </c>
     </row>
     <row r="15" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I15" s="65"/>
-      <c r="AM15" s="33" t="s">
+      <c r="I15" s="64"/>
+      <c r="AM15" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="AN15" s="34">
+      <c r="AN15" s="33">
         <v>800</v>
       </c>
-      <c r="AO15" s="33" t="s">
+      <c r="AO15" s="32" t="s">
         <v>25</v>
       </c>
       <c r="AP15" s="16">
         <v>1500</v>
       </c>
-      <c r="AQ15" s="33" t="s">
+      <c r="AQ15" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="AR15" s="34">
+      <c r="AR15" s="33">
         <v>2100</v>
       </c>
-      <c r="BM15" s="33" t="s">
+      <c r="BM15" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="BN15" s="34">
+      <c r="BN15" s="33">
         <v>1500</v>
       </c>
     </row>
     <row r="16" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="I16" s="65"/>
+      <c r="I16" s="64"/>
       <c r="S16" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T16" s="4">
         <v>6020</v>
       </c>
-      <c r="AM16" s="33" t="s">
+      <c r="AM16" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AN16" s="34">
+      <c r="AN16" s="33">
         <v>801</v>
       </c>
-      <c r="AO16" s="33" t="s">
+      <c r="AO16" s="32" t="s">
         <v>26</v>
       </c>
       <c r="AP16" s="16">
         <v>1501</v>
       </c>
-      <c r="AQ16" s="33" t="s">
+      <c r="AQ16" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AR16" s="34">
+      <c r="AR16" s="33">
         <v>2101</v>
       </c>
-      <c r="BM16" s="33" t="s">
+      <c r="BM16" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="BN16" s="34">
+      <c r="BN16" s="33">
         <v>1501</v>
       </c>
     </row>
     <row r="17" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="I17" s="65"/>
-      <c r="S17" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="T17" s="51">
+      <c r="I17" s="64"/>
+      <c r="S17" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="T17" s="50">
         <v>6021</v>
       </c>
-      <c r="AG17" s="43"/>
-      <c r="AH17" s="43"/>
-      <c r="AI17" s="43"/>
-      <c r="AJ17" s="43"/>
-      <c r="AM17" s="33" t="s">
+      <c r="AG17" s="42"/>
+      <c r="AH17" s="42"/>
+      <c r="AI17" s="42"/>
+      <c r="AJ17" s="42"/>
+      <c r="AM17" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="AN17" s="34">
+      <c r="AN17" s="33">
         <v>900</v>
       </c>
-      <c r="AO17" s="33" t="s">
+      <c r="AO17" s="32" t="s">
         <v>27</v>
       </c>
       <c r="AP17" s="16">
         <v>1600</v>
       </c>
-      <c r="AQ17" s="33" t="s">
+      <c r="AQ17" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="AR17" s="34">
+      <c r="AR17" s="33">
         <v>2200</v>
       </c>
-      <c r="BM17" s="33" t="s">
+      <c r="BM17" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="BN17" s="34">
+      <c r="BN17" s="33">
         <v>1600</v>
       </c>
     </row>
     <row r="18" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="I18" s="65"/>
-      <c r="AM18" s="33" t="s">
+      <c r="I18" s="64"/>
+      <c r="AM18" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AN18" s="34">
+      <c r="AN18" s="33">
         <v>901</v>
       </c>
       <c r="AO18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AP18" s="46">
+      <c r="AP18" s="45">
         <v>1601</v>
       </c>
-      <c r="AQ18" s="33" t="s">
+      <c r="AQ18" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AR18" s="34">
+      <c r="AR18" s="33">
         <v>2201</v>
       </c>
-      <c r="BM18" s="33" t="s">
+      <c r="BM18" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="BN18" s="34">
+      <c r="BN18" s="33">
         <v>1601</v>
       </c>
     </row>
     <row r="19" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="I19" s="65"/>
-      <c r="AM19" s="33" t="s">
+      <c r="I19" s="64"/>
+      <c r="AM19" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AN19" s="34">
+      <c r="AN19" s="33">
         <v>1000</v>
       </c>
       <c r="AO19" s="16"/>
       <c r="AP19" s="16"/>
-      <c r="AQ19" s="33" t="s">
+      <c r="AQ19" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AR19" s="34">
+      <c r="AR19" s="33">
         <v>2300</v>
       </c>
     </row>
     <row r="20" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="I20" s="65"/>
-      <c r="AM20" s="33" t="s">
+      <c r="I20" s="64"/>
+      <c r="AM20" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AN20" s="34">
+      <c r="AN20" s="33">
         <v>1001</v>
       </c>
       <c r="AO20" s="16"/>
       <c r="AP20" s="16"/>
-      <c r="AQ20" s="33" t="s">
+      <c r="AQ20" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AR20" s="34">
+      <c r="AR20" s="33">
         <v>2301</v>
       </c>
     </row>
     <row r="21" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="I21" s="65"/>
+      <c r="I21" s="64"/>
       <c r="AM21" s="12" t="s">
         <v>14</v>
       </c>
@@ -2104,84 +2107,84 @@
       </c>
       <c r="AO21" s="16"/>
       <c r="AP21" s="16"/>
-      <c r="AQ21" s="44" t="s">
+      <c r="AQ21" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="AR21" s="34">
+      <c r="AR21" s="33">
         <v>2400</v>
       </c>
     </row>
     <row r="22" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AO22" s="32"/>
-      <c r="AP22" s="32"/>
-      <c r="AQ22" s="44" t="s">
+      <c r="AO22" s="31"/>
+      <c r="AP22" s="31"/>
+      <c r="AQ22" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="AR22" s="45">
+      <c r="AR22" s="44">
         <v>2401</v>
       </c>
     </row>
     <row r="23" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM23" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN23" s="54"/>
-      <c r="AO23" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="AP23" s="74"/>
-      <c r="AQ23" s="47" t="s">
+      <c r="AM23" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="AN23" s="53"/>
+      <c r="AO23" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="AP23" s="73"/>
+      <c r="AQ23" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="AR23" s="48">
+      <c r="AR23" s="47">
         <v>2500</v>
       </c>
     </row>
     <row r="24" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM24" s="33" t="s">
+      <c r="AM24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="AN24" s="45">
+      <c r="AN24" s="44">
         <v>450</v>
       </c>
-      <c r="AO24" s="33" t="s">
+      <c r="AO24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="AP24" s="45">
+      <c r="AP24" s="44">
         <v>1150</v>
       </c>
-      <c r="AQ24" s="44" t="s">
+      <c r="AQ24" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="AR24" s="45">
+      <c r="AR24" s="44">
         <v>2501</v>
       </c>
     </row>
     <row r="25" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM25" s="33" t="s">
+      <c r="AM25" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AN25" s="45">
+      <c r="AN25" s="44">
         <v>451</v>
       </c>
-      <c r="AO25" s="33" t="s">
+      <c r="AO25" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AP25" s="45">
+      <c r="AP25" s="44">
         <v>1151</v>
       </c>
-      <c r="AQ25" s="44" t="s">
+      <c r="AQ25" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="AR25" s="45">
+      <c r="AR25" s="44">
         <v>2600</v>
       </c>
     </row>
     <row r="26" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AQ26" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AR26" s="50">
+      <c r="AQ26" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR26" s="49">
         <v>2601</v>
       </c>
     </row>
@@ -2190,149 +2193,288 @@
       <c r="AR27" s="16"/>
     </row>
     <row r="28" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM28" s="33" t="s">
+      <c r="AM28" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AN28" s="34">
+      <c r="AN28" s="33">
         <v>500</v>
       </c>
-      <c r="AO28" s="33" t="s">
+      <c r="AO28" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AP28" s="34">
+      <c r="AP28" s="33">
         <v>500</v>
       </c>
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
     <row r="29" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM29" s="33" t="s">
+      <c r="AM29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AN29" s="34">
+      <c r="AN29" s="33">
         <v>501</v>
       </c>
-      <c r="AO29" s="33" t="s">
+      <c r="AO29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AP29" s="34">
+      <c r="AP29" s="33">
         <v>501</v>
       </c>
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
     <row r="30" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM30" s="33" t="s">
+      <c r="AM30" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AN30" s="34">
+      <c r="AN30" s="33">
         <v>600</v>
       </c>
-      <c r="AO30" s="33" t="s">
+      <c r="AO30" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP30" s="34">
+      <c r="AP30" s="33">
         <v>600</v>
       </c>
-      <c r="AQ30" s="16"/>
-      <c r="AR30" s="16"/>
+      <c r="AQ30" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR30" s="72"/>
     </row>
     <row r="31" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM31" s="33" t="s">
+      <c r="AM31" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AN31" s="34">
+      <c r="AN31" s="33">
         <v>601</v>
       </c>
-      <c r="AO31" s="33" t="s">
+      <c r="AO31" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AP31" s="34">
+      <c r="AP31" s="33">
         <v>601</v>
       </c>
-      <c r="AQ31" s="16"/>
-      <c r="AR31" s="16"/>
+      <c r="AQ31" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR31" s="44">
+        <v>1750</v>
+      </c>
     </row>
     <row r="32" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AM32" s="33" t="s">
+      <c r="AM32" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN32" s="33">
+        <v>700</v>
+      </c>
+      <c r="AO32" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP32" s="33">
+        <v>700</v>
+      </c>
+      <c r="AQ32" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR32" s="44">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="33" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AM33" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="AN32" s="34">
-        <v>700</v>
-      </c>
-      <c r="AO32" s="33" t="s">
+      <c r="AN33" s="33">
+        <v>701</v>
+      </c>
+      <c r="AO33" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="AP32" s="34">
-        <v>700</v>
-      </c>
-      <c r="AQ32" s="16"/>
-      <c r="AR32" s="16"/>
-    </row>
-    <row r="33" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM33" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN33" s="34">
+      <c r="AP33" s="33">
         <v>701</v>
       </c>
-      <c r="AO33" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP33" s="34">
-        <v>701</v>
-      </c>
-      <c r="AQ33" s="16"/>
-      <c r="AR33" s="16"/>
+      <c r="AQ33" s="43"/>
+      <c r="AR33" s="33"/>
     </row>
     <row r="34" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM34" s="33" t="s">
+      <c r="AM34" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="AN34" s="34">
+      <c r="AN34" s="33">
         <v>800</v>
       </c>
-      <c r="AO34" s="33" t="s">
+      <c r="AO34" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="AP34" s="34">
+      <c r="AP34" s="33">
         <v>800</v>
       </c>
-      <c r="AQ34" s="16"/>
-      <c r="AR34" s="16"/>
+      <c r="AQ34" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR34" s="33">
+        <v>1800</v>
+      </c>
     </row>
     <row r="35" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM35" s="33" t="s">
+      <c r="AM35" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AN35" s="34">
+      <c r="AN35" s="33">
         <v>801</v>
       </c>
-      <c r="AO35" s="33" t="s">
+      <c r="AO35" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AP35" s="34">
+      <c r="AP35" s="33">
         <v>801</v>
       </c>
-      <c r="AQ35" s="31"/>
-      <c r="AR35" s="31"/>
+      <c r="AQ35" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR35" s="33">
+        <v>1801</v>
+      </c>
     </row>
     <row r="36" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM36" s="33"/>
-      <c r="AN36" s="34"/>
+      <c r="AM36" s="32"/>
+      <c r="AN36" s="33"/>
       <c r="AO36" s="19"/>
       <c r="AP36" s="19"/>
-      <c r="AQ36" s="19"/>
-      <c r="AR36" s="19"/>
+      <c r="AQ36" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR36" s="33">
+        <v>1900</v>
+      </c>
     </row>
     <row r="37" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AO37" s="19"/>
       <c r="AP37" s="19"/>
-      <c r="AQ37" s="19"/>
-      <c r="AR37" s="19"/>
+      <c r="AQ37" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR37" s="33">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="38" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ38" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR38" s="33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ39" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR39" s="33">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="40" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ40" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR40" s="33">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="41" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ41" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR41" s="33">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="42" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ42" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR42" s="33">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="43" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ43" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR43" s="33">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="44" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ44" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR44" s="33">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="45" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ45" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR45" s="33">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="46" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ46" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR46" s="33">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="47" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ47" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR47" s="44">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="48" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AQ48" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR48" s="47">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="49" spans="43:44" x14ac:dyDescent="0.3">
+      <c r="AQ49" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR49" s="44">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="50" spans="43:44" x14ac:dyDescent="0.3">
+      <c r="AQ50" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR50" s="44">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="51" spans="43:44" x14ac:dyDescent="0.3">
+      <c r="AQ51" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR51" s="49">
+        <v>2601</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="AQ30:AR30"/>
     <mergeCell ref="I6:I21"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2389,20 +2531,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="24"/>
@@ -2490,25 +2632,25 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="39">
+      <c r="A8" s="38">
         <v>4</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2528,13 +2670,13 @@
       <c r="E9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="39" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="A10" s="38">
         <v>6</v>
       </c>
       <c r="B10" s="29" t="s">
@@ -2547,45 +2689,45 @@
         <v>105</v>
       </c>
       <c r="E10" s="29"/>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="39" t="s">
         <v>78</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>7</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="D11" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="E11" s="29"/>
+      <c r="F11" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="39">
-        <v>8</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>124</v>
-      </c>
       <c r="C12" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>123</v>
-      </c>
       <c r="E12" s="29"/>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="39" t="s">
         <v>78</v>
       </c>
       <c r="G12" s="4"/>
@@ -2678,14 +2820,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -2749,93 +2891,93 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.21875" style="37"/>
+    <col min="2" max="2" width="9.21875" style="36"/>
     <col min="3" max="3" width="40.88671875" customWidth="1"/>
     <col min="4" max="4" width="55.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="42">
+      <c r="B5" s="41">
         <v>1</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="42">
+      <c r="B6" s="41">
         <v>2</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="42"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="42"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="42"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="42"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="42"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="42"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="42"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="42"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add animation Hold for small, big, raccoon Mario: run
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A656E000-17D2-4C37-B6BF-3B9E1BD54A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A043227-D9F6-4CFC-89C4-DAE694D536CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="136">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -1181,7 +1181,7 @@
   <dimension ref="B4:BP51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR32" sqref="AR32"/>
+      <selection activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2197,13 +2197,13 @@
         <v>21</v>
       </c>
       <c r="AN28" s="33">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="AO28" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AP28" s="33">
-        <v>500</v>
+      <c r="AP28" s="16">
+        <v>1250</v>
       </c>
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
@@ -2213,13 +2213,13 @@
         <v>22</v>
       </c>
       <c r="AN29" s="33">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="AO29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AP29" s="33">
-        <v>501</v>
+      <c r="AP29" s="16">
+        <v>1251</v>
       </c>
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
@@ -2229,13 +2229,13 @@
         <v>23</v>
       </c>
       <c r="AN30" s="33">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="AO30" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP30" s="33">
-        <v>600</v>
+      <c r="AP30" s="16">
+        <v>1350</v>
       </c>
       <c r="AQ30" s="74" t="s">
         <v>134</v>
@@ -2247,13 +2247,13 @@
         <v>24</v>
       </c>
       <c r="AN31" s="33">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="AO31" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AP31" s="33">
-        <v>601</v>
+      <c r="AP31" s="16">
+        <v>1351</v>
       </c>
       <c r="AQ31" s="32" t="s">
         <v>20</v>
@@ -2270,10 +2270,10 @@
         <v>700</v>
       </c>
       <c r="AO32" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP32" s="33">
-        <v>700</v>
+        <v>31</v>
+      </c>
+      <c r="AP32" s="16">
+        <v>1400</v>
       </c>
       <c r="AQ32" s="32" t="s">
         <v>19</v>
@@ -2290,10 +2290,10 @@
         <v>701</v>
       </c>
       <c r="AO33" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP33" s="33">
-        <v>701</v>
+        <v>32</v>
+      </c>
+      <c r="AP33" s="16">
+        <v>1401</v>
       </c>
       <c r="AQ33" s="43"/>
       <c r="AR33" s="33"/>
@@ -2306,16 +2306,16 @@
         <v>800</v>
       </c>
       <c r="AO34" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP34" s="33">
-        <v>800</v>
+        <v>25</v>
+      </c>
+      <c r="AP34" s="16">
+        <v>1500</v>
       </c>
       <c r="AQ34" s="32" t="s">
         <v>21</v>
       </c>
       <c r="AR34" s="33">
-        <v>1800</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="35" spans="39:44" x14ac:dyDescent="0.3">
@@ -2326,38 +2326,46 @@
         <v>801</v>
       </c>
       <c r="AO35" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP35" s="33">
-        <v>801</v>
+        <v>26</v>
+      </c>
+      <c r="AP35" s="16">
+        <v>1501</v>
       </c>
       <c r="AQ35" s="32" t="s">
         <v>22</v>
       </c>
       <c r="AR35" s="33">
-        <v>1801</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="36" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AM36" s="32"/>
       <c r="AN36" s="33"/>
-      <c r="AO36" s="19"/>
-      <c r="AP36" s="19"/>
+      <c r="AO36" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP36" s="16">
+        <v>1600</v>
+      </c>
       <c r="AQ36" s="32" t="s">
         <v>23</v>
       </c>
       <c r="AR36" s="33">
-        <v>1900</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="37" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AO37" s="19"/>
-      <c r="AP37" s="19"/>
+      <c r="AO37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP37" s="45">
+        <v>1601</v>
+      </c>
       <c r="AQ37" s="32" t="s">
         <v>24</v>
       </c>
       <c r="AR37" s="33">
-        <v>1901</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="38" spans="39:44" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Cleaning up all warnings and create some filters
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A043227-D9F6-4CFC-89C4-DAE694D536CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482624F0-FF1F-409F-8BC4-9B4018425777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="136">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP31" sqref="AP31"/>
+    <sheetView tabSelected="1" topLeftCell="AD19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP35" sqref="AP35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2267,14 +2267,10 @@
         <v>116</v>
       </c>
       <c r="AN32" s="33">
-        <v>700</v>
-      </c>
-      <c r="AO32" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP32" s="16">
-        <v>1400</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="AO32" s="32"/>
+      <c r="AP32" s="16"/>
       <c r="AQ32" s="32" t="s">
         <v>19</v>
       </c>
@@ -2287,14 +2283,10 @@
         <v>117</v>
       </c>
       <c r="AN33" s="33">
-        <v>701</v>
-      </c>
-      <c r="AO33" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP33" s="16">
-        <v>1401</v>
-      </c>
+        <v>751</v>
+      </c>
+      <c r="AO33" s="32"/>
+      <c r="AP33" s="16"/>
       <c r="AQ33" s="43"/>
       <c r="AR33" s="33"/>
     </row>
@@ -2309,7 +2301,7 @@
         <v>25</v>
       </c>
       <c r="AP34" s="16">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="AQ34" s="32" t="s">
         <v>21</v>
@@ -2329,7 +2321,7 @@
         <v>26</v>
       </c>
       <c r="AP35" s="16">
-        <v>1501</v>
+        <v>1551</v>
       </c>
       <c r="AQ35" s="32" t="s">
         <v>22</v>
@@ -2401,36 +2393,20 @@
       </c>
     </row>
     <row r="42" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AQ42" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR42" s="33">
-        <v>2200</v>
-      </c>
+      <c r="AQ42" s="32"/>
+      <c r="AR42" s="33"/>
     </row>
     <row r="43" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AQ43" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR43" s="33">
-        <v>2201</v>
-      </c>
+      <c r="AQ43" s="32"/>
+      <c r="AR43" s="33"/>
     </row>
     <row r="44" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AQ44" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR44" s="33">
-        <v>2300</v>
-      </c>
+      <c r="AQ44" s="32"/>
+      <c r="AR44" s="33"/>
     </row>
     <row r="45" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AQ45" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR45" s="33">
-        <v>2301</v>
-      </c>
+      <c r="AQ45" s="32"/>
+      <c r="AR45" s="33"/>
     </row>
     <row r="46" spans="39:44" x14ac:dyDescent="0.3">
       <c r="AQ46" s="43" t="s">

</xml_diff>

<commit_message>
Add animation Kick for small, big, raccoon Mario
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482624F0-FF1F-409F-8BC4-9B4018425777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D664C5C1-9F89-4BAC-A4DA-625C7C80641D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -457,6 +457,15 @@
   </si>
   <si>
     <t>Attack Left</t>
+  </si>
+  <si>
+    <t>Kick right</t>
+  </si>
+  <si>
+    <t>Kick left</t>
+  </si>
+  <si>
+    <t>kick left</t>
   </si>
 </sst>
 </file>
@@ -1180,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP35" sqref="AP35"/>
+    <sheetView tabSelected="1" topLeftCell="AE15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR28" sqref="AR28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,8 +2080,12 @@
       <c r="AN19" s="33">
         <v>1000</v>
       </c>
-      <c r="AO19" s="16"/>
-      <c r="AP19" s="16"/>
+      <c r="AO19" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP19" s="19">
+        <v>310</v>
+      </c>
       <c r="AQ19" s="32" t="s">
         <v>31</v>
       </c>
@@ -2088,8 +2101,12 @@
       <c r="AN20" s="33">
         <v>1001</v>
       </c>
-      <c r="AO20" s="16"/>
-      <c r="AP20" s="16"/>
+      <c r="AO20" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="AP20" s="19">
+        <v>311</v>
+      </c>
       <c r="AQ20" s="32" t="s">
         <v>32</v>
       </c>
@@ -2189,8 +2206,12 @@
       </c>
     </row>
     <row r="27" spans="9:66" x14ac:dyDescent="0.3">
-      <c r="AQ27" s="16"/>
-      <c r="AR27" s="16"/>
+      <c r="AQ27" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR27" s="44">
+        <v>320</v>
+      </c>
     </row>
     <row r="28" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM28" s="32" t="s">
@@ -2205,8 +2226,12 @@
       <c r="AP28" s="16">
         <v>1250</v>
       </c>
-      <c r="AQ28" s="16"/>
-      <c r="AR28" s="16"/>
+      <c r="AQ28" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR28" s="44">
+        <v>321</v>
+      </c>
     </row>
     <row r="29" spans="9:66" x14ac:dyDescent="0.3">
       <c r="AM29" s="32" t="s">
@@ -2365,18 +2390,30 @@
         <v>25</v>
       </c>
       <c r="AR38" s="33">
-        <v>2000</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="39" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AM39" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN39" s="44">
+        <v>300</v>
+      </c>
       <c r="AQ39" s="32" t="s">
         <v>26</v>
       </c>
       <c r="AR39" s="33">
-        <v>2001</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="40" spans="39:44" x14ac:dyDescent="0.3">
+      <c r="AM40" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN40">
+        <v>301</v>
+      </c>
       <c r="AQ40" s="32" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Add animation for P character in HUD's speed bar
</commit_message>
<xml_diff>
--- a/Project_Notes/To_Do_List.xlsx
+++ b/Project_Notes/To_Do_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieu\Desktop\Game\MarioProject_dx10\Project_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D664C5C1-9F89-4BAC-A4DA-625C7C80641D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAFAEC8-CA10-4FE7-98A0-00D16FE3E5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B3E1A348-B592-4DFB-9E4E-C289F0BA6556}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="141">
   <si>
     <t>World 1-1: ground terrain</t>
   </si>
@@ -466,6 +466,12 @@
   </si>
   <si>
     <t>kick left</t>
+  </si>
+  <si>
+    <t>p char normal</t>
+  </si>
+  <si>
+    <t>p char max speed</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9DF5F8-B94E-49CD-BCE5-4B9CB83C5116}">
   <dimension ref="B4:BP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR28" sqref="AR28"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BG15" sqref="BG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,8 +1223,8 @@
     <col min="52" max="52" width="8.44140625" customWidth="1"/>
     <col min="53" max="53" width="12.109375" customWidth="1"/>
     <col min="54" max="58" width="8.44140625" customWidth="1"/>
-    <col min="59" max="59" width="5.6640625" customWidth="1"/>
-    <col min="60" max="63" width="7.77734375" customWidth="1"/>
+    <col min="59" max="60" width="15.77734375" customWidth="1"/>
+    <col min="61" max="63" width="7.77734375" customWidth="1"/>
     <col min="64" max="64" width="11.6640625" customWidth="1"/>
     <col min="65" max="66" width="13.44140625" customWidth="1"/>
     <col min="67" max="67" width="13.109375" customWidth="1"/>
@@ -1734,6 +1740,12 @@
       <c r="AR8" s="33">
         <v>1710</v>
       </c>
+      <c r="BG8" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH8">
+        <v>16002</v>
+      </c>
       <c r="BM8" s="32" t="s">
         <v>19</v>
       </c>
@@ -1771,6 +1783,12 @@
       </c>
       <c r="AR9" s="33">
         <v>1800</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH9">
+        <v>16003</v>
       </c>
       <c r="BM9" s="32" t="s">
         <v>21</v>

</xml_diff>